<commit_message>
Address Chris' EC comments
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -12,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$64:$O$84</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$T$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$T$27</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="138">
   <si>
     <t>Cost</t>
   </si>
@@ -375,9 +375,6 @@
     <t>Existing</t>
   </si>
   <si>
-    <t>20+</t>
-  </si>
-  <si>
     <t>Halawa</t>
   </si>
   <si>
@@ -412,6 +409,30 @@
   </si>
   <si>
     <t>Project Status (@2012)</t>
+  </si>
+  <si>
+    <t>Makakilo Mauka Frontage Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalaeloa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Makakilo </t>
+  </si>
+  <si>
+    <t>Frontage Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamokila </t>
+  </si>
+  <si>
+    <t>Kapolei</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
+    <t>additional</t>
   </si>
 </sst>
 </file>
@@ -499,7 +520,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -536,6 +557,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1210,13 +1237,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB96"/>
+  <dimension ref="A1:AB98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,11 +1252,11 @@
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="6" width="32.5703125" customWidth="1"/>
     <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="5" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="5" hidden="1" customWidth="1"/>
-    <col min="12" max="14" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="5" customWidth="1"/>
+    <col min="12" max="14" width="13.7109375" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" style="18" customWidth="1"/>
     <col min="16" max="16" width="18" style="5" customWidth="1"/>
     <col min="17" max="19" width="18" customWidth="1"/>
@@ -1321,7 +1348,7 @@
         <v>62</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>0</v>
@@ -1379,7 +1406,7 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="22" t="s">
         <v>40</v>
       </c>
       <c r="J10">
@@ -1412,15 +1439,15 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" t="s">
         <v>119</v>
       </c>
-      <c r="E11" t="s">
-        <v>120</v>
-      </c>
       <c r="F11" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="G11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="22" t="s">
         <v>40</v>
       </c>
       <c r="J11" s="6"/>
@@ -1449,15 +1476,15 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="E12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="22" t="s">
         <v>117</v>
       </c>
       <c r="J12" s="6"/>
@@ -1486,21 +1513,21 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" t="s">
         <v>124</v>
       </c>
-      <c r="E13" t="s">
-        <v>125</v>
-      </c>
       <c r="F13" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="22" t="s">
         <v>73</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="7"/>
       <c r="O13" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P13" s="8">
         <v>0</v>
@@ -1534,7 +1561,7 @@
       <c r="F14" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="22" t="s">
         <v>40</v>
       </c>
       <c r="J14">
@@ -1575,7 +1602,7 @@
       <c r="F15" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="22" t="s">
         <v>40</v>
       </c>
       <c r="J15"/>
@@ -1611,7 +1638,7 @@
       <c r="F16" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="22" t="s">
         <v>40</v>
       </c>
       <c r="J16">
@@ -1649,7 +1676,7 @@
       <c r="F17" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="22" t="s">
         <v>73</v>
       </c>
       <c r="J17"/>
@@ -1684,7 +1711,7 @@
       <c r="F18" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="23" t="s">
         <v>40</v>
       </c>
       <c r="J18"/>
@@ -1707,40 +1734,37 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>73</v>
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <v>4</v>
-      </c>
-      <c r="P19" s="5">
+        <v>2</v>
+      </c>
+      <c r="P19" s="8">
         <v>0</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19">
         <v>1</v>
@@ -1751,35 +1775,37 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>12</v>
-      </c>
-      <c r="B20" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
       <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
         <v>79</v>
       </c>
-      <c r="D20" t="s">
-        <v>84</v>
-      </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>40</v>
+      <c r="G20" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P20" s="5">
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R20">
         <v>1</v>
@@ -1793,33 +1819,32 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B21" s="4"/>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="N21" t="s">
-        <v>115</v>
-      </c>
-      <c r="O21" s="18" t="s">
-        <v>129</v>
+        <v>8</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
       </c>
       <c r="P21" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21">
         <v>1</v>
@@ -1836,21 +1861,21 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
         <v>87</v>
-      </c>
-      <c r="E22" t="s">
-        <v>91</v>
       </c>
       <c r="F22" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="22" t="s">
         <v>117</v>
       </c>
       <c r="J22"/>
@@ -1859,7 +1884,7 @@
         <v>115</v>
       </c>
       <c r="O22" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P22" s="5">
         <v>1</v>
@@ -1879,30 +1904,30 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="22" t="s">
         <v>117</v>
       </c>
       <c r="J23"/>
-      <c r="K23" s="10"/>
+      <c r="K23"/>
       <c r="N23" t="s">
         <v>115</v>
       </c>
       <c r="O23" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P23" s="5">
         <v>1</v>
@@ -1922,75 +1947,71 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>73</v>
+        <v>89</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>117</v>
       </c>
       <c r="J24"/>
-      <c r="K24"/>
+      <c r="K24" s="10"/>
       <c r="N24" t="s">
         <v>115</v>
       </c>
-      <c r="P24" s="8">
-        <v>0</v>
+      <c r="O24" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="P24" s="5">
+        <v>1</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24">
         <v>1</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25">
-        <v>2</v>
-      </c>
-      <c r="K25">
-        <v>4</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25"/>
+      <c r="K25"/>
       <c r="N25" t="s">
         <v>115</v>
       </c>
@@ -1998,45 +2019,98 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25">
         <v>1</v>
       </c>
       <c r="S25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>118</v>
+      <c r="A26" s="4">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
       </c>
       <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="N26" t="s">
+        <v>115</v>
+      </c>
+      <c r="P26" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>22</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" t="s">
         <v>116</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="J26"/>
-      <c r="K26"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="J27"/>
-      <c r="K27"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
       <c r="G28" s="4"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2202,11 +2276,21 @@
       <c r="K44"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
       <c r="G45" s="4"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
       <c r="G46" s="4"/>
       <c r="J46"/>
       <c r="K46"/>
@@ -2287,10 +2371,12 @@
       <c r="K61"/>
     </row>
     <row r="62" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G62" s="4"/>
       <c r="J62"/>
       <c r="K62"/>
     </row>
     <row r="63" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G63" s="4"/>
       <c r="J63"/>
       <c r="K63"/>
     </row>
@@ -2307,41 +2393,34 @@
       <c r="K66"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="O67" s="19"/>
-      <c r="P67" s="8"/>
-      <c r="Q67" s="8"/>
-      <c r="R67" s="8"/>
-      <c r="S67" s="8"/>
+      <c r="J67"/>
+      <c r="K67"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
       <c r="O68" s="19"/>
       <c r="P68" s="8"/>
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
       <c r="S68" s="8"/>
     </row>
-    <row r="69" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J69" s="8"/>
-      <c r="K69" s="5"/>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="G69" s="4"/>
       <c r="O69" s="19"/>
       <c r="P69" s="8"/>
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
       <c r="S69" s="8"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="I70" s="4"/>
+    <row r="70" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="5"/>
       <c r="O70" s="19"/>
       <c r="P70" s="8"/>
       <c r="Q70" s="8"/>
@@ -2351,7 +2430,12 @@
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
       <c r="I71" s="4"/>
       <c r="O71" s="19"/>
       <c r="P71" s="8"/>
@@ -2362,8 +2446,9 @@
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
       <c r="O72" s="19"/>
       <c r="P72" s="8"/>
       <c r="Q72" s="8"/>
@@ -2374,7 +2459,7 @@
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
       <c r="O73" s="19"/>
       <c r="P73" s="8"/>
       <c r="Q73" s="8"/>
@@ -2429,6 +2514,7 @@
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
       <c r="O78" s="19"/>
       <c r="P78" s="8"/>
       <c r="Q78" s="8"/>
@@ -2439,6 +2525,7 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
       <c r="O79" s="19"/>
       <c r="P79" s="8"/>
       <c r="Q79" s="8"/>
@@ -2499,7 +2586,6 @@
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
       <c r="O85" s="19"/>
       <c r="P85" s="8"/>
       <c r="Q85" s="8"/>
@@ -2509,7 +2595,6 @@
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
       <c r="G86" s="4"/>
       <c r="O86" s="19"/>
       <c r="P86" s="8"/>
@@ -2520,8 +2605,8 @@
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
       <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
       <c r="O87" s="19"/>
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
@@ -2531,10 +2616,8 @@
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
       <c r="G88" s="4"/>
-      <c r="I88" s="5"/>
-      <c r="J88" s="9"/>
-      <c r="K88" s="8"/>
       <c r="O88" s="19"/>
       <c r="P88" s="8"/>
       <c r="Q88" s="8"/>
@@ -2544,9 +2627,9 @@
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
       <c r="G89" s="4"/>
-      <c r="I89" s="5"/>
-      <c r="J89" s="8"/>
+      <c r="J89" s="9"/>
       <c r="K89" s="8"/>
       <c r="O89" s="19"/>
       <c r="P89" s="8"/>
@@ -2567,15 +2650,34 @@
       <c r="R90" s="8"/>
       <c r="S90" s="8"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="8"/>
+      <c r="K91" s="8"/>
+      <c r="O91" s="19"/>
+      <c r="P91" s="8"/>
+      <c r="Q91" s="8"/>
+      <c r="R91" s="8"/>
+      <c r="S91" s="8"/>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T26"/>
+  <autoFilter ref="A9:T27"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="H88:H90"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="H90:H92"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="20" orientation="landscape" r:id="rId1"/>
@@ -2968,7 +3070,7 @@
       </c>
       <c r="J23"/>
       <c r="O23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2987,7 +3089,7 @@
       </c>
       <c r="J24"/>
       <c r="O24" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -3006,7 +3108,7 @@
       <c r="J25"/>
       <c r="K25"/>
       <c r="O25" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>

</xml_diff>

<commit_message>
Add King St. Bike Project
Reduces the lanes on King St. in order to accommodate a pilot bike track.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -12,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$64:$O$84</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$T$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$T$29</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="142">
   <si>
     <t>Cost</t>
   </si>
@@ -433,6 +433,18 @@
   </si>
   <si>
     <t>additional</t>
+  </si>
+  <si>
+    <t>King St. Bike Track</t>
+  </si>
+  <si>
+    <t>Alapai St</t>
+  </si>
+  <si>
+    <t>Isenberg St</t>
+  </si>
+  <si>
+    <t>Capacity Reduction for bike lane</t>
   </si>
 </sst>
 </file>
@@ -1237,13 +1249,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB98"/>
+  <dimension ref="A1:AB99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,22 +2132,49 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="4"/>
+      <c r="A28" s="4">
+        <v>23</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="J28"/>
       <c r="K28"/>
+      <c r="P28" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>116</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2311,6 +2350,11 @@
       <c r="K46"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
       <c r="G47" s="4"/>
       <c r="J47"/>
       <c r="K47"/>
@@ -2396,6 +2440,7 @@
       <c r="K63"/>
     </row>
     <row r="64" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G64" s="4"/>
       <c r="J64"/>
       <c r="K64"/>
     </row>
@@ -2412,46 +2457,34 @@
       <c r="K67"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="O68" s="19"/>
-      <c r="P68" s="8"/>
-      <c r="Q68" s="8"/>
-      <c r="R68" s="8"/>
-      <c r="S68" s="8"/>
+      <c r="J68"/>
+      <c r="K68"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="G69" s="4"/>
       <c r="O69" s="19"/>
       <c r="P69" s="8"/>
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
       <c r="S69" s="8"/>
     </row>
-    <row r="70" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="H70"/>
-      <c r="I70"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="5"/>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="G70" s="4"/>
       <c r="O70" s="19"/>
       <c r="P70" s="8"/>
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
       <c r="S70" s="8"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
+    <row r="71" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="5"/>
       <c r="O71" s="19"/>
       <c r="P71" s="8"/>
       <c r="Q71" s="8"/>
@@ -2461,8 +2494,12 @@
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="O72" s="19"/>
       <c r="P72" s="8"/>
@@ -2473,6 +2510,7 @@
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
+      <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="I73" s="4"/>
       <c r="O73" s="19"/>
@@ -2485,7 +2523,7 @@
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
       <c r="O74" s="19"/>
       <c r="P74" s="8"/>
       <c r="Q74" s="8"/>
@@ -2551,6 +2589,7 @@
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
       <c r="O80" s="19"/>
       <c r="P80" s="8"/>
       <c r="Q80" s="8"/>
@@ -2621,7 +2660,6 @@
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
       <c r="O87" s="19"/>
       <c r="P87" s="8"/>
       <c r="Q87" s="8"/>
@@ -2631,8 +2669,8 @@
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
       <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
       <c r="O88" s="19"/>
       <c r="P88" s="8"/>
       <c r="Q88" s="8"/>
@@ -2644,8 +2682,6 @@
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="G89" s="4"/>
-      <c r="J89" s="9"/>
-      <c r="K89" s="8"/>
       <c r="O89" s="19"/>
       <c r="P89" s="8"/>
       <c r="Q89" s="8"/>
@@ -2655,9 +2691,9 @@
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
       <c r="G90" s="4"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="8"/>
+      <c r="J90" s="9"/>
       <c r="K90" s="8"/>
       <c r="O90" s="19"/>
       <c r="P90" s="8"/>
@@ -2683,16 +2719,29 @@
       <c r="B92" s="4"/>
       <c r="G92" s="4"/>
       <c r="I92" s="5"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
+      <c r="J92" s="8"/>
+      <c r="K92" s="8"/>
+      <c r="O92" s="19"/>
+      <c r="P92" s="8"/>
+      <c r="Q92" s="8"/>
+      <c r="R92" s="8"/>
+      <c r="S92" s="8"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T28"/>
+  <autoFilter ref="A9:T29"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="H90:H92"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="H91:H93"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="20" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Add transit-supporting links to EC network
Links 10670,10672,10674,10675
All around the H2/Pearl Highlands interchange
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="141">
   <si>
     <t>Cost</t>
   </si>
@@ -430,9 +430,6 @@
   </si>
   <si>
     <t>FDR</t>
-  </si>
-  <si>
-    <t>additional</t>
   </si>
   <si>
     <t>King St. Bike Track</t>
@@ -1255,7 +1252,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,16 +2133,16 @@
         <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>40</v>
@@ -2169,8 +2166,8 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>137</v>
+      <c r="A29">
+        <v>24</v>
       </c>
       <c r="C29" t="s">
         <v>116</v>
@@ -2178,6 +2175,21 @@
       <c r="G29" s="4"/>
       <c r="J29"/>
       <c r="K29"/>
+      <c r="P29" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>

</xml_diff>

<commit_message>
Update networks and project management sheet
Incorporated Heather's latest route system.  Made highway
modifications where necessary.  Corrected a few projects
in the highway layer and project management list.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="286">
   <si>
     <t>Cost</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>Partially Funded</t>
-  </si>
-  <si>
-    <t>All</t>
   </si>
   <si>
     <t>Fort Barrette Rd</t>
@@ -881,6 +878,12 @@
   </si>
   <si>
     <t>bus/rail integration + HUB</t>
+  </si>
+  <si>
+    <t>2040 LRTP</t>
+  </si>
+  <si>
+    <t>South St Reverse Direction</t>
   </si>
 </sst>
 </file>
@@ -1768,6 +1771,7 @@
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1840,13 +1844,13 @@
     </row>
     <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>18</v>
@@ -1861,7 +1865,7 @@
         <v>62</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>0</v>
@@ -1894,16 +1898,16 @@
         <v>72</v>
       </c>
       <c r="S9" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="T9" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="U9" s="3" t="s">
-        <v>279</v>
-      </c>
       <c r="V9" s="3" t="s">
-        <v>74</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -1915,13 +1919,13 @@
         <v>205</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>236</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -1961,13 +1965,13 @@
         <v>351</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>9</v>
@@ -2007,13 +2011,13 @@
         <v>356</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>9</v>
@@ -2044,7 +2048,7 @@
         <v>1</v>
       </c>
       <c r="Y12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -2056,10 +2060,10 @@
         <v>251</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>55</v>
@@ -2102,16 +2106,16 @@
         <v>353</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H14" s="4"/>
       <c r="K14">
@@ -2150,7 +2154,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
         <v>29</v>
@@ -2190,23 +2194,23 @@
         <v>306</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" t="s">
         <v>241</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>242</v>
-      </c>
-      <c r="G16" t="s">
-        <v>243</v>
       </c>
       <c r="H16" s="4"/>
       <c r="K16" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q16" s="5">
         <v>0</v>
@@ -2239,20 +2243,20 @@
         <v>57</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H17" s="4"/>
       <c r="K17" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q17" s="5">
         <v>0</v>
@@ -2287,7 +2291,7 @@
         <v>42</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>73</v>
@@ -2314,7 +2318,7 @@
         <v>1</v>
       </c>
       <c r="AC18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
@@ -2334,7 +2338,7 @@
         <v>23</v>
       </c>
       <c r="G19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H19" s="21" t="s">
         <v>40</v>
@@ -2367,7 +2371,7 @@
         <v>2012</v>
       </c>
       <c r="AD19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
@@ -2381,13 +2385,13 @@
         <v>24</v>
       </c>
       <c r="E20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" t="s">
         <v>117</v>
       </c>
-      <c r="F20" t="s">
-        <v>118</v>
-      </c>
       <c r="G20" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H20" s="21" t="s">
         <v>40</v>
@@ -2416,7 +2420,7 @@
         <v>2020</v>
       </c>
       <c r="AD20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
@@ -2430,16 +2434,16 @@
         <v>24</v>
       </c>
       <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="F21" t="s">
-        <v>118</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>120</v>
-      </c>
       <c r="H21" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="7"/>
@@ -2465,7 +2469,7 @@
         <v>2030</v>
       </c>
       <c r="AD21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
@@ -2479,21 +2483,21 @@
         <v>24</v>
       </c>
       <c r="E22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" t="s">
         <v>121</v>
       </c>
-      <c r="F22" t="s">
-        <v>122</v>
-      </c>
       <c r="G22" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K22" s="6"/>
       <c r="L22" s="7"/>
       <c r="P22" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q22" s="8">
         <v>0</v>
@@ -2523,12 +2527,12 @@
         <v>357</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H23" s="4"/>
       <c r="K23">
@@ -2564,16 +2568,16 @@
         <v>301</v>
       </c>
       <c r="D24" t="s">
+        <v>264</v>
+      </c>
+      <c r="E24" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" t="s">
         <v>265</v>
       </c>
-      <c r="E24" t="s">
-        <v>233</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>267</v>
       </c>
       <c r="H24" s="4"/>
       <c r="K24">
@@ -2610,10 +2614,10 @@
         <v>211</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>31</v>
@@ -2652,19 +2656,19 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26">
         <v>302</v>
       </c>
       <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
         <v>109</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>110</v>
-      </c>
-      <c r="F26" t="s">
-        <v>111</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
@@ -2679,7 +2683,7 @@
         <v>4</v>
       </c>
       <c r="O26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q26" s="8">
         <v>0</v>
@@ -2709,16 +2713,16 @@
         <v>354</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="G27" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H27" s="4"/>
       <c r="K27">
@@ -2755,13 +2759,13 @@
         <v>207</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>9</v>
@@ -2847,19 +2851,19 @@
         <v>803</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>134</v>
-      </c>
       <c r="G30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -2895,16 +2899,16 @@
         <v>352</v>
       </c>
       <c r="D31" t="s">
+        <v>252</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G31" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H31" s="4"/>
       <c r="K31">
@@ -2940,27 +2944,27 @@
         <v>804</v>
       </c>
       <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" t="s">
         <v>90</v>
       </c>
-      <c r="E32" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" t="s">
-        <v>91</v>
-      </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K32"/>
       <c r="L32"/>
       <c r="O32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P32" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q32" s="5">
         <v>1</v>
@@ -2995,7 +2999,7 @@
         <v>44</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H33" s="22" t="s">
         <v>40</v>
@@ -3006,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="R33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S33">
         <v>1</v>
@@ -3030,16 +3034,16 @@
         <v>303</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>232</v>
-      </c>
       <c r="G34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H34" s="4"/>
       <c r="K34">
@@ -3076,16 +3080,16 @@
         <v>801</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" t="s">
         <v>84</v>
       </c>
-      <c r="F35" t="s">
-        <v>85</v>
-      </c>
       <c r="G35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H35" s="22" t="s">
         <v>40</v>
@@ -3124,16 +3128,16 @@
         <v>305</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F36" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" t="s">
         <v>239</v>
-      </c>
-      <c r="G36" t="s">
-        <v>240</v>
       </c>
       <c r="H36" s="4"/>
       <c r="K36">
@@ -3169,16 +3173,16 @@
         <v>858</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="H37" s="21" t="s">
         <v>40</v>
@@ -3213,13 +3217,13 @@
         <v>304</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>9</v>
@@ -3264,13 +3268,13 @@
         <v>53</v>
       </c>
       <c r="E39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" t="s">
         <v>79</v>
       </c>
-      <c r="F39" t="s">
-        <v>80</v>
-      </c>
       <c r="G39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H39" s="21" t="s">
         <v>73</v>
@@ -3311,10 +3315,10 @@
         <v>53</v>
       </c>
       <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" t="s">
         <v>79</v>
-      </c>
-      <c r="F40" t="s">
-        <v>80</v>
       </c>
       <c r="G40" t="s">
         <v>9</v>
@@ -3350,22 +3354,22 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41">
         <v>210</v>
       </c>
       <c r="D41" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H41" s="22" t="s">
         <v>73</v>
@@ -3373,7 +3377,7 @@
       <c r="K41"/>
       <c r="L41"/>
       <c r="O41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q41" s="8">
         <v>0</v>
@@ -3402,16 +3406,16 @@
         <v>355</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="H42" s="22" t="s">
         <v>17</v>
@@ -3452,10 +3456,10 @@
         <v>26</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G43" t="s">
         <v>8</v>
@@ -3493,10 +3497,13 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D44" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+      <c r="G44" t="s">
+        <v>285</v>
       </c>
       <c r="H44" s="4"/>
       <c r="K44"/>
@@ -3529,13 +3536,13 @@
         <v>209</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>229</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>9</v>
@@ -3574,27 +3581,27 @@
         <v>805</v>
       </c>
       <c r="D46" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" t="s">
         <v>95</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>96</v>
       </c>
-      <c r="F46" t="s">
-        <v>97</v>
-      </c>
       <c r="G46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K46"/>
       <c r="L46" s="10"/>
       <c r="O46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P46" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q46" s="5">
         <v>1</v>
@@ -3624,7 +3631,7 @@
         <v>307</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -3661,27 +3668,27 @@
         <v>806</v>
       </c>
       <c r="D48" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" t="s">
+        <v>86</v>
+      </c>
+      <c r="G48" t="s">
         <v>88</v>
       </c>
-      <c r="E48" t="s">
-        <v>86</v>
-      </c>
-      <c r="F48" t="s">
-        <v>87</v>
-      </c>
-      <c r="G48" t="s">
-        <v>89</v>
-      </c>
       <c r="H48" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K48"/>
       <c r="L48"/>
       <c r="O48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P48" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q48" s="5">
         <v>1</v>
@@ -4249,7 +4256,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>40</v>
@@ -4257,7 +4264,7 @@
       <c r="J10"/>
       <c r="K10"/>
       <c r="O10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -4280,7 +4287,7 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="O11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -4303,14 +4310,14 @@
       <c r="J12"/>
       <c r="K12"/>
       <c r="O12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
@@ -4327,7 +4334,7 @@
       <c r="J13"/>
       <c r="K13" s="10"/>
       <c r="O13" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -4350,7 +4357,7 @@
       </c>
       <c r="J14"/>
       <c r="O14" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -4374,7 +4381,7 @@
       <c r="J15"/>
       <c r="K15"/>
       <c r="O15" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -4419,86 +4426,86 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
         <v>92</v>
       </c>
-      <c r="D18" t="s">
-        <v>93</v>
-      </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G18" s="4"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="N18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
         <v>98</v>
       </c>
-      <c r="D19" t="s">
-        <v>99</v>
-      </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G19" s="4"/>
       <c r="J19"/>
       <c r="K19"/>
       <c r="N19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="N20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G21" s="4"/>
       <c r="J21"/>
       <c r="K21" s="10"/>
       <c r="N21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G22" s="4"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="N22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4515,11 +4522,11 @@
         <v>34</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J23"/>
       <c r="O23" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4534,11 +4541,11 @@
         <v>36</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J24"/>
       <c r="O24" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -4549,15 +4556,15 @@
         <v>20</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
       <c r="O25" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
@@ -5022,18 +5029,18 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5044,10 +5051,10 @@
         <v>18</v>
       </c>
       <c r="I3" t="s">
+        <v>267</v>
+      </c>
+      <c r="J3" t="s">
         <v>268</v>
-      </c>
-      <c r="J3" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5055,7 +5062,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5073,7 +5080,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -5091,7 +5098,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -5109,7 +5116,7 @@
         <v>36</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -5127,7 +5134,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -5163,7 +5170,7 @@
         <v>30</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -5289,7 +5296,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C17">
         <v>14</v>
@@ -5307,7 +5314,7 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C18">
         <v>15</v>
@@ -5325,7 +5332,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C19">
         <v>16</v>
@@ -5343,7 +5350,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20">
         <v>17</v>
@@ -5361,7 +5368,7 @@
         <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C21">
         <v>18</v>
@@ -5379,7 +5386,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C22">
         <v>19</v>
@@ -5415,7 +5422,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C24">
         <v>21</v>
@@ -5433,7 +5440,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C25">
         <v>22</v>
@@ -5451,7 +5458,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26">
         <v>23</v>
@@ -5487,7 +5494,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C28">
         <v>25</v>
@@ -5505,7 +5512,7 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29">
         <v>26</v>
@@ -5523,7 +5530,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C30">
         <v>27</v>
@@ -5541,7 +5548,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C31">
         <v>28</v>
@@ -5559,7 +5566,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C32">
         <v>29</v>
@@ -5613,7 +5620,7 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C35">
         <v>32</v>
@@ -5631,7 +5638,7 @@
         <v>20</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C36">
         <v>33</v>
@@ -5667,7 +5674,7 @@
         <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C38">
         <v>35</v>
@@ -5685,7 +5692,7 @@
         <v>25</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C39">
         <v>36</v>
@@ -5703,7 +5710,7 @@
         <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40">
         <v>37</v>
@@ -5721,7 +5728,7 @@
         <v>32</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C41">
         <v>38</v>
@@ -5739,7 +5746,7 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42">
         <v>39</v>
@@ -8134,70 +8141,70 @@
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" t="s">
         <v>142</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>143</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>144</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>145</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" t="s">
         <v>148</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>149</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>150</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" t="s">
         <v>152</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>153</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>154</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>155</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>156</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>157</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>158</v>
-      </c>
-      <c r="V1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
@@ -8211,34 +8218,34 @@
         <v>205</v>
       </c>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" t="s">
         <v>163</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L2">
         <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N2">
         <v>33</v>
@@ -8279,34 +8286,34 @@
         <v>351</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L3">
         <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N3">
         <v>233.1</v>
@@ -8347,34 +8354,34 @@
         <v>356</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L4">
         <v>13</v>
       </c>
       <c r="M4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N4">
         <v>130.80000000000004</v>
@@ -8415,34 +8422,34 @@
         <v>353</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L5">
         <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N5">
         <v>10.713452725559549</v>
@@ -8483,34 +8490,34 @@
         <v>251</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" t="s">
         <v>163</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="K6" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L6">
         <v>12</v>
       </c>
       <c r="M6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N6">
         <v>23.5</v>
@@ -8551,34 +8558,34 @@
         <v>301</v>
       </c>
       <c r="D7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" t="s">
         <v>167</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" t="s">
+        <v>163</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K7" s="24" t="s">
         <v>168</v>
-      </c>
-      <c r="H7" t="s">
-        <v>163</v>
-      </c>
-      <c r="I7" t="s">
-        <v>164</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>169</v>
       </c>
       <c r="L7">
         <v>100</v>
       </c>
       <c r="M7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N7">
         <v>120</v>
@@ -8619,34 +8626,34 @@
         <v>852</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" t="s">
         <v>206</v>
       </c>
-      <c r="H8" t="s">
-        <v>163</v>
-      </c>
-      <c r="I8" t="s">
-        <v>207</v>
-      </c>
       <c r="J8" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L8">
         <v>100</v>
       </c>
       <c r="M8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N8">
         <v>5532.5</v>
@@ -8687,34 +8694,34 @@
         <v>204</v>
       </c>
       <c r="D9" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>160</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="H9" t="s">
         <v>162</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>163</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K9" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L9">
         <v>13</v>
       </c>
       <c r="M9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N9">
         <v>47.7</v>
@@ -8746,7 +8753,7 @@
     </row>
     <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B10">
         <v>29</v>
@@ -8755,34 +8762,34 @@
         <v>503</v>
       </c>
       <c r="D10" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>160</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>161</v>
-      </c>
       <c r="G10" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10" t="s">
+        <v>162</v>
+      </c>
+      <c r="I10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K10" s="24" t="s">
         <v>193</v>
-      </c>
-      <c r="H10" t="s">
-        <v>163</v>
-      </c>
-      <c r="I10" t="s">
-        <v>164</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>194</v>
       </c>
       <c r="L10">
         <v>100</v>
       </c>
       <c r="M10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N10">
         <v>100</v>
@@ -8823,34 +8830,34 @@
         <v>208</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H11" t="s">
+        <v>162</v>
+      </c>
+      <c r="I11" t="s">
         <v>163</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="K11" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="K11" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L11">
         <v>100</v>
       </c>
       <c r="M11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N11">
         <v>100</v>
@@ -8891,34 +8898,34 @@
         <v>306</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" t="s">
         <v>163</v>
       </c>
-      <c r="I12" t="s">
-        <v>164</v>
-      </c>
       <c r="J12" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L12">
         <v>100</v>
       </c>
       <c r="M12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N12">
         <v>16.2</v>
@@ -8959,34 +8966,34 @@
         <v>952</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G13" t="s">
+        <v>223</v>
+      </c>
+      <c r="H13" t="s">
+        <v>203</v>
+      </c>
+      <c r="I13" t="s">
+        <v>163</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="K13" s="24" t="s">
         <v>224</v>
-      </c>
-      <c r="H13" t="s">
-        <v>204</v>
-      </c>
-      <c r="I13" t="s">
-        <v>164</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>225</v>
       </c>
       <c r="L13">
         <v>15</v>
       </c>
       <c r="M13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N13">
         <v>540.29999999999995</v>
@@ -9027,34 +9034,34 @@
         <v>357</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L14">
         <v>14</v>
       </c>
       <c r="M14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N14">
         <v>102.5</v>
@@ -9095,34 +9102,34 @@
         <v>307</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H15" t="s">
+        <v>162</v>
+      </c>
+      <c r="I15" t="s">
         <v>163</v>
       </c>
-      <c r="I15" t="s">
-        <v>164</v>
-      </c>
       <c r="J15" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L15">
         <v>13</v>
       </c>
       <c r="M15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N15">
         <v>30.6</v>
@@ -9163,34 +9170,34 @@
         <v>211</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G16" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="H16" t="s">
         <v>203</v>
       </c>
-      <c r="H16" t="s">
-        <v>204</v>
-      </c>
       <c r="I16" t="s">
+        <v>163</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="K16" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L16">
         <v>15</v>
       </c>
       <c r="M16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N16">
         <v>75</v>
@@ -9231,34 +9238,34 @@
         <v>302</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" t="s">
         <v>171</v>
       </c>
-      <c r="G17" t="s">
-        <v>172</v>
-      </c>
       <c r="H17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I17" t="s">
         <v>163</v>
       </c>
-      <c r="I17" t="s">
-        <v>164</v>
-      </c>
       <c r="J17" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L17">
         <v>13</v>
       </c>
       <c r="M17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N17">
         <v>30</v>
@@ -9299,34 +9306,34 @@
         <v>354</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L18">
         <v>14</v>
       </c>
       <c r="M18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N18">
         <v>271.10000000000002</v>
@@ -9367,34 +9374,34 @@
         <v>207</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H19" t="s">
+        <v>162</v>
+      </c>
+      <c r="I19" t="s">
         <v>163</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K19" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L19">
         <v>18</v>
       </c>
       <c r="M19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N19">
         <v>130</v>
@@ -9435,34 +9442,34 @@
         <v>352</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L20">
         <v>12</v>
       </c>
       <c r="M20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N20">
         <v>24.2</v>
@@ -9503,34 +9510,34 @@
         <v>303</v>
       </c>
       <c r="D21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H21" t="s">
+        <v>162</v>
+      </c>
+      <c r="I21" t="s">
         <v>163</v>
       </c>
-      <c r="I21" t="s">
-        <v>164</v>
-      </c>
       <c r="J21" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L21">
         <v>18</v>
       </c>
       <c r="M21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N21">
         <v>44.1</v>
@@ -9571,34 +9578,34 @@
         <v>801</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G22" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" t="s">
+        <v>162</v>
+      </c>
+      <c r="I22" t="s">
+        <v>163</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K22" s="24" t="s">
         <v>176</v>
-      </c>
-      <c r="H22" t="s">
-        <v>163</v>
-      </c>
-      <c r="I22" t="s">
-        <v>164</v>
-      </c>
-      <c r="J22" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K22" s="24" t="s">
-        <v>177</v>
       </c>
       <c r="L22">
         <v>18</v>
       </c>
       <c r="M22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N22">
         <v>13.3</v>
@@ -9639,34 +9646,34 @@
         <v>305</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H23" t="s">
+        <v>162</v>
+      </c>
+      <c r="I23" t="s">
         <v>163</v>
       </c>
-      <c r="I23" t="s">
-        <v>164</v>
-      </c>
       <c r="J23" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L23">
         <v>9</v>
       </c>
       <c r="M23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N23">
         <v>209.5</v>
@@ -9707,34 +9714,34 @@
         <v>206</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E24" s="24">
         <v>1</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H24" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="I24" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="I24" s="24" t="s">
+      <c r="J24" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="K24" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L24" s="24">
         <v>12</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N24" s="24">
         <v>200</v>
@@ -9775,34 +9782,34 @@
         <v>304</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H25" t="s">
+        <v>162</v>
+      </c>
+      <c r="I25" t="s">
         <v>163</v>
       </c>
-      <c r="I25" t="s">
-        <v>164</v>
-      </c>
       <c r="J25" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L25">
         <v>12</v>
       </c>
       <c r="M25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N25">
         <v>200</v>
@@ -9843,34 +9850,34 @@
         <v>210</v>
       </c>
       <c r="D26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G26" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="H26" t="s">
+        <v>162</v>
+      </c>
+      <c r="I26" t="s">
         <v>200</v>
       </c>
-      <c r="H26" t="s">
-        <v>163</v>
-      </c>
-      <c r="I26" t="s">
-        <v>201</v>
-      </c>
       <c r="J26" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L26">
         <v>12</v>
       </c>
       <c r="M26" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N26">
         <v>69.09</v>
@@ -9911,34 +9918,34 @@
         <v>355</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K27" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L27">
         <v>10</v>
       </c>
       <c r="M27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N27">
         <v>18.2</v>
@@ -9979,34 +9986,34 @@
         <v>209</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H28" t="s">
+        <v>162</v>
+      </c>
+      <c r="I28" t="s">
         <v>163</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="K28" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="J28" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="K28" s="24" t="s">
-        <v>165</v>
       </c>
       <c r="L28">
         <v>13</v>
       </c>
       <c r="M28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N28">
         <v>66</v>

</xml_diff>

<commit_message>
Make additional corrections addressing #8
In addition to the Java model, changes were made to the highway
and project list while working to correct issue #8.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="287">
   <si>
     <t>Cost</t>
   </si>
@@ -884,6 +884,9 @@
   </si>
   <si>
     <t>South St Reverse Direction</t>
+  </si>
+  <si>
+    <t>Makaiwa Frontage Road</t>
   </si>
 </sst>
 </file>
@@ -3709,77 +3712,118 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>40</v>
+      </c>
+      <c r="D49" t="s">
+        <v>286</v>
+      </c>
+      <c r="E49" t="s">
+        <v>232</v>
+      </c>
+      <c r="F49" t="s">
+        <v>232</v>
+      </c>
+      <c r="G49" t="s">
+        <v>239</v>
+      </c>
+      <c r="K49" s="5">
+        <v>0</v>
+      </c>
+      <c r="L49" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>0</v>
+      </c>
+      <c r="R49" s="8">
+        <v>0</v>
+      </c>
+      <c r="S49" s="8">
+        <v>0</v>
+      </c>
+      <c r="T49" s="8">
+        <v>0</v>
+      </c>
+      <c r="U49" s="8">
+        <v>0</v>
+      </c>
+      <c r="V49" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
       <c r="K50"/>
       <c r="L50"/>
     </row>
-    <row r="51" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H51" s="4"/>
       <c r="K51"/>
       <c r="L51"/>
     </row>
-    <row r="52" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H52" s="4"/>
       <c r="K52"/>
       <c r="L52"/>
     </row>
-    <row r="53" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H53" s="4"/>
       <c r="K53"/>
       <c r="L53"/>
     </row>
-    <row r="54" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H54" s="4"/>
       <c r="K54"/>
       <c r="L54"/>
     </row>
-    <row r="55" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H55" s="4"/>
       <c r="K55"/>
       <c r="L55"/>
     </row>
-    <row r="56" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H56" s="4"/>
       <c r="K56"/>
       <c r="L56"/>
     </row>
-    <row r="57" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H57" s="4"/>
       <c r="K57"/>
       <c r="L57"/>
     </row>
-    <row r="58" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
       <c r="K58"/>
       <c r="L58"/>
     </row>
-    <row r="59" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H59" s="4"/>
       <c r="K59"/>
       <c r="L59"/>
     </row>
-    <row r="60" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H60" s="4"/>
       <c r="K60"/>
       <c r="L60"/>
     </row>
-    <row r="61" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H61" s="4"/>
       <c r="K61"/>
       <c r="L61"/>
     </row>
-    <row r="62" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H62" s="4"/>
       <c r="K62"/>
       <c r="L62"/>
     </row>
-    <row r="63" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H63" s="4"/>
       <c r="K63"/>
       <c r="L63"/>
     </row>
-    <row r="64" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H64" s="4"/>
       <c r="K64"/>
       <c r="L64"/>

</xml_diff>

<commit_message>
Update two projects post-TAC meeting
ProjID 33 (Makakilo Frontage Road) was removed from the
2040 scenario.
ProjID 11 (H1 PM WB Shoulder Lane) was shortened to drop
at Moanalua Rd instead of the H1/H2 merge.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -2391,7 +2391,7 @@
         <v>116</v>
       </c>
       <c r="F20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>122</v>
@@ -3445,7 +3445,7 @@
         <v>0</v>
       </c>
       <c r="V42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Move project 357 to mid range dev funded
Also, change ID to 308.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -2527,7 +2527,7 @@
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4">
-        <v>357</v>
+        <v>308</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>263</v>
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="T23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23">
         <v>0</v>

</xml_diff>

<commit_message>
Revised Networks with HDOT improvments this summer. 1.  H-1 AM EB Shoulder Kualakai to Kunia Rd. 2.  AM zipper lane 2 lanes. 3.  No PM HOV H-1 EB. 4.  No PM HOV H-2 SB 5.  No PM Moanalua Fwy EB.
Also updated the project management tool.xlsx with these additional projects.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="305">
   <si>
     <t>Cost</t>
   </si>
@@ -887,6 +887,60 @@
   </si>
   <si>
     <t>Makaiwa Frontage Road</t>
+  </si>
+  <si>
+    <t>East-West Arterial</t>
+  </si>
+  <si>
+    <t>UHWO Roads</t>
+  </si>
+  <si>
+    <t>Hoopili Roads</t>
+  </si>
+  <si>
+    <t>AM ZIPPER Lane</t>
+  </si>
+  <si>
+    <t>Pearl Harbor Exit from zipper</t>
+  </si>
+  <si>
+    <t>Added Capacity</t>
+  </si>
+  <si>
+    <t>HDOT</t>
+  </si>
+  <si>
+    <t>increased capacity per HDOT</t>
+  </si>
+  <si>
+    <t>H-2 HOV SB PM Removal</t>
+  </si>
+  <si>
+    <t>H-2 Mililani Interchange</t>
+  </si>
+  <si>
+    <t>Removed PM HOV lane (added lane back to GP lanes)</t>
+  </si>
+  <si>
+    <t>H-1 HOV WB PM Removal</t>
+  </si>
+  <si>
+    <t>Keehi Interchange</t>
+  </si>
+  <si>
+    <t>Moanalua HOV EB PM Removal</t>
+  </si>
+  <si>
+    <t>Middle Street Merge</t>
+  </si>
+  <si>
+    <t>H-1 WB Shoulder Lane</t>
+  </si>
+  <si>
+    <t>Kualakai Pkwy</t>
+  </si>
+  <si>
+    <t>Kunia Road Interchange</t>
   </si>
 </sst>
 </file>
@@ -1751,10 +1805,10 @@
   <dimension ref="A1:AD99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,44 +3808,322 @@
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>41</v>
+      </c>
+      <c r="D50" t="s">
+        <v>287</v>
+      </c>
+      <c r="E50" t="s">
+        <v>232</v>
+      </c>
+      <c r="F50" t="s">
+        <v>235</v>
+      </c>
+      <c r="G50" t="s">
+        <v>239</v>
+      </c>
       <c r="H50" s="4"/>
       <c r="K50"/>
       <c r="L50"/>
+      <c r="Q50" s="8">
+        <v>0</v>
+      </c>
+      <c r="R50" s="8">
+        <v>0</v>
+      </c>
+      <c r="S50" s="8">
+        <v>0</v>
+      </c>
+      <c r="T50" s="8">
+        <v>0</v>
+      </c>
+      <c r="U50" s="8">
+        <v>0</v>
+      </c>
+      <c r="V50" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>42</v>
+      </c>
+      <c r="D51" t="s">
+        <v>288</v>
+      </c>
+      <c r="G51" t="s">
+        <v>239</v>
+      </c>
       <c r="H51" s="4"/>
       <c r="K51"/>
       <c r="L51"/>
+      <c r="Q51" s="8">
+        <v>0</v>
+      </c>
+      <c r="R51" s="8">
+        <v>0</v>
+      </c>
+      <c r="S51" s="8">
+        <v>0</v>
+      </c>
+      <c r="T51" s="8">
+        <v>0</v>
+      </c>
+      <c r="U51" s="8">
+        <v>0</v>
+      </c>
+      <c r="V51" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>43</v>
+      </c>
+      <c r="D52" t="s">
+        <v>289</v>
+      </c>
+      <c r="G52" t="s">
+        <v>239</v>
+      </c>
       <c r="H52" s="4"/>
       <c r="K52"/>
       <c r="L52"/>
+      <c r="Q52" s="8">
+        <v>0</v>
+      </c>
+      <c r="R52" s="8">
+        <v>0</v>
+      </c>
+      <c r="S52" s="8">
+        <v>0</v>
+      </c>
+      <c r="T52" s="8">
+        <v>0</v>
+      </c>
+      <c r="U52" s="8">
+        <v>0</v>
+      </c>
+      <c r="V52" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>44</v>
+      </c>
+      <c r="D53" t="s">
+        <v>290</v>
+      </c>
+      <c r="E53" t="s">
+        <v>117</v>
+      </c>
+      <c r="F53" t="s">
+        <v>291</v>
+      </c>
+      <c r="G53" t="s">
+        <v>292</v>
+      </c>
       <c r="H53" s="4"/>
-      <c r="K53"/>
-      <c r="L53"/>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="O53" t="s">
+        <v>293</v>
+      </c>
+      <c r="P53" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>45</v>
+      </c>
+      <c r="D54" t="s">
+        <v>295</v>
+      </c>
+      <c r="E54" t="s">
+        <v>296</v>
+      </c>
+      <c r="F54" t="s">
+        <v>117</v>
+      </c>
+      <c r="G54" t="s">
+        <v>297</v>
+      </c>
       <c r="H54" s="4"/>
-      <c r="K54"/>
-      <c r="L54"/>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="8">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>1</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>46</v>
+      </c>
+      <c r="D55" t="s">
+        <v>298</v>
+      </c>
+      <c r="E55" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" t="s">
+        <v>299</v>
+      </c>
+      <c r="G55" t="s">
+        <v>297</v>
+      </c>
       <c r="H55" s="4"/>
-      <c r="K55"/>
-      <c r="L55"/>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="8">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>1</v>
+      </c>
+      <c r="S55">
+        <v>1</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="U55">
+        <v>1</v>
+      </c>
+      <c r="V55">
+        <v>1</v>
+      </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>47</v>
+      </c>
+      <c r="D56" t="s">
+        <v>300</v>
+      </c>
+      <c r="E56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F56" t="s">
+        <v>301</v>
+      </c>
+      <c r="G56" t="s">
+        <v>297</v>
+      </c>
       <c r="H56" s="4"/>
-      <c r="K56"/>
-      <c r="L56"/>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="8">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>1</v>
+      </c>
+      <c r="S56">
+        <v>1</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+      <c r="V56">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>48</v>
+      </c>
+      <c r="D57" t="s">
+        <v>302</v>
+      </c>
+      <c r="E57" t="s">
+        <v>303</v>
+      </c>
+      <c r="F57" t="s">
+        <v>304</v>
+      </c>
+      <c r="G57" t="s">
+        <v>292</v>
+      </c>
       <c r="H57" s="4"/>
-      <c r="K57"/>
-      <c r="L57"/>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="8">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <v>1</v>
+      </c>
+      <c r="V57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H58" s="4"/>
@@ -4180,8 +4512,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I91:I93"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="3" scale="20" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="3" scale="20" orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5056,8 +5388,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="H12 H10 H85:H87"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="3" scale="20" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="3" scale="20" orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Correct master network error
Project 8 was duplicated in both p1 and p2. Removed it
from p2. Cleared filter from project management sheet.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4308" yWindow="456" windowWidth="18516" windowHeight="12012"/>
+    <workbookView xWindow="4305" yWindow="450" windowWidth="18510" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Proj Attributes and Scenarios" sheetId="1" r:id="rId1"/>
@@ -1814,8 +1814,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2245360" y="0"/>
-          <a:ext cx="10303436" cy="1313343"/>
+          <a:off x="2197100" y="0"/>
+          <a:ext cx="10049436" cy="1366683"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -2427,75 +2427,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="W75" sqref="W75"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="7" width="32.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" style="5" customWidth="1"/>
-    <col min="13" max="15" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" style="18" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="7" width="32.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="5" customWidth="1"/>
+    <col min="13" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
     <col min="17" max="17" width="18" style="5" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P1" s="16"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P2" s="16"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P3" s="16"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P4" s="16"/>
       <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P5" s="16"/>
       <c r="Q5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P6" s="16"/>
       <c r="Q6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P7" s="16"/>
       <c r="Q7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2527,7 +2527,7 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
-    <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>273</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>5</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>7</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>8</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>14</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>15</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>16</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>17</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>18</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>19</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>21</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>22</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>23</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>24</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>26</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>27</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>28</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>29</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>30</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>31</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>32</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>33</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>34</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>35</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>36</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>37</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>38</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>39</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>40</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>41</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>42</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>44</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>45</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>46</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>47</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>48</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
         <v>101</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="29">
         <v>102</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="29">
         <v>103</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="29">
         <v>104</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="29">
         <v>105</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="29">
         <v>106</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="29">
         <v>107</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="29">
         <v>108</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="29">
         <v>109</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="29">
         <v>110</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="29">
         <v>111</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="29">
         <v>112</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="29">
         <v>113</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="29">
         <v>114</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="29">
         <v>115</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="29">
         <v>116</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="29">
         <v>117</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="29">
         <v>118</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>119</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>120</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -5490,7 +5490,7 @@
       <c r="T78" s="8"/>
       <c r="U78" s="8"/>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -5503,7 +5503,7 @@
       <c r="T79" s="8"/>
       <c r="U79" s="8"/>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -5516,7 +5516,7 @@
       <c r="T80" s="8"/>
       <c r="U80" s="8"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -5528,7 +5528,7 @@
       <c r="T81" s="8"/>
       <c r="U81" s="8"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -5540,7 +5540,7 @@
       <c r="T82" s="8"/>
       <c r="U82" s="8"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -5552,7 +5552,7 @@
       <c r="T83" s="8"/>
       <c r="U83" s="8"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -5564,7 +5564,7 @@
       <c r="T84" s="8"/>
       <c r="U84" s="8"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -5576,7 +5576,7 @@
       <c r="T85" s="8"/>
       <c r="U85" s="8"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -5588,7 +5588,7 @@
       <c r="T86" s="8"/>
       <c r="U86" s="8"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -5600,7 +5600,7 @@
       <c r="T87" s="8"/>
       <c r="U87" s="8"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -5613,7 +5613,7 @@
       <c r="T88" s="8"/>
       <c r="U88" s="8"/>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -5626,7 +5626,7 @@
       <c r="T89" s="8"/>
       <c r="U89" s="8"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -5641,7 +5641,7 @@
       <c r="T90" s="8"/>
       <c r="U90" s="8"/>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -5656,7 +5656,7 @@
       <c r="T91" s="8"/>
       <c r="U91" s="8"/>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -5671,14 +5671,14 @@
       <c r="T92" s="8"/>
       <c r="U92" s="8"/>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="H93" s="4"/>
       <c r="J93" s="5"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -5686,16 +5686,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:V77">
-    <filterColumn colId="19">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="21">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A10:T48">
       <sortCondition ref="A9:A30"/>
     </sortState>
@@ -5723,27 +5713,27 @@
       <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="6" width="32.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="6" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5768,7 +5758,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -5815,7 +5805,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>38</v>
@@ -5835,7 +5825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>45</v>
@@ -5858,7 +5848,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>49</v>
@@ -5881,7 +5871,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -5905,7 +5895,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -5928,7 +5918,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -5952,7 +5942,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>63</v>
@@ -5972,7 +5962,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>69</v>
@@ -5992,7 +5982,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>91</v>
       </c>
@@ -6015,7 +6005,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>97</v>
       </c>
@@ -6038,7 +6028,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>104</v>
       </c>
@@ -6054,7 +6044,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>99</v>
       </c>
@@ -6065,7 +6055,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>111</v>
       </c>
@@ -6076,7 +6066,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>27</v>
       </c>
@@ -6097,7 +6087,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>35</v>
       </c>
@@ -6116,7 +6106,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>19</v>
       </c>
@@ -6140,7 +6130,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -6150,7 +6140,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -6160,7 +6150,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -6170,7 +6160,7 @@
       <c r="J28"/>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -6180,7 +6170,7 @@
       <c r="J29"/>
       <c r="K29"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -6190,7 +6180,7 @@
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -6200,7 +6190,7 @@
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -6210,7 +6200,7 @@
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -6220,7 +6210,7 @@
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -6230,7 +6220,7 @@
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -6240,7 +6230,7 @@
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -6250,7 +6240,7 @@
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -6260,7 +6250,7 @@
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -6270,7 +6260,7 @@
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -6280,7 +6270,7 @@
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -6290,7 +6280,7 @@
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -6300,129 +6290,129 @@
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G42" s="4"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G43" s="4"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G44" s="4"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G45" s="4"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G46" s="4"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G47" s="4"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G48" s="4"/>
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G49" s="4"/>
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G50" s="4"/>
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G51" s="4"/>
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G52" s="4"/>
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G53" s="4"/>
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G54" s="4"/>
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G55" s="4"/>
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G56" s="4"/>
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G57" s="4"/>
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G58" s="4"/>
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J62"/>
       <c r="K62"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J63"/>
       <c r="K63"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="G64" s="4"/>
       <c r="O64" s="4"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="O65" s="4"/>
     </row>
-    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J66" s="8"/>
       <c r="K66" s="5"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="F67" s="4"/>
@@ -6430,119 +6420,119 @@
       <c r="I67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="G68" s="4"/>
       <c r="I68" s="4"/>
       <c r="O68" s="4"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="O70" s="4"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="O71" s="4"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="O72" s="4"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="O73" s="4"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="O74" s="4"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="G75" s="4"/>
       <c r="O75" s="4"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="G76" s="4"/>
       <c r="O76" s="4"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="G77" s="4"/>
       <c r="O77" s="4"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="G78" s="4"/>
       <c r="O78" s="4"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="G79" s="4"/>
       <c r="O79" s="4"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="G80" s="4"/>
       <c r="O80" s="4"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="G81" s="4"/>
       <c r="O81" s="4"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="O82" s="4"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="G83" s="4"/>
       <c r="O83" s="4"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="G84" s="4"/>
       <c r="O84" s="4"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="G85" s="4"/>
@@ -6551,7 +6541,7 @@
       <c r="K85" s="8"/>
       <c r="O85" s="4"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="G86" s="4"/>
@@ -6560,7 +6550,7 @@
       <c r="K86" s="8"/>
       <c r="O86" s="4"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="G87" s="4"/>
@@ -6569,7 +6559,7 @@
       <c r="K87" s="8"/>
       <c r="O87" s="4"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -6593,9 +6583,9 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>271</v>
       </c>
@@ -6603,7 +6593,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -6611,7 +6601,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -6625,7 +6615,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>27</v>
       </c>
@@ -6643,7 +6633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>37</v>
       </c>
@@ -6661,7 +6651,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>41</v>
       </c>
@@ -6679,7 +6669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>36</v>
       </c>
@@ -6697,7 +6687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>39</v>
       </c>
@@ -6715,7 +6705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -6733,7 +6723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>30</v>
       </c>
@@ -6751,7 +6741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>33</v>
       </c>
@@ -6769,7 +6759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -6787,7 +6777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -6805,7 +6795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -6823,7 +6813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>18</v>
       </c>
@@ -6841,7 +6831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>19</v>
       </c>
@@ -6859,7 +6849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>42</v>
       </c>
@@ -6877,7 +6867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43</v>
       </c>
@@ -6895,7 +6885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>34</v>
       </c>
@@ -6913,7 +6903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -6931,7 +6921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>40</v>
       </c>
@@ -6949,7 +6939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>31</v>
       </c>
@@ -6967,7 +6957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -6985,7 +6975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -7003,7 +6993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>38</v>
       </c>
@@ -7021,7 +7011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>14</v>
       </c>
@@ -7039,7 +7029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>10</v>
       </c>
@@ -7057,7 +7047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -7075,7 +7065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>12</v>
       </c>
@@ -7093,7 +7083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -7111,7 +7101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>23</v>
       </c>
@@ -7129,7 +7119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>28</v>
       </c>
@@ -7147,7 +7137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>11</v>
       </c>
@@ -7165,7 +7155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>44</v>
       </c>
@@ -7183,7 +7173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>16</v>
       </c>
@@ -7201,7 +7191,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>20</v>
       </c>
@@ -7219,7 +7209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -7237,7 +7227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>24</v>
       </c>
@@ -7255,7 +7245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>25</v>
       </c>
@@ -7273,7 +7263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>15</v>
       </c>
@@ -7291,7 +7281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>32</v>
       </c>
@@ -7309,7 +7299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>13</v>
       </c>
@@ -7327,7 +7317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="I43">
         <v>37</v>
@@ -7337,7 +7327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I44">
         <v>37</v>
       </c>
@@ -7346,7 +7336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I45">
         <v>37</v>
       </c>
@@ -7355,7 +7345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I46">
         <v>27</v>
       </c>
@@ -7364,7 +7354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I47">
         <v>33</v>
       </c>
@@ -7373,7 +7363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I48">
         <v>36</v>
       </c>
@@ -7382,7 +7372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I49">
         <v>37</v>
       </c>
@@ -7391,7 +7381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I50">
         <v>27</v>
       </c>
@@ -7400,7 +7390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I51">
         <v>27</v>
       </c>
@@ -7409,7 +7399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I52">
         <v>37</v>
       </c>
@@ -7418,7 +7408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I53">
         <v>27</v>
       </c>
@@ -7427,7 +7417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I54">
         <v>37</v>
       </c>
@@ -7436,7 +7426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I55">
         <v>39</v>
       </c>
@@ -7445,7 +7435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I56">
         <v>31</v>
       </c>
@@ -7454,7 +7444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I57">
         <v>41</v>
       </c>
@@ -7463,7 +7453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I58">
         <v>30</v>
       </c>
@@ -7472,7 +7462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I59">
         <v>30</v>
       </c>
@@ -7481,7 +7471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I60">
         <v>32</v>
       </c>
@@ -7490,7 +7480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I61">
         <v>32</v>
       </c>
@@ -7499,7 +7489,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I62">
         <v>32</v>
       </c>
@@ -7508,7 +7498,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I63">
         <v>31</v>
       </c>
@@ -7517,7 +7507,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I64">
         <v>42</v>
       </c>
@@ -7526,7 +7516,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I65">
         <v>41</v>
       </c>
@@ -7535,7 +7525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I66">
         <v>5</v>
       </c>
@@ -7544,7 +7534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I67">
         <v>41</v>
       </c>
@@ -7553,7 +7543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I68">
         <v>5</v>
       </c>
@@ -7562,7 +7552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I69">
         <v>5</v>
       </c>
@@ -7571,7 +7561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I70">
         <v>5</v>
       </c>
@@ -7580,7 +7570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I71">
         <v>41</v>
       </c>
@@ -7589,7 +7579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I72">
         <v>41</v>
       </c>
@@ -7598,7 +7588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I73">
         <v>5</v>
       </c>
@@ -7607,7 +7597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I74">
         <v>41</v>
       </c>
@@ -7616,7 +7606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I75">
         <v>41</v>
       </c>
@@ -7625,7 +7615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I76">
         <v>5</v>
       </c>
@@ -7634,7 +7624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I77">
         <v>5</v>
       </c>
@@ -7643,7 +7633,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I78">
         <v>41</v>
       </c>
@@ -7652,7 +7642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I79">
         <v>41</v>
       </c>
@@ -7661,7 +7651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I80">
         <v>41</v>
       </c>
@@ -7670,7 +7660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I81">
         <v>41</v>
       </c>
@@ -7679,7 +7669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I82">
         <v>41</v>
       </c>
@@ -7688,7 +7678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I83">
         <v>6</v>
       </c>
@@ -7697,7 +7687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I84">
         <v>6</v>
       </c>
@@ -7706,7 +7696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I85">
         <v>6</v>
       </c>
@@ -7715,7 +7705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I86">
         <v>30</v>
       </c>
@@ -7724,7 +7714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I87">
         <v>30</v>
       </c>
@@ -7733,7 +7723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I88">
         <v>42</v>
       </c>
@@ -7742,7 +7732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I89">
         <v>41</v>
       </c>
@@ -7751,7 +7741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I90">
         <v>41</v>
       </c>
@@ -7760,7 +7750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I91">
         <v>41</v>
       </c>
@@ -7769,7 +7759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I92">
         <v>41</v>
       </c>
@@ -7778,7 +7768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I93">
         <v>41</v>
       </c>
@@ -7787,7 +7777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I94">
         <v>18</v>
       </c>
@@ -7796,7 +7786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I95">
         <v>30</v>
       </c>
@@ -7805,7 +7795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I96">
         <v>30</v>
       </c>
@@ -7814,7 +7804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I97">
         <v>30</v>
       </c>
@@ -7823,7 +7813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I98">
         <v>30</v>
       </c>
@@ -7832,7 +7822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I99">
         <v>30</v>
       </c>
@@ -7841,7 +7831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I100">
         <v>30</v>
       </c>
@@ -7850,7 +7840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I101">
         <v>30</v>
       </c>
@@ -7859,7 +7849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I102">
         <v>30</v>
       </c>
@@ -7868,7 +7858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I103">
         <v>32</v>
       </c>
@@ -7877,7 +7867,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I104">
         <v>32</v>
       </c>
@@ -7886,7 +7876,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I105">
         <v>32</v>
       </c>
@@ -7895,7 +7885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I106">
         <v>32</v>
       </c>
@@ -7904,7 +7894,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I107">
         <v>18</v>
       </c>
@@ -7913,7 +7903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I108">
         <v>18</v>
       </c>
@@ -7922,7 +7912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I109">
         <v>41</v>
       </c>
@@ -7931,7 +7921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I110">
         <v>42</v>
       </c>
@@ -7940,7 +7930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I111">
         <v>42</v>
       </c>
@@ -7949,7 +7939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I112">
         <v>42</v>
       </c>
@@ -7958,7 +7948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I113">
         <v>42</v>
       </c>
@@ -7967,7 +7957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I114">
         <v>42</v>
       </c>
@@ -7976,7 +7966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="115" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I115">
         <v>42</v>
       </c>
@@ -7985,7 +7975,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I116">
         <v>42</v>
       </c>
@@ -7994,7 +7984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I117">
         <v>42</v>
       </c>
@@ -8003,7 +7993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I118">
         <v>42</v>
       </c>
@@ -8012,7 +8002,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I119">
         <v>14</v>
       </c>
@@ -8021,7 +8011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I120">
         <v>23</v>
       </c>
@@ -8030,7 +8020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I121">
         <v>2</v>
       </c>
@@ -8039,7 +8029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I122">
         <v>25</v>
       </c>
@@ -8048,7 +8038,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="123" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I123">
         <v>25</v>
       </c>
@@ -8057,7 +8047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="124" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I124">
         <v>25</v>
       </c>
@@ -8066,7 +8056,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="125" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I125">
         <v>25</v>
       </c>
@@ -8075,7 +8065,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="126" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I126">
         <v>25</v>
       </c>
@@ -8084,7 +8074,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="127" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I127">
         <v>25</v>
       </c>
@@ -8093,7 +8083,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I128">
         <v>25</v>
       </c>
@@ -8102,7 +8092,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="129" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I129">
         <v>26</v>
       </c>
@@ -8111,7 +8101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I130">
         <v>2</v>
       </c>
@@ -8120,7 +8110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I131">
         <v>2</v>
       </c>
@@ -8129,7 +8119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I132">
         <v>39</v>
       </c>
@@ -8138,7 +8128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I133">
         <v>2</v>
       </c>
@@ -8147,7 +8137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I134">
         <v>2</v>
       </c>
@@ -8156,7 +8146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I135">
         <v>2</v>
       </c>
@@ -8165,7 +8155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I136">
         <v>14</v>
       </c>
@@ -8174,7 +8164,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I137">
         <v>14</v>
       </c>
@@ -8183,7 +8173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I138">
         <v>14</v>
       </c>
@@ -8192,7 +8182,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I139">
         <v>14</v>
       </c>
@@ -8201,7 +8191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I140">
         <v>14</v>
       </c>
@@ -8210,7 +8200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I141">
         <v>14</v>
       </c>
@@ -8219,7 +8209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I142">
         <v>14</v>
       </c>
@@ -8228,7 +8218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I143">
         <v>23</v>
       </c>
@@ -8237,7 +8227,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I144">
         <v>14</v>
       </c>
@@ -8246,7 +8236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I145">
         <v>23</v>
       </c>
@@ -8255,7 +8245,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I146">
         <v>14</v>
       </c>
@@ -8264,7 +8254,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I147">
         <v>14</v>
       </c>
@@ -8273,7 +8263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="148" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I148">
         <v>23</v>
       </c>
@@ -8282,7 +8272,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="149" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I149">
         <v>14</v>
       </c>
@@ -8291,7 +8281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I150">
         <v>14</v>
       </c>
@@ -8300,7 +8290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I151">
         <v>14</v>
       </c>
@@ -8309,7 +8299,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="152" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I152">
         <v>23</v>
       </c>
@@ -8318,7 +8308,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I153">
         <v>23</v>
       </c>
@@ -8327,7 +8317,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="154" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I154">
         <v>23</v>
       </c>
@@ -8336,7 +8326,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="155" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I155">
         <v>23</v>
       </c>
@@ -8345,7 +8335,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="156" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I156">
         <v>14</v>
       </c>
@@ -8354,7 +8344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I157">
         <v>14</v>
       </c>
@@ -8363,7 +8353,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I158">
         <v>14</v>
       </c>
@@ -8372,7 +8362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I159">
         <v>14</v>
       </c>
@@ -8381,7 +8371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="160" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I160">
         <v>14</v>
       </c>
@@ -8390,7 +8380,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="161" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I161">
         <v>14</v>
       </c>
@@ -8399,7 +8389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I162">
         <v>23</v>
       </c>
@@ -8408,7 +8398,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I163">
         <v>23</v>
       </c>
@@ -8417,7 +8407,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I164">
         <v>23</v>
       </c>
@@ -8426,7 +8416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="165" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I165">
         <v>23</v>
       </c>
@@ -8435,7 +8425,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="166" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I166">
         <v>23</v>
       </c>
@@ -8444,7 +8434,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I167">
         <v>23</v>
       </c>
@@ -8453,7 +8443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="168" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I168">
         <v>14</v>
       </c>
@@ -8462,7 +8452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="169" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I169">
         <v>14</v>
       </c>
@@ -8471,7 +8461,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I170">
         <v>14</v>
       </c>
@@ -8480,7 +8470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="171" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I171">
         <v>23</v>
       </c>
@@ -8489,7 +8479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="172" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I172">
         <v>15</v>
       </c>
@@ -8498,7 +8488,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="173" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I173">
         <v>15</v>
       </c>
@@ -8507,7 +8497,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="174" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I174">
         <v>2</v>
       </c>
@@ -8516,7 +8506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I175">
         <v>2</v>
       </c>
@@ -8525,7 +8515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I176">
         <v>2</v>
       </c>
@@ -8534,7 +8524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I177">
         <v>2</v>
       </c>
@@ -8543,7 +8533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I178">
         <v>2</v>
       </c>
@@ -8552,7 +8542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I179">
         <v>2</v>
       </c>
@@ -8561,7 +8551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I180">
         <v>2</v>
       </c>
@@ -8570,7 +8560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I181">
         <v>2</v>
       </c>
@@ -8579,7 +8569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I182">
         <v>26</v>
       </c>
@@ -8588,7 +8578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I183">
         <v>2</v>
       </c>
@@ -8597,7 +8587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I184">
         <v>2</v>
       </c>
@@ -8606,7 +8596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I185">
         <v>2</v>
       </c>
@@ -8615,7 +8605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I186">
         <v>2</v>
       </c>
@@ -8624,7 +8614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I187">
         <v>2</v>
       </c>
@@ -8633,7 +8623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I188">
         <v>2</v>
       </c>
@@ -8642,7 +8632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I189">
         <v>2</v>
       </c>
@@ -8651,7 +8641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I190">
         <v>2</v>
       </c>
@@ -8660,7 +8650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I191">
         <v>23</v>
       </c>
@@ -8669,7 +8659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="192" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I192">
         <v>23</v>
       </c>
@@ -8678,7 +8668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="193" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I193">
         <v>14</v>
       </c>
@@ -8687,7 +8677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="194" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I194">
         <v>23</v>
       </c>
@@ -8696,7 +8686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="195" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I195">
         <v>2</v>
       </c>
@@ -8705,7 +8695,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I196">
         <v>2</v>
       </c>
@@ -8714,7 +8704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I197">
         <v>9</v>
       </c>
@@ -8723,7 +8713,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I198">
         <v>2</v>
       </c>
@@ -8732,7 +8722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I199">
         <v>2</v>
       </c>
@@ -8741,7 +8731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I200">
         <v>13</v>
       </c>
@@ -8750,7 +8740,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="201" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I201">
         <v>23</v>
       </c>
@@ -8759,7 +8749,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="202" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I202">
         <v>23</v>
       </c>
@@ -8768,7 +8758,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="203" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I203">
         <v>13</v>
       </c>
@@ -8777,7 +8767,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="204" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I204">
         <v>13</v>
       </c>
@@ -8786,7 +8776,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="205" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I205">
         <v>13</v>
       </c>
@@ -8795,7 +8785,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="206" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I206">
         <v>13</v>
       </c>
@@ -8804,7 +8794,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="207" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I207">
         <v>23</v>
       </c>
@@ -8813,7 +8803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="208" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I208">
         <v>23</v>
       </c>
@@ -8822,7 +8812,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="209" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I209">
         <v>2</v>
       </c>
@@ -8831,7 +8821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I210">
         <v>2</v>
       </c>
@@ -8840,7 +8830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I211">
         <v>2</v>
       </c>
@@ -8849,7 +8839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I212">
         <v>2</v>
       </c>
@@ -8858,7 +8848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I213">
         <v>2</v>
       </c>
@@ -8867,7 +8857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I214">
         <v>34</v>
       </c>
@@ -8876,7 +8866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="215" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I215">
         <v>33</v>
       </c>
@@ -8885,7 +8875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I216">
         <v>4</v>
       </c>
@@ -8894,7 +8884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="217" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I217">
         <v>40</v>
       </c>
@@ -8903,7 +8893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I218">
         <v>4</v>
       </c>
@@ -8912,7 +8902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="219" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I219">
         <v>4</v>
       </c>
@@ -8921,7 +8911,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="220" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I220">
         <v>4</v>
       </c>
@@ -8930,7 +8920,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="221" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I221">
         <v>4</v>
       </c>
@@ -8939,7 +8929,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="222" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I222">
         <v>34</v>
       </c>
@@ -8948,7 +8938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I223">
         <v>34</v>
       </c>
@@ -8957,7 +8947,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="224" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I224">
         <v>34</v>
       </c>
@@ -8966,7 +8956,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I225">
         <v>34</v>
       </c>
@@ -8975,7 +8965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I226">
         <v>15</v>
       </c>
@@ -8984,7 +8974,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="227" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I227">
         <v>15</v>
       </c>
@@ -8993,7 +8983,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="228" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I228">
         <v>15</v>
       </c>
@@ -9002,7 +8992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="229" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I229">
         <v>15</v>
       </c>
@@ -9011,7 +9001,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="230" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I230">
         <v>15</v>
       </c>
@@ -9020,7 +9010,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="231" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I231">
         <v>12</v>
       </c>
@@ -9029,7 +9019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="232" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I232">
         <v>14</v>
       </c>
@@ -9038,7 +9028,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="233" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I233">
         <v>14</v>
       </c>
@@ -9047,7 +9037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="234" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I234">
         <v>23</v>
       </c>
@@ -9056,7 +9046,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="235" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I235">
         <v>23</v>
       </c>
@@ -9065,7 +9055,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="236" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I236">
         <v>28</v>
       </c>
@@ -9074,7 +9064,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="237" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I237">
         <v>11</v>
       </c>
@@ -9083,7 +9073,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="238" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I238">
         <v>28</v>
       </c>
@@ -9092,7 +9082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="239" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I239">
         <v>32</v>
       </c>
@@ -9101,7 +9091,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="240" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I240">
         <v>32</v>
       </c>
@@ -9110,7 +9100,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="241" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I241">
         <v>32</v>
       </c>
@@ -9119,7 +9109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="242" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I242">
         <v>43</v>
       </c>
@@ -9128,7 +9118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I243">
         <v>16</v>
       </c>
@@ -9137,7 +9127,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="244" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I244">
         <v>12</v>
       </c>
@@ -9146,7 +9136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="245" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I245">
         <v>36</v>
       </c>
@@ -9155,7 +9145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I246">
         <v>12</v>
       </c>
@@ -9164,7 +9154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="247" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I247">
         <v>16</v>
       </c>
@@ -9173,7 +9163,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="248" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I248">
         <v>10</v>
       </c>
@@ -9182,7 +9172,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="249" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I249">
         <v>10</v>
       </c>
@@ -9191,7 +9181,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="250" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I250">
         <v>10</v>
       </c>
@@ -9200,7 +9190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="251" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I251">
         <v>43</v>
       </c>
@@ -9209,7 +9199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I252">
         <v>43</v>
       </c>
@@ -9218,7 +9208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="253" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I253">
         <v>37</v>
       </c>
@@ -9227,7 +9217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I254">
         <v>43</v>
       </c>
@@ -9236,7 +9226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I255">
         <v>43</v>
       </c>
@@ -9245,7 +9235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I256">
         <v>37</v>
       </c>
@@ -9254,7 +9244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I257">
         <v>43</v>
       </c>
@@ -9263,7 +9253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I258">
         <v>43</v>
       </c>
@@ -9272,7 +9262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I259">
         <v>43</v>
       </c>
@@ -9281,7 +9271,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I260">
         <v>43</v>
       </c>
@@ -9290,7 +9280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I261">
         <v>43</v>
       </c>
@@ -9299,7 +9289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I262">
         <v>43</v>
       </c>
@@ -9308,7 +9298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I263">
         <v>43</v>
       </c>
@@ -9317,7 +9307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I264">
         <v>16</v>
       </c>
@@ -9326,7 +9316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="265" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I265">
         <v>37</v>
       </c>
@@ -9335,7 +9325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I266">
         <v>22</v>
       </c>
@@ -9344,7 +9334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="267" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I267">
         <v>40</v>
       </c>
@@ -9353,7 +9343,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="268" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I268">
         <v>40</v>
       </c>
@@ -9362,7 +9352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="269" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I269">
         <v>40</v>
       </c>
@@ -9371,7 +9361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="270" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I270">
         <v>27</v>
       </c>
@@ -9380,7 +9370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I271">
         <v>28</v>
       </c>
@@ -9389,7 +9379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="272" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I272">
         <v>27</v>
       </c>
@@ -9398,7 +9388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I273">
         <v>40</v>
       </c>
@@ -9407,7 +9397,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="274" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I274">
         <v>12</v>
       </c>
@@ -9416,7 +9406,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="275" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I275">
         <v>43</v>
       </c>
@@ -9425,7 +9415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I276">
         <v>43</v>
       </c>
@@ -9434,7 +9424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I277">
         <v>26</v>
       </c>
@@ -9443,7 +9433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I278">
         <v>26</v>
       </c>
@@ -9452,7 +9442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I279">
         <v>26</v>
       </c>
@@ -9461,7 +9451,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I280">
         <v>26</v>
       </c>
@@ -9470,7 +9460,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I281">
         <v>16</v>
       </c>
@@ -9479,7 +9469,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="282" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I282">
         <v>16</v>
       </c>
@@ -9488,7 +9478,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="283" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I283">
         <v>16</v>
       </c>
@@ -9497,7 +9487,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="284" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I284">
         <v>27</v>
       </c>
@@ -9506,7 +9496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I285">
         <v>24</v>
       </c>
@@ -9515,7 +9505,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="286" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I286">
         <v>24</v>
       </c>
@@ -9524,7 +9514,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="287" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I287">
         <v>24</v>
       </c>
@@ -9533,7 +9523,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="288" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I288">
         <v>24</v>
       </c>
@@ -9542,7 +9532,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="289" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I289">
         <v>28</v>
       </c>
@@ -9551,7 +9541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="290" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I290">
         <v>27</v>
       </c>
@@ -9560,7 +9550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I291">
         <v>40</v>
       </c>
@@ -9569,7 +9559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="292" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I292">
         <v>40</v>
       </c>
@@ -9578,7 +9568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="293" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I293">
         <v>40</v>
       </c>
@@ -9587,7 +9577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="294" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I294">
         <v>38</v>
       </c>
@@ -9596,7 +9586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="295" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I295">
         <v>29</v>
       </c>
@@ -9605,7 +9595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="296" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I296">
         <v>29</v>
       </c>
@@ -9614,7 +9604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="297" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I297">
         <v>10</v>
       </c>
@@ -9623,7 +9613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="298" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I298">
         <v>3</v>
       </c>
@@ -9632,7 +9622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="299" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I299">
         <v>3</v>
       </c>
@@ -9641,7 +9631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="300" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I300">
         <v>29</v>
       </c>
@@ -9650,7 +9640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="301" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I301">
         <v>29</v>
       </c>
@@ -9659,7 +9649,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="302" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I302">
         <v>28</v>
       </c>
@@ -9668,7 +9658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="303" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I303">
         <v>28</v>
       </c>
@@ -9677,7 +9667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="304" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I304">
         <v>44</v>
       </c>
@@ -9702,12 +9692,12 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="118" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>237</v>
       </c>
@@ -9775,7 +9765,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>27</v>
       </c>
@@ -9843,7 +9833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>37</v>
       </c>
@@ -9911,7 +9901,7 @@
         <v>233.1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>41</v>
       </c>
@@ -9979,7 +9969,7 @@
         <v>43.164000000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>39</v>
       </c>
@@ -10047,7 +10037,7 @@
         <v>10.713452725559549</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>36</v>
       </c>
@@ -10115,7 +10105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -10183,7 +10173,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>35</v>
       </c>
@@ -10251,7 +10241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -10319,7 +10309,7 @@
         <v>9.5399999999999991</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>248</v>
       </c>
@@ -10387,7 +10377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>33</v>
       </c>
@@ -10455,7 +10445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>30</v>
       </c>
@@ -10523,7 +10513,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>33</v>
       </c>
@@ -10591,7 +10581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>42</v>
       </c>
@@ -10659,7 +10649,7 @@
         <v>102.5</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>32</v>
       </c>
@@ -10727,7 +10717,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>34</v>
       </c>
@@ -10795,7 +10785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -10863,7 +10853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>40</v>
       </c>
@@ -10931,7 +10921,7 @@
         <v>216.88</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>31</v>
       </c>
@@ -10999,7 +10989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>38</v>
       </c>
@@ -11067,7 +11057,7 @@
         <v>24.15396614489789</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>26</v>
       </c>
@@ -11135,7 +11125,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>12</v>
       </c>
@@ -11203,7 +11193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>29</v>
       </c>
@@ -11271,7 +11261,7 @@
         <v>188.6</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>28</v>
       </c>
@@ -11339,7 +11329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>28</v>
       </c>
@@ -11407,7 +11397,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>16</v>
       </c>
@@ -11475,7 +11465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>20</v>
       </c>
@@ -11543,7 +11533,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -11627,9 +11617,9 @@
       <selection activeCell="F19" sqref="F19:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>305</v>
       </c>
@@ -11640,7 +11630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11651,7 +11641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11662,7 +11652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11673,7 +11663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11684,7 +11674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11695,7 +11685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11706,7 +11696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11720,7 +11710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11737,7 +11727,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -11754,7 +11744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -11771,7 +11761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14</v>
       </c>
@@ -11788,7 +11778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -11805,7 +11795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>16</v>
       </c>
@@ -11822,7 +11812,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>18</v>
       </c>
@@ -11839,7 +11829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>19</v>
       </c>
@@ -11857,7 +11847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>21</v>
       </c>
@@ -11877,7 +11867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>23</v>
       </c>
@@ -11894,7 +11884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>24</v>
       </c>
@@ -11911,7 +11901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>25</v>
       </c>
@@ -11928,7 +11918,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>26</v>
       </c>
@@ -11945,7 +11935,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>27</v>
       </c>
@@ -11962,7 +11952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>29</v>
       </c>
@@ -11979,7 +11969,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>30</v>
       </c>
@@ -11996,7 +11986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>31</v>
       </c>
@@ -12013,7 +12003,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>32</v>
       </c>
@@ -12030,7 +12020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>33</v>
       </c>
@@ -12047,7 +12037,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>35</v>
       </c>
@@ -12064,7 +12054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>38</v>
       </c>
@@ -12081,7 +12071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>40</v>
       </c>
@@ -12092,7 +12082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>41</v>
       </c>
@@ -12106,7 +12096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>42</v>
       </c>
@@ -12117,7 +12107,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>43</v>
       </c>
@@ -12128,7 +12118,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>101</v>
       </c>
@@ -12139,7 +12129,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>102</v>
       </c>
@@ -12147,7 +12137,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>103</v>
       </c>
@@ -12155,7 +12145,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>104</v>
       </c>
@@ -12163,7 +12153,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>105</v>
       </c>
@@ -12171,7 +12161,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>106</v>
       </c>
@@ -12179,7 +12169,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>107</v>
       </c>
@@ -12187,7 +12177,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>108</v>
       </c>
@@ -12195,7 +12185,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>109</v>
       </c>
@@ -12203,7 +12193,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>110</v>
       </c>
@@ -12211,7 +12201,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>111</v>
       </c>
@@ -12219,7 +12209,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>112</v>
       </c>
@@ -12227,7 +12217,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>113</v>
       </c>
@@ -12235,7 +12225,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
Round project length to two decimals
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -2423,7 +2423,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD97"/>
+  <dimension ref="A1:AI97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
@@ -2452,43 +2452,43 @@
     <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P1" s="16"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P2" s="16"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P3" s="16"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P4" s="16"/>
       <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P5" s="16"/>
       <c r="Q5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P6" s="16"/>
       <c r="Q6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P7" s="16"/>
       <c r="Q7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2520,7 +2520,7 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
-    <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>271</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="H10" s="4"/>
       <c r="J10" s="31">
-        <v>2.5040770000000001</v>
+        <v>2.5</v>
       </c>
       <c r="K10" s="28">
         <v>2</v>
@@ -2643,7 +2643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="H11" s="4"/>
       <c r="J11" s="31">
-        <v>7.1985114999999995</v>
+        <v>7.2</v>
       </c>
       <c r="K11" s="28">
         <v>4</v>
@@ -2697,8 +2697,9 @@
       <c r="V11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI11" s="28"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -2720,7 +2721,7 @@
       </c>
       <c r="H12" s="4"/>
       <c r="J12" s="31">
-        <v>2.7484425000000003</v>
+        <v>2.75</v>
       </c>
       <c r="K12" s="28">
         <v>4</v>
@@ -2755,8 +2756,9 @@
       <c r="Y12" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI12" s="28"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2778,7 +2780,7 @@
       </c>
       <c r="H13" s="4"/>
       <c r="J13" s="31">
-        <v>1.2529369999999997</v>
+        <v>1.25</v>
       </c>
       <c r="K13" s="4">
         <v>2</v>
@@ -2810,8 +2812,9 @@
       <c r="V13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI13" s="28"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>5</v>
       </c>
@@ -2833,7 +2836,7 @@
       </c>
       <c r="H14" s="4"/>
       <c r="J14" s="31">
-        <v>0.28132499999999999</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K14" s="4">
         <v>2</v>
@@ -2865,8 +2868,9 @@
       <c r="V14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI14" s="28"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2889,7 +2893,7 @@
         <v>40</v>
       </c>
       <c r="J15" s="31">
-        <v>1.0511140000000001</v>
+        <v>1.05</v>
       </c>
       <c r="K15" s="4">
         <v>5</v>
@@ -2921,8 +2925,9 @@
       <c r="V15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI15" s="28"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>7</v>
       </c>
@@ -2944,7 +2949,7 @@
       </c>
       <c r="H16" s="4"/>
       <c r="J16" s="31">
-        <v>1.7461354999999998</v>
+        <v>1.75</v>
       </c>
       <c r="K16" s="12">
         <v>8</v>
@@ -2976,8 +2981,9 @@
       <c r="V16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI16" s="28"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>8</v>
       </c>
@@ -2999,7 +3005,7 @@
       </c>
       <c r="H17" s="4"/>
       <c r="J17" s="31">
-        <v>2.0251964999999998</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="K17" s="12">
         <v>5</v>
@@ -3031,8 +3037,9 @@
       <c r="V17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI17" s="28"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -3052,7 +3059,7 @@
         <v>73</v>
       </c>
       <c r="J18" s="31">
-        <v>9.9100000000000004E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K18" s="4">
         <v>0</v>
@@ -3088,8 +3095,9 @@
       <c r="AC18" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI18" s="28"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -3112,7 +3120,7 @@
         <v>40</v>
       </c>
       <c r="J19" s="31">
-        <v>4.1771409999999998</v>
+        <v>4.18</v>
       </c>
       <c r="K19" s="4">
         <v>6</v>
@@ -3150,8 +3158,9 @@
       <c r="AD19" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI19" s="28"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -3174,7 +3183,7 @@
         <v>40</v>
       </c>
       <c r="J20" s="31">
-        <v>1.0767329999999999</v>
+        <v>1.08</v>
       </c>
       <c r="K20" s="12">
         <v>0</v>
@@ -3212,8 +3221,9 @@
       <c r="AD20" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI20" s="28"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -3236,7 +3246,7 @@
         <v>115</v>
       </c>
       <c r="J21" s="31">
-        <v>1.3563859999999999</v>
+        <v>1.36</v>
       </c>
       <c r="K21" s="12">
         <v>0</v>
@@ -3274,8 +3284,9 @@
       <c r="AD21" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI21" s="28"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -3321,8 +3332,9 @@
       <c r="V22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI22" s="28"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>14</v>
       </c>
@@ -3340,7 +3352,7 @@
       </c>
       <c r="H23" s="4"/>
       <c r="J23" s="31">
-        <v>5.5674774999999999</v>
+        <v>5.57</v>
       </c>
       <c r="K23" s="4">
         <v>0</v>
@@ -3372,8 +3384,9 @@
       <c r="V23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI23" s="28"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>15</v>
       </c>
@@ -3394,7 +3407,7 @@
       </c>
       <c r="H24" s="4"/>
       <c r="J24" s="31">
-        <v>2.7244279999999996</v>
+        <v>2.72</v>
       </c>
       <c r="K24" s="4">
         <v>0</v>
@@ -3426,8 +3439,9 @@
       <c r="V24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI24" s="28"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>16</v>
       </c>
@@ -3449,7 +3463,7 @@
       </c>
       <c r="H25" s="4"/>
       <c r="J25" s="31">
-        <v>3.3249329999999997</v>
+        <v>3.32</v>
       </c>
       <c r="K25" s="4">
         <v>2</v>
@@ -3481,8 +3495,9 @@
       <c r="V25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI25" s="28"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>17</v>
       </c>
@@ -3508,7 +3523,7 @@
         <v>40</v>
       </c>
       <c r="J26" s="31">
-        <v>1.2573460000000001</v>
+        <v>1.26</v>
       </c>
       <c r="K26" s="4">
         <v>2</v>
@@ -3543,8 +3558,9 @@
       <c r="V26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI26" s="28"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>18</v>
       </c>
@@ -3566,7 +3582,7 @@
       </c>
       <c r="H27" s="4"/>
       <c r="J27" s="31">
-        <v>3.9915409999999998</v>
+        <v>3.99</v>
       </c>
       <c r="K27" s="4">
         <v>0</v>
@@ -3598,8 +3614,9 @@
       <c r="V27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI27" s="28"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>19</v>
       </c>
@@ -3621,7 +3638,7 @@
       </c>
       <c r="H28" s="4"/>
       <c r="J28" s="31">
-        <v>1.9001210000000002</v>
+        <v>1.9</v>
       </c>
       <c r="K28" s="4">
         <v>3</v>
@@ -3653,8 +3670,9 @@
       <c r="V28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI28" s="28"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -3677,7 +3695,7 @@
         <v>40</v>
       </c>
       <c r="J29" s="31">
-        <v>0.43381999999999998</v>
+        <v>0.43</v>
       </c>
       <c r="K29" s="4">
         <v>4</v>
@@ -3709,8 +3727,9 @@
       <c r="V29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI29" s="28"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>21</v>
       </c>
@@ -3733,7 +3752,7 @@
         <v>115</v>
       </c>
       <c r="J30" s="31">
-        <v>0.194163</v>
+        <v>0.19</v>
       </c>
       <c r="K30" s="4">
         <v>0</v>
@@ -3765,8 +3784,9 @@
       <c r="V30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI30" s="28"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>22</v>
       </c>
@@ -3788,7 +3808,7 @@
       </c>
       <c r="H31" s="4"/>
       <c r="J31" s="31">
-        <v>0.64731099999999997</v>
+        <v>0.65</v>
       </c>
       <c r="K31" s="4">
         <v>0</v>
@@ -3820,8 +3840,9 @@
       <c r="V31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI31" s="28"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>23</v>
       </c>
@@ -3844,7 +3865,7 @@
         <v>115</v>
       </c>
       <c r="J32" s="31">
-        <v>2.2996899999999996</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K32" s="4">
         <v>6</v>
@@ -3879,8 +3900,9 @@
       <c r="V32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI32" s="28"/>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>24</v>
       </c>
@@ -3900,7 +3922,7 @@
         <v>40</v>
       </c>
       <c r="J33" s="31">
-        <v>0.42677799999999999</v>
+        <v>0.43</v>
       </c>
       <c r="K33" s="4">
         <v>0</v>
@@ -3932,8 +3954,9 @@
       <c r="V33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI33" s="28"/>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -3955,7 +3978,7 @@
       </c>
       <c r="H34" s="4"/>
       <c r="J34" s="31">
-        <v>1.2772359999999998</v>
+        <v>1.28</v>
       </c>
       <c r="K34" s="4">
         <v>0</v>
@@ -3987,8 +4010,9 @@
       <c r="V34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI34" s="28"/>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>26</v>
       </c>
@@ -4012,7 +4036,7 @@
         <v>40</v>
       </c>
       <c r="J35" s="31">
-        <v>1.434102</v>
+        <v>1.43</v>
       </c>
       <c r="K35" s="4">
         <v>0</v>
@@ -4044,8 +4068,9 @@
       <c r="V35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI35" s="28"/>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>27</v>
       </c>
@@ -4067,7 +4092,7 @@
       </c>
       <c r="H36" s="4"/>
       <c r="J36" s="31">
-        <v>2.1870430000000001</v>
+        <v>2.19</v>
       </c>
       <c r="K36" s="4">
         <v>0</v>
@@ -4099,8 +4124,9 @@
       <c r="V36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI36" s="28"/>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>28</v>
       </c>
@@ -4123,7 +4149,7 @@
         <v>40</v>
       </c>
       <c r="J37" s="31">
-        <v>1.0030085000000002</v>
+        <v>1</v>
       </c>
       <c r="K37" s="4">
         <v>5</v>
@@ -4155,8 +4181,9 @@
       <c r="V37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI37" s="28"/>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>29</v>
       </c>
@@ -4178,7 +4205,7 @@
       </c>
       <c r="H38" s="4"/>
       <c r="J38" s="31">
-        <v>2.361138</v>
+        <v>2.36</v>
       </c>
       <c r="K38" s="4">
         <v>4</v>
@@ -4210,8 +4237,9 @@
       <c r="V38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI38" s="28"/>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>30</v>
       </c>
@@ -4237,7 +4265,7 @@
         <v>73</v>
       </c>
       <c r="J39" s="31">
-        <v>0.35058</v>
+        <v>0.35</v>
       </c>
       <c r="K39" s="4">
         <v>0</v>
@@ -4269,8 +4297,9 @@
       <c r="V39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI39" s="28"/>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>31</v>
       </c>
@@ -4291,7 +4320,7 @@
       </c>
       <c r="H40" s="4"/>
       <c r="J40" s="31">
-        <v>0.353379</v>
+        <v>0.35</v>
       </c>
       <c r="K40" s="4">
         <v>0</v>
@@ -4323,8 +4352,9 @@
       <c r="V40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI40" s="28"/>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>32</v>
       </c>
@@ -4350,7 +4380,7 @@
         <v>73</v>
       </c>
       <c r="J41" s="31">
-        <v>2.4777050000000003</v>
+        <v>2.48</v>
       </c>
       <c r="K41" s="4">
         <v>0</v>
@@ -4385,8 +4415,9 @@
       <c r="V41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI41" s="28"/>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>33</v>
       </c>
@@ -4409,7 +4440,7 @@
         <v>17</v>
       </c>
       <c r="J42" s="31">
-        <v>0.53654900000000005</v>
+        <v>0.54</v>
       </c>
       <c r="K42" s="4">
         <v>0</v>
@@ -4441,8 +4472,9 @@
       <c r="V42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI42" s="28"/>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>34</v>
       </c>
@@ -4465,7 +4497,7 @@
         <v>40</v>
       </c>
       <c r="J43" s="31">
-        <v>0.466557</v>
+        <v>0.47</v>
       </c>
       <c r="K43" s="4">
         <v>2</v>
@@ -4497,8 +4529,9 @@
       <c r="V43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI43" s="28"/>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>35</v>
       </c>
@@ -4513,7 +4546,7 @@
       </c>
       <c r="H44" s="4"/>
       <c r="J44" s="31">
-        <v>0.50720299999999996</v>
+        <v>0.51</v>
       </c>
       <c r="K44" s="12" t="s">
         <v>349</v>
@@ -4545,8 +4578,9 @@
       <c r="V44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI44" s="28"/>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>36</v>
       </c>
@@ -4568,7 +4602,7 @@
       </c>
       <c r="H45" s="4"/>
       <c r="J45" s="31">
-        <v>1.4611879999999999</v>
+        <v>1.46</v>
       </c>
       <c r="K45" s="4">
         <v>2</v>
@@ -4600,8 +4634,9 @@
       <c r="V45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI45" s="28"/>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>37</v>
       </c>
@@ -4624,7 +4659,7 @@
         <v>115</v>
       </c>
       <c r="J46" s="31">
-        <v>0.88918099999999989</v>
+        <v>0.89</v>
       </c>
       <c r="K46" s="4">
         <v>5</v>
@@ -4659,8 +4694,9 @@
       <c r="V46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI46" s="28"/>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>38</v>
       </c>
@@ -4678,7 +4714,7 @@
       </c>
       <c r="H47" s="4"/>
       <c r="J47" s="31">
-        <v>1.2545204999999999</v>
+        <v>1.25</v>
       </c>
       <c r="K47" s="4">
         <v>2</v>
@@ -4710,8 +4746,9 @@
       <c r="V47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI47" s="28"/>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>39</v>
       </c>
@@ -4734,7 +4771,7 @@
         <v>115</v>
       </c>
       <c r="J48" s="31">
-        <v>0.289636</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K48" s="4">
         <v>4</v>
@@ -4769,8 +4806,9 @@
       <c r="V48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI48" s="28"/>
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>40</v>
       </c>
@@ -4787,7 +4825,7 @@
         <v>238</v>
       </c>
       <c r="J49" s="31">
-        <v>19.813119</v>
+        <v>19.809999999999999</v>
       </c>
       <c r="K49" s="8">
         <v>0</v>
@@ -4819,8 +4857,9 @@
       <c r="V49" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI49" s="28"/>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>41</v>
       </c>
@@ -4838,7 +4877,7 @@
       </c>
       <c r="H50" s="4"/>
       <c r="J50" s="31">
-        <v>3.8825969999999996</v>
+        <v>3.88</v>
       </c>
       <c r="K50" s="8">
         <v>0</v>
@@ -4870,8 +4909,9 @@
       <c r="V50" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI50" s="28"/>
+    </row>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>42</v>
       </c>
@@ -4883,7 +4923,7 @@
       </c>
       <c r="H51" s="4"/>
       <c r="J51" s="31">
-        <v>2.6757</v>
+        <v>2.68</v>
       </c>
       <c r="K51" s="8">
         <v>0</v>
@@ -4915,8 +4955,9 @@
       <c r="V51" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI51" s="28"/>
+    </row>
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43</v>
       </c>
@@ -4928,7 +4969,7 @@
       </c>
       <c r="H52" s="4"/>
       <c r="J52" s="31">
-        <v>5.3646930000000008</v>
+        <v>5.36</v>
       </c>
       <c r="K52" s="8">
         <v>0</v>
@@ -4960,8 +5001,9 @@
       <c r="V52" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI52" s="28"/>
+    </row>
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>44</v>
       </c>
@@ -4979,7 +5021,7 @@
       </c>
       <c r="H53" s="4"/>
       <c r="J53" s="31">
-        <v>2.953376</v>
+        <v>2.95</v>
       </c>
       <c r="K53" s="4">
         <v>1</v>
@@ -5014,8 +5056,9 @@
       <c r="V53" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI53" s="28"/>
+    </row>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>45</v>
       </c>
@@ -5065,8 +5108,9 @@
       <c r="V54" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI54" s="28"/>
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>46</v>
       </c>
@@ -5084,7 +5128,7 @@
       </c>
       <c r="H55" s="4"/>
       <c r="J55" s="31">
-        <v>7.6104390000000013</v>
+        <v>7.61</v>
       </c>
       <c r="K55" s="4">
         <v>1</v>
@@ -5116,8 +5160,9 @@
       <c r="V55" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI55" s="28"/>
+    </row>
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>47</v>
       </c>
@@ -5135,7 +5180,7 @@
       </c>
       <c r="H56" s="4"/>
       <c r="J56" s="31">
-        <v>2.9312590000000003</v>
+        <v>2.93</v>
       </c>
       <c r="K56" s="4">
         <v>1</v>
@@ -5167,8 +5212,9 @@
       <c r="V56" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI56" s="28"/>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>48</v>
       </c>
@@ -5186,7 +5232,7 @@
       </c>
       <c r="H57" s="4"/>
       <c r="J57" s="31">
-        <v>0.78104649999999998</v>
+        <v>0.78</v>
       </c>
       <c r="K57" s="4">
         <v>0</v>
@@ -5218,8 +5264,9 @@
       <c r="V57" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI57" s="28"/>
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" s="28">
         <v>102</v>
       </c>
@@ -5231,7 +5278,7 @@
       </c>
       <c r="H58" s="4"/>
       <c r="J58" s="31">
-        <v>0.22734399999999999</v>
+        <v>0.23</v>
       </c>
       <c r="K58" s="4">
         <v>1</v>
@@ -5263,8 +5310,9 @@
       <c r="V58" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI58" s="28"/>
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" s="28">
         <v>103</v>
       </c>
@@ -5276,7 +5324,7 @@
       </c>
       <c r="H59" s="4"/>
       <c r="J59" s="31">
-        <v>0.41011600000000004</v>
+        <v>0.41</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -5308,8 +5356,9 @@
       <c r="V59" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI59" s="28"/>
+    </row>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" s="28">
         <v>104</v>
       </c>
@@ -5359,8 +5408,9 @@
       <c r="V60" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI60" s="28"/>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61" s="28">
         <v>105</v>
       </c>
@@ -5378,7 +5428,7 @@
       </c>
       <c r="H61" s="4"/>
       <c r="J61" s="31">
-        <v>6.279827</v>
+        <v>6.28</v>
       </c>
       <c r="K61">
         <v>2</v>
@@ -5410,8 +5460,9 @@
       <c r="V61" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI61" s="28"/>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" s="28">
         <v>106</v>
       </c>
@@ -5423,7 +5474,7 @@
       </c>
       <c r="H62" s="4"/>
       <c r="J62" s="31">
-        <v>5.0626499999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="K62">
         <v>0</v>
@@ -5455,8 +5506,9 @@
       <c r="V62" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI62" s="28"/>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" s="28">
         <v>107</v>
       </c>
@@ -5474,7 +5526,7 @@
       </c>
       <c r="H63" s="4"/>
       <c r="J63" s="31">
-        <v>0.48705300000000001</v>
+        <v>0.49</v>
       </c>
       <c r="K63">
         <v>4</v>
@@ -5506,8 +5558,9 @@
       <c r="V63" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI63" s="28"/>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64" s="28">
         <v>108</v>
       </c>
@@ -5524,7 +5577,7 @@
         <v>290</v>
       </c>
       <c r="J64" s="31">
-        <v>3.2425380000000006</v>
+        <v>3.24</v>
       </c>
       <c r="K64">
         <v>3</v>
@@ -5556,8 +5609,9 @@
       <c r="V64" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI64" s="28"/>
+    </row>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" s="28">
         <v>109</v>
       </c>
@@ -5568,7 +5622,7 @@
         <v>330</v>
       </c>
       <c r="J65" s="31">
-        <v>3.8108604999999995</v>
+        <v>3.81</v>
       </c>
       <c r="K65">
         <v>2</v>
@@ -5600,8 +5654,9 @@
       <c r="V65" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI65" s="28"/>
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" s="28">
         <v>110</v>
       </c>
@@ -5618,7 +5673,7 @@
         <v>290</v>
       </c>
       <c r="J66" s="31">
-        <v>0.68827700000000003</v>
+        <v>0.69</v>
       </c>
       <c r="K66" s="5">
         <v>3</v>
@@ -5650,8 +5705,9 @@
       <c r="V66" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI66" s="28"/>
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" s="28">
         <v>111</v>
       </c>
@@ -5668,7 +5724,7 @@
         <v>290</v>
       </c>
       <c r="J67" s="31">
-        <v>16.185812000000002</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="K67">
         <v>0</v>
@@ -5700,8 +5756,9 @@
       <c r="V67" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI67" s="28"/>
+    </row>
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" s="28">
         <v>112</v>
       </c>
@@ -5718,7 +5775,7 @@
         <v>290</v>
       </c>
       <c r="J68" s="31">
-        <v>3.2503919999999997</v>
+        <v>3.25</v>
       </c>
       <c r="K68" s="5">
         <v>0</v>
@@ -5751,8 +5808,9 @@
       <c r="V68" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI68" s="28"/>
+    </row>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" s="28">
         <v>113</v>
       </c>
@@ -5772,7 +5830,7 @@
       </c>
       <c r="H69" s="4"/>
       <c r="J69" s="31">
-        <v>4.8497159999999999</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="K69" s="8">
         <v>0</v>
@@ -5805,8 +5863,9 @@
       <c r="V69" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI69" s="28"/>
+    </row>
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" s="28">
         <v>115</v>
       </c>
@@ -5827,7 +5886,7 @@
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="J70" s="31">
-        <v>0.29454999999999998</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K70" s="8">
         <v>0</v>
@@ -5860,8 +5919,9 @@
       <c r="V70" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI70" s="28"/>
+    </row>
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71" s="28">
         <v>116</v>
       </c>
@@ -5875,7 +5935,7 @@
       </c>
       <c r="H71" s="4"/>
       <c r="J71" s="31">
-        <v>0.22639400000000001</v>
+        <v>0.23</v>
       </c>
       <c r="K71" s="8">
         <v>0</v>
@@ -5908,8 +5968,9 @@
       <c r="V71" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI71" s="28"/>
+    </row>
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72" s="28">
         <v>117</v>
       </c>
@@ -5923,7 +5984,7 @@
       </c>
       <c r="H72" s="4"/>
       <c r="J72" s="31">
-        <v>0.42425299999999999</v>
+        <v>0.42</v>
       </c>
       <c r="K72" s="8">
         <v>0</v>
@@ -5956,8 +6017,9 @@
       <c r="V72" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI72" s="28"/>
+    </row>
+    <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73" s="28">
         <v>118</v>
       </c>
@@ -5972,7 +6034,7 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="31">
-        <v>4.4136069999999998</v>
+        <v>4.41</v>
       </c>
       <c r="K73" s="8">
         <v>0</v>
@@ -6005,8 +6067,9 @@
       <c r="V73" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI73" s="28"/>
+    </row>
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>119</v>
       </c>
@@ -6027,7 +6090,7 @@
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
       <c r="J74" s="31">
-        <v>2.5748820000000001</v>
+        <v>2.57</v>
       </c>
       <c r="K74" s="8">
         <v>4</v>
@@ -6060,8 +6123,9 @@
       <c r="V74" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI74" s="28"/>
+    </row>
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>120</v>
       </c>
@@ -6082,7 +6146,7 @@
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="J75" s="31">
-        <v>0.367091</v>
+        <v>0.37</v>
       </c>
       <c r="K75" s="8">
         <v>5</v>
@@ -6115,8 +6179,9 @@
       <c r="V75" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="AI75" s="28"/>
+    </row>
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -6130,7 +6195,7 @@
       <c r="T76" s="8"/>
       <c r="U76" s="8"/>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -6144,7 +6209,7 @@
       <c r="T77" s="8"/>
       <c r="U77" s="8"/>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -6158,7 +6223,7 @@
       <c r="T78" s="8"/>
       <c r="U78" s="8"/>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -6170,7 +6235,7 @@
       <c r="T79" s="8"/>
       <c r="U79" s="8"/>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>

</xml_diff>

<commit_message>
Remove non-cmp projects from CMP representative link tab
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -12,16 +12,16 @@
     <sheet name="CMP_Rep_Link" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$64:$O$84</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$V$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$W$75</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="249">
   <si>
     <t>Cost</t>
   </si>
@@ -1479,8 +1479,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2177143" y="0"/>
-          <a:ext cx="10071207" cy="1366683"/>
+          <a:off x="2181225" y="0"/>
+          <a:ext cx="10049436" cy="1366683"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -2097,7 +2097,7 @@
   </sheetPr>
   <dimension ref="A1:AJ97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -6288,7 +6288,7 @@
       <c r="D97" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:V75"/>
+  <autoFilter ref="A9:W75"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I89:I91"/>
   </dataValidations>
@@ -7288,10 +7288,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7392,358 +7392,345 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="8"/>
+        <v>171</v>
+      </c>
+      <c r="C9" s="8">
+        <v>8857</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C10" s="8">
-        <v>8857</v>
+        <v>10577</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C11" s="8">
-        <v>10577</v>
+        <v>4379</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="C12" s="8">
-        <v>4379</v>
+        <v>4089</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
       <c r="C13" s="8">
-        <v>4089</v>
+        <v>10126</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C14" s="8">
-        <v>10126</v>
+        <v>4213</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="C15" s="8">
-        <v>4213</v>
+        <v>10951</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="C16" s="8">
-        <v>10951</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10416</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="C17" s="8">
-        <v>10416</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10952</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="C18" s="8">
-        <v>10952</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10507</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>147</v>
+        <v>53</v>
       </c>
       <c r="C19" s="8">
-        <v>10507</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10428</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="8">
-        <v>10428</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>167</v>
       </c>
       <c r="C21" s="8">
-        <v>11003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10447</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
       <c r="C22" s="8">
-        <v>10447</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8768</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="C23" s="8">
-        <v>8768</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3508</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="C24" s="8">
-        <v>3508</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3737</v>
+      </c>
+      <c r="E24" s="24"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="E25" s="24"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C26" s="8">
-        <v>3737</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3994</v>
+      </c>
+      <c r="E26" s="24"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C27" s="8">
+        <v>10431</v>
+      </c>
+      <c r="E27" s="24"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="C28" s="8">
+        <v>4394</v>
+      </c>
+      <c r="E28" s="24"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E29" s="24"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>109</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E30" s="24"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>110</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="8">
+        <v>5321</v>
+      </c>
+      <c r="E31" s="24"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>111</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="8">
+        <v>8735</v>
+      </c>
+      <c r="E32" s="24"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>112</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C33" s="8">
+        <v>10420</v>
+      </c>
+      <c r="E33" s="24"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>113</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="8">
+        <v>10421</v>
+      </c>
+      <c r="E34" s="24"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>115</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="8">
+        <v>4071</v>
+      </c>
+      <c r="E35" s="24"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>116</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C36" s="8">
+        <v>10456</v>
+      </c>
+      <c r="E36" s="24"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>117</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C37" s="8">
+        <v>10490</v>
+      </c>
+      <c r="E37" s="24"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>120</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C29" s="8">
-        <v>3994</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>106</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="C30" s="8">
-        <v>10431</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>107</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C31" s="8">
-        <v>4394</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>108</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>109</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>110</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C34" s="8">
-        <v>5321</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>111</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C35" s="8">
-        <v>8735</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>112</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C36" s="8">
-        <v>10420</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>113</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C37" s="8">
-        <v>10421</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>115</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>234</v>
-      </c>
       <c r="C38" s="8">
-        <v>4071</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>116</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C39" s="8">
-        <v>10456</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>117</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="C40" s="8">
-        <v>10490</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>120</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C41" s="8">
         <v>9870</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Congested Corridor Identification
If the project is along a congested corridor, assign 1. Otherwise, 0.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="450" windowWidth="18510" windowHeight="12015"/>
+    <workbookView xWindow="4308" yWindow="456" windowWidth="18516" windowHeight="12012" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Proj Attributes and Scenarios" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="250">
   <si>
     <t>Cost</t>
   </si>
@@ -768,6 +768,9 @@
   </si>
   <si>
     <t>10780;4622;10779;2227</t>
+  </si>
+  <si>
+    <t>congested corridor?</t>
   </si>
 </sst>
 </file>
@@ -1479,8 +1482,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2177143" y="0"/>
-          <a:ext cx="10071207" cy="1366683"/>
+          <a:off x="2253343" y="0"/>
+          <a:ext cx="10288922" cy="1328583"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -1675,8 +1678,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1181100" y="0"/>
-          <a:ext cx="10049436" cy="1366683"/>
+          <a:off x="1219200" y="0"/>
+          <a:ext cx="10293276" cy="1313343"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -2097,71 +2100,71 @@
   </sheetPr>
   <dimension ref="A1:AJ97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A69" sqref="A69:XFD69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="7" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="5" customWidth="1"/>
-    <col min="13" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="7" width="32.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" style="5" customWidth="1"/>
+    <col min="13" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="18" customWidth="1"/>
     <col min="17" max="17" width="18" style="5" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="24" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P1" s="16"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P2" s="16"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P3" s="16"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P4" s="16"/>
       <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P5" s="16"/>
       <c r="Q5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P6" s="16"/>
       <c r="Q6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P7" s="16"/>
       <c r="Q7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2194,7 +2197,7 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>176</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -2382,7 +2385,7 @@
       </c>
       <c r="AJ11" s="24"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -2444,7 +2447,7 @@
       </c>
       <c r="AJ12" s="24"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2503,7 +2506,7 @@
       </c>
       <c r="AJ13" s="24"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>5</v>
       </c>
@@ -2562,7 +2565,7 @@
       </c>
       <c r="AJ14" s="24"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2622,7 +2625,7 @@
       </c>
       <c r="AJ15" s="24"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>7</v>
       </c>
@@ -2681,7 +2684,7 @@
       </c>
       <c r="AJ16" s="24"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>8</v>
       </c>
@@ -2740,7 +2743,7 @@
       </c>
       <c r="AJ17" s="24"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -2801,7 +2804,7 @@
       </c>
       <c r="AJ18" s="24"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10</v>
       </c>
@@ -2867,7 +2870,7 @@
       </c>
       <c r="AJ19" s="24"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>11</v>
       </c>
@@ -2933,7 +2936,7 @@
       </c>
       <c r="AJ20" s="24"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -2999,7 +3002,7 @@
       </c>
       <c r="AJ21" s="24"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>13</v>
       </c>
@@ -3050,7 +3053,7 @@
       </c>
       <c r="AJ22" s="24"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>14</v>
       </c>
@@ -3105,7 +3108,7 @@
       </c>
       <c r="AJ23" s="24"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>15</v>
       </c>
@@ -3163,7 +3166,7 @@
       </c>
       <c r="AJ24" s="24"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>16</v>
       </c>
@@ -3222,7 +3225,7 @@
       </c>
       <c r="AJ25" s="24"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>17</v>
       </c>
@@ -3288,7 +3291,7 @@
       </c>
       <c r="AJ26" s="24"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>18</v>
       </c>
@@ -3347,7 +3350,7 @@
       </c>
       <c r="AJ27" s="24"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>19</v>
       </c>
@@ -3406,7 +3409,7 @@
       </c>
       <c r="AJ28" s="24"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
@@ -3466,7 +3469,7 @@
       </c>
       <c r="AJ29" s="24"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>21</v>
       </c>
@@ -3526,7 +3529,7 @@
       </c>
       <c r="AJ30" s="24"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>22</v>
       </c>
@@ -3585,7 +3588,7 @@
       </c>
       <c r="AJ31" s="24"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>23</v>
       </c>
@@ -3648,7 +3651,7 @@
       </c>
       <c r="AJ32" s="24"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>24</v>
       </c>
@@ -3705,7 +3708,7 @@
       </c>
       <c r="AJ33" s="24"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -3764,7 +3767,7 @@
       </c>
       <c r="AJ34" s="24"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>26</v>
       </c>
@@ -3825,7 +3828,7 @@
       </c>
       <c r="AJ35" s="24"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>27</v>
       </c>
@@ -3884,7 +3887,7 @@
       </c>
       <c r="AJ36" s="24"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>28</v>
       </c>
@@ -3944,7 +3947,7 @@
       </c>
       <c r="AJ37" s="24"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>29</v>
       </c>
@@ -4003,7 +4006,7 @@
       </c>
       <c r="AJ38" s="24"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>30</v>
       </c>
@@ -4066,7 +4069,7 @@
       </c>
       <c r="AJ39" s="24"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>31</v>
       </c>
@@ -4124,7 +4127,7 @@
       </c>
       <c r="AJ40" s="24"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>32</v>
       </c>
@@ -4190,7 +4193,7 @@
       </c>
       <c r="AJ41" s="24"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>33</v>
       </c>
@@ -4250,7 +4253,7 @@
       </c>
       <c r="AJ42" s="24"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>34</v>
       </c>
@@ -4310,7 +4313,7 @@
       </c>
       <c r="AJ43" s="24"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>35</v>
       </c>
@@ -4362,7 +4365,7 @@
       </c>
       <c r="AJ44" s="24"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>36</v>
       </c>
@@ -4421,7 +4424,7 @@
       </c>
       <c r="AJ45" s="24"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>37</v>
       </c>
@@ -4484,7 +4487,7 @@
       </c>
       <c r="AJ46" s="24"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>38</v>
       </c>
@@ -4539,7 +4542,7 @@
       </c>
       <c r="AJ47" s="24"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>39</v>
       </c>
@@ -4602,7 +4605,7 @@
       </c>
       <c r="AJ48" s="24"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>40</v>
       </c>
@@ -4656,7 +4659,7 @@
       </c>
       <c r="AJ49" s="24"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>41</v>
       </c>
@@ -4711,7 +4714,7 @@
       </c>
       <c r="AJ50" s="24"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>42</v>
       </c>
@@ -4760,7 +4763,7 @@
       </c>
       <c r="AJ51" s="24"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>43</v>
       </c>
@@ -4809,7 +4812,7 @@
       </c>
       <c r="AJ52" s="24"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>44</v>
       </c>
@@ -4867,7 +4870,7 @@
       </c>
       <c r="AJ53" s="24"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>45</v>
       </c>
@@ -4922,7 +4925,7 @@
       </c>
       <c r="AJ54" s="24"/>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>46</v>
       </c>
@@ -4977,7 +4980,7 @@
       </c>
       <c r="AJ55" s="24"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>47</v>
       </c>
@@ -5032,7 +5035,7 @@
       </c>
       <c r="AJ56" s="24"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>48</v>
       </c>
@@ -5087,7 +5090,7 @@
       </c>
       <c r="AJ57" s="24"/>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A58" s="24">
         <v>102</v>
       </c>
@@ -5136,7 +5139,7 @@
       </c>
       <c r="AJ58" s="24"/>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A59" s="24">
         <v>103</v>
       </c>
@@ -5185,7 +5188,7 @@
       </c>
       <c r="AJ59" s="24"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A60" s="24">
         <v>104</v>
       </c>
@@ -5240,7 +5243,7 @@
       </c>
       <c r="AJ60" s="24"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A61" s="24">
         <v>105</v>
       </c>
@@ -5295,7 +5298,7 @@
       </c>
       <c r="AJ61" s="24"/>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A62" s="24">
         <v>106</v>
       </c>
@@ -5344,7 +5347,7 @@
       </c>
       <c r="AJ62" s="24"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A63" s="24">
         <v>107</v>
       </c>
@@ -5399,7 +5402,7 @@
       </c>
       <c r="AJ63" s="24"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A64" s="24">
         <v>108</v>
       </c>
@@ -5453,7 +5456,7 @@
       </c>
       <c r="AJ64" s="24"/>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A65" s="24">
         <v>109</v>
       </c>
@@ -5501,7 +5504,7 @@
       </c>
       <c r="AJ65" s="24"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A66" s="24">
         <v>110</v>
       </c>
@@ -5555,7 +5558,7 @@
       </c>
       <c r="AJ66" s="24"/>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A67" s="24">
         <v>111</v>
       </c>
@@ -5609,7 +5612,7 @@
       </c>
       <c r="AJ67" s="24"/>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A68" s="24">
         <v>112</v>
       </c>
@@ -5664,7 +5667,7 @@
       </c>
       <c r="AJ68" s="24"/>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A69" s="24">
         <v>113</v>
       </c>
@@ -5722,7 +5725,7 @@
       </c>
       <c r="AJ69" s="24"/>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A70" s="24">
         <v>115</v>
       </c>
@@ -5781,7 +5784,7 @@
       </c>
       <c r="AJ70" s="24"/>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A71" s="24">
         <v>116</v>
       </c>
@@ -5833,7 +5836,7 @@
       </c>
       <c r="AJ71" s="24"/>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A72" s="24">
         <v>117</v>
       </c>
@@ -5885,7 +5888,7 @@
       </c>
       <c r="AJ72" s="24"/>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A73" s="24">
         <v>118</v>
       </c>
@@ -5938,7 +5941,7 @@
       </c>
       <c r="AJ73" s="24"/>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>119</v>
       </c>
@@ -5997,7 +6000,7 @@
       </c>
       <c r="AJ74" s="24"/>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>120</v>
       </c>
@@ -6056,7 +6059,7 @@
       </c>
       <c r="AJ75" s="24"/>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -6071,7 +6074,7 @@
       <c r="U76" s="8"/>
       <c r="W76" s="8"/>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -6086,7 +6089,7 @@
       <c r="U77" s="8"/>
       <c r="W77" s="8"/>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -6101,7 +6104,7 @@
       <c r="U78" s="8"/>
       <c r="W78" s="8"/>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -6114,7 +6117,7 @@
       <c r="U79" s="8"/>
       <c r="W79" s="8"/>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -6127,7 +6130,7 @@
       <c r="U80" s="8"/>
       <c r="W80" s="8"/>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -6140,7 +6143,7 @@
       <c r="U81" s="8"/>
       <c r="W81" s="8"/>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -6153,7 +6156,7 @@
       <c r="U82" s="8"/>
       <c r="W82" s="8"/>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -6166,7 +6169,7 @@
       <c r="U83" s="8"/>
       <c r="W83" s="8"/>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -6179,7 +6182,7 @@
       <c r="U84" s="8"/>
       <c r="W84" s="8"/>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -6192,7 +6195,7 @@
       <c r="U85" s="8"/>
       <c r="W85" s="8"/>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -6206,7 +6209,7 @@
       <c r="U86" s="8"/>
       <c r="W86" s="8"/>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -6220,7 +6223,7 @@
       <c r="U87" s="8"/>
       <c r="W87" s="8"/>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -6236,7 +6239,7 @@
       <c r="U88" s="8"/>
       <c r="W88" s="8"/>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -6251,7 +6254,7 @@
       <c r="U89" s="8"/>
       <c r="W89" s="8"/>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -6266,22 +6269,22 @@
       <c r="U90" s="8"/>
       <c r="W90" s="8"/>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J94" s="5"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -6312,27 +6315,27 @@
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="6" width="32.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="6" width="32.5546875" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6357,7 +6360,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -6404,7 +6407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>38</v>
@@ -6424,7 +6427,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>45</v>
@@ -6447,7 +6450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>49</v>
@@ -6470,7 +6473,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -6494,7 +6497,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -6517,7 +6520,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -6541,7 +6544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>63</v>
@@ -6561,7 +6564,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>69</v>
@@ -6581,7 +6584,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C18" s="4" t="s">
         <v>91</v>
       </c>
@@ -6604,7 +6607,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C19" s="4" t="s">
         <v>97</v>
       </c>
@@ -6627,7 +6630,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>104</v>
       </c>
@@ -6643,7 +6646,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C21" s="4" t="s">
         <v>99</v>
       </c>
@@ -6654,7 +6657,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C22" s="4" t="s">
         <v>111</v>
       </c>
@@ -6665,7 +6668,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">
         <v>27</v>
       </c>
@@ -6686,7 +6689,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="4" t="s">
         <v>35</v>
       </c>
@@ -6705,7 +6708,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>19</v>
       </c>
@@ -6729,7 +6732,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -6739,7 +6742,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -6749,7 +6752,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>176</v>
       </c>
@@ -6817,7 +6820,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24">
         <v>114</v>
       </c>
@@ -6851,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="24">
         <v>101</v>
       </c>
@@ -6891,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -6901,7 +6904,7 @@
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -6911,7 +6914,7 @@
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -6921,7 +6924,7 @@
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -6931,7 +6934,7 @@
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -6941,7 +6944,7 @@
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -6951,7 +6954,7 @@
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -6961,7 +6964,7 @@
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -6971,7 +6974,7 @@
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -6981,7 +6984,7 @@
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -6991,7 +6994,7 @@
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -7001,129 +7004,129 @@
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G42" s="4"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G43" s="4"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G44" s="4"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G45" s="4"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G46" s="4"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G47" s="4"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G48" s="4"/>
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G49" s="4"/>
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G50" s="4"/>
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G51" s="4"/>
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G52" s="4"/>
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G53" s="4"/>
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G54" s="4"/>
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G55" s="4"/>
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G56" s="4"/>
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G57" s="4"/>
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G58" s="4"/>
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J62"/>
       <c r="K62"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J63"/>
       <c r="K63"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="G64" s="4"/>
       <c r="O64" s="4"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="O65" s="4"/>
     </row>
-    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="J66" s="8"/>
       <c r="K66" s="5"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="F67" s="4"/>
@@ -7131,119 +7134,119 @@
       <c r="I67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="G68" s="4"/>
       <c r="I68" s="4"/>
       <c r="O68" s="4"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="O70" s="4"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="O71" s="4"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="O72" s="4"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="O73" s="4"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="O74" s="4"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="G75" s="4"/>
       <c r="O75" s="4"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="G76" s="4"/>
       <c r="O76" s="4"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="G77" s="4"/>
       <c r="O77" s="4"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="G78" s="4"/>
       <c r="O78" s="4"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="G79" s="4"/>
       <c r="O79" s="4"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="G80" s="4"/>
       <c r="O80" s="4"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="G81" s="4"/>
       <c r="O81" s="4"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="O82" s="4"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="G83" s="4"/>
       <c r="O83" s="4"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="G84" s="4"/>
       <c r="O84" s="4"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="G85" s="4"/>
@@ -7252,7 +7255,7 @@
       <c r="K85" s="8"/>
       <c r="O85" s="4"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="G86" s="4"/>
@@ -7261,7 +7264,7 @@
       <c r="K86" s="8"/>
       <c r="O86" s="4"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="G87" s="4"/>
@@ -7270,7 +7273,7 @@
       <c r="K87" s="8"/>
       <c r="O87" s="4"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -7288,21 +7291,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="15.6640625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>176</v>
       </c>
@@ -7312,8 +7315,11 @@
       <c r="C1" s="28" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="28" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -7323,8 +7329,11 @@
       <c r="C2" s="8">
         <v>10140</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -7334,8 +7343,11 @@
       <c r="C3" s="8" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -7345,8 +7357,11 @@
       <c r="C4" s="8">
         <v>3838</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -7356,8 +7371,11 @@
       <c r="C5" s="8">
         <v>10452</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -7367,8 +7385,11 @@
       <c r="C6" s="8">
         <v>10109</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>7</v>
       </c>
@@ -7378,8 +7399,11 @@
       <c r="C7" s="8" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>8</v>
       </c>
@@ -7389,8 +7413,11 @@
       <c r="C8" s="8">
         <v>7456</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>13</v>
       </c>
@@ -7399,7 +7426,7 @@
       </c>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>14</v>
       </c>
@@ -7409,8 +7436,11 @@
       <c r="C10" s="8">
         <v>8857</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>15</v>
       </c>
@@ -7420,8 +7450,11 @@
       <c r="C11" s="8">
         <v>10577</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>16</v>
       </c>
@@ -7431,8 +7464,11 @@
       <c r="C12" s="8">
         <v>4379</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>17</v>
       </c>
@@ -7442,8 +7478,11 @@
       <c r="C13" s="8">
         <v>4089</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>18</v>
       </c>
@@ -7453,8 +7492,11 @@
       <c r="C14" s="8">
         <v>10126</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>19</v>
       </c>
@@ -7464,8 +7506,11 @@
       <c r="C15" s="8">
         <v>4213</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>22</v>
       </c>
@@ -7475,8 +7520,11 @@
       <c r="C16" s="8">
         <v>10951</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>25</v>
       </c>
@@ -7486,8 +7534,11 @@
       <c r="C17" s="8">
         <v>10416</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>27</v>
       </c>
@@ -7497,8 +7548,11 @@
       <c r="C18" s="8">
         <v>10952</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>29</v>
       </c>
@@ -7508,8 +7562,11 @@
       <c r="C19" s="8">
         <v>10507</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>30</v>
       </c>
@@ -7519,8 +7576,11 @@
       <c r="C20" s="8">
         <v>10428</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>31</v>
       </c>
@@ -7530,8 +7590,11 @@
       <c r="C21" s="8">
         <v>11003</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>32</v>
       </c>
@@ -7541,8 +7604,11 @@
       <c r="C22" s="8">
         <v>10447</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>33</v>
       </c>
@@ -7552,8 +7618,11 @@
       <c r="C23" s="8">
         <v>8768</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>36</v>
       </c>
@@ -7563,8 +7632,11 @@
       <c r="C24" s="8">
         <v>3508</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>38</v>
       </c>
@@ -7572,8 +7644,11 @@
         <v>156</v>
       </c>
       <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>102</v>
       </c>
@@ -7583,8 +7658,11 @@
       <c r="C26" s="8">
         <v>3737</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>103</v>
       </c>
@@ -7592,8 +7670,11 @@
         <v>210</v>
       </c>
       <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>104</v>
       </c>
@@ -7603,8 +7684,11 @@
       <c r="C28" s="8" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>105</v>
       </c>
@@ -7614,8 +7698,11 @@
       <c r="C29" s="8">
         <v>3994</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>106</v>
       </c>
@@ -7625,8 +7712,11 @@
       <c r="C30" s="8">
         <v>10431</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>107</v>
       </c>
@@ -7636,8 +7726,11 @@
       <c r="C31" s="8">
         <v>4394</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>108</v>
       </c>
@@ -7647,8 +7740,11 @@
       <c r="C32" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>109</v>
       </c>
@@ -7658,8 +7754,11 @@
       <c r="C33" s="8" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>110</v>
       </c>
@@ -7669,8 +7768,11 @@
       <c r="C34" s="8">
         <v>5321</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>111</v>
       </c>
@@ -7680,8 +7782,11 @@
       <c r="C35" s="8">
         <v>8735</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>112</v>
       </c>
@@ -7691,8 +7796,11 @@
       <c r="C36" s="8">
         <v>10420</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>113</v>
       </c>
@@ -7702,8 +7810,11 @@
       <c r="C37" s="8">
         <v>10421</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>115</v>
       </c>
@@ -7713,8 +7824,11 @@
       <c r="C38" s="8">
         <v>4071</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>116</v>
       </c>
@@ -7724,8 +7838,11 @@
       <c r="C39" s="8">
         <v>10456</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>117</v>
       </c>
@@ -7735,8 +7852,11 @@
       <c r="C40" s="8">
         <v>10490</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>120</v>
       </c>
@@ -7745,6 +7865,9 @@
       </c>
       <c r="C41" s="8">
         <v>9870</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CMP project scores
Now includes the congested roadway score
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4308" yWindow="456" windowWidth="18516" windowHeight="12012" activeTab="2"/>
+    <workbookView xWindow="4305" yWindow="450" windowWidth="18510" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="Proj Attributes and Scenarios" sheetId="1" r:id="rId1"/>
@@ -1482,8 +1482,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2244436" y="0"/>
-          <a:ext cx="10284964" cy="1293947"/>
+          <a:off x="2182091" y="0"/>
+          <a:ext cx="10021727" cy="1366683"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -2100,71 +2100,71 @@
   </sheetPr>
   <dimension ref="A1:AJ97"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="7" width="32.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" style="5" customWidth="1"/>
-    <col min="13" max="15" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" style="18" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="7" width="32.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="5" customWidth="1"/>
+    <col min="13" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
     <col min="17" max="17" width="18" style="5" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="24" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P1" s="16"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P2" s="16"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P3" s="16"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P4" s="16"/>
       <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P5" s="16"/>
       <c r="Q5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P6" s="16"/>
       <c r="Q6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="P7" s="16"/>
       <c r="Q7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2197,7 +2197,7 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>176</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="AJ11" s="24"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -2447,7 +2447,7 @@
       </c>
       <c r="AJ12" s="24"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
       <c r="AJ13" s="24"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>5</v>
       </c>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="AJ14" s="24"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="AJ15" s="24"/>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>7</v>
       </c>
@@ -2684,7 +2684,7 @@
       </c>
       <c r="AJ16" s="24"/>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>8</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="AJ17" s="24"/>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="AJ18" s="24"/>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -2870,7 +2870,7 @@
       </c>
       <c r="AJ19" s="24"/>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="AJ20" s="24"/>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="AJ21" s="24"/>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="AJ22" s="24"/>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>14</v>
       </c>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="AJ23" s="24"/>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>15</v>
       </c>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="AJ24" s="24"/>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>16</v>
       </c>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="AJ25" s="24"/>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>17</v>
       </c>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="AJ26" s="24"/>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>18</v>
       </c>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="AJ27" s="24"/>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>19</v>
       </c>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="AJ28" s="24"/>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20</v>
       </c>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="AJ29" s="24"/>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>21</v>
       </c>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="AJ30" s="24"/>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>22</v>
       </c>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="AJ31" s="24"/>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>23</v>
       </c>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="AJ32" s="24"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>24</v>
       </c>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="AJ33" s="24"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="AJ34" s="24"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>26</v>
       </c>
@@ -3828,7 +3828,7 @@
       </c>
       <c r="AJ35" s="24"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>27</v>
       </c>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="AJ36" s="24"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>28</v>
       </c>
@@ -3947,7 +3947,7 @@
       </c>
       <c r="AJ37" s="24"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>29</v>
       </c>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="AJ38" s="24"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>30</v>
       </c>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="AJ39" s="24"/>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>31</v>
       </c>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="AJ40" s="24"/>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>32</v>
       </c>
@@ -4193,7 +4193,7 @@
       </c>
       <c r="AJ41" s="24"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>33</v>
       </c>
@@ -4253,7 +4253,7 @@
       </c>
       <c r="AJ42" s="24"/>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>34</v>
       </c>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="AJ43" s="24"/>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>35</v>
       </c>
@@ -4365,7 +4365,7 @@
       </c>
       <c r="AJ44" s="24"/>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>36</v>
       </c>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="AJ45" s="24"/>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>37</v>
       </c>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="AJ46" s="24"/>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>38</v>
       </c>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="AJ47" s="24"/>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>39</v>
       </c>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="AJ48" s="24"/>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>40</v>
       </c>
@@ -4659,7 +4659,7 @@
       </c>
       <c r="AJ49" s="24"/>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>41</v>
       </c>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="AJ50" s="24"/>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>42</v>
       </c>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="AJ51" s="24"/>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43</v>
       </c>
@@ -4812,7 +4812,7 @@
       </c>
       <c r="AJ52" s="24"/>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>44</v>
       </c>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="AJ53" s="24"/>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>45</v>
       </c>
@@ -4925,7 +4925,7 @@
       </c>
       <c r="AJ54" s="24"/>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>46</v>
       </c>
@@ -4980,7 +4980,7 @@
       </c>
       <c r="AJ55" s="24"/>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>47</v>
       </c>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="AJ56" s="24"/>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>48</v>
       </c>
@@ -5090,7 +5090,7 @@
       </c>
       <c r="AJ57" s="24"/>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="24">
         <v>102</v>
       </c>
@@ -5139,7 +5139,7 @@
       </c>
       <c r="AJ58" s="24"/>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="24">
         <v>103</v>
       </c>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="AJ59" s="24"/>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="24">
         <v>104</v>
       </c>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="AJ60" s="24"/>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="24">
         <v>105</v>
       </c>
@@ -5298,7 +5298,7 @@
       </c>
       <c r="AJ61" s="24"/>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <v>106</v>
       </c>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="AJ62" s="24"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="24">
         <v>107</v>
       </c>
@@ -5402,7 +5402,7 @@
       </c>
       <c r="AJ63" s="24"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="24">
         <v>108</v>
       </c>
@@ -5456,7 +5456,7 @@
       </c>
       <c r="AJ64" s="24"/>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="24">
         <v>109</v>
       </c>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="AJ65" s="24"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="24">
         <v>110</v>
       </c>
@@ -5558,7 +5558,7 @@
       </c>
       <c r="AJ66" s="24"/>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="24">
         <v>111</v>
       </c>
@@ -5612,7 +5612,7 @@
       </c>
       <c r="AJ67" s="24"/>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="24">
         <v>112</v>
       </c>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="AJ68" s="24"/>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="24">
         <v>113</v>
       </c>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="AJ69" s="24"/>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="24">
         <v>115</v>
       </c>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="AJ70" s="24"/>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="24">
         <v>116</v>
       </c>
@@ -5836,7 +5836,7 @@
       </c>
       <c r="AJ71" s="24"/>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="24">
         <v>117</v>
       </c>
@@ -5888,7 +5888,7 @@
       </c>
       <c r="AJ72" s="24"/>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="24">
         <v>118</v>
       </c>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="AJ73" s="24"/>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>119</v>
       </c>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="AJ74" s="24"/>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>120</v>
       </c>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="AJ75" s="24"/>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -6074,7 +6074,7 @@
       <c r="U76" s="8"/>
       <c r="W76" s="8"/>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -6089,7 +6089,7 @@
       <c r="U77" s="8"/>
       <c r="W77" s="8"/>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -6104,7 +6104,7 @@
       <c r="U78" s="8"/>
       <c r="W78" s="8"/>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -6117,7 +6117,7 @@
       <c r="U79" s="8"/>
       <c r="W79" s="8"/>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -6130,7 +6130,7 @@
       <c r="U80" s="8"/>
       <c r="W80" s="8"/>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -6143,7 +6143,7 @@
       <c r="U81" s="8"/>
       <c r="W81" s="8"/>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -6156,7 +6156,7 @@
       <c r="U82" s="8"/>
       <c r="W82" s="8"/>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -6169,7 +6169,7 @@
       <c r="U83" s="8"/>
       <c r="W83" s="8"/>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -6182,7 +6182,7 @@
       <c r="U84" s="8"/>
       <c r="W84" s="8"/>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -6195,7 +6195,7 @@
       <c r="U85" s="8"/>
       <c r="W85" s="8"/>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -6209,7 +6209,7 @@
       <c r="U86" s="8"/>
       <c r="W86" s="8"/>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -6223,7 +6223,7 @@
       <c r="U87" s="8"/>
       <c r="W87" s="8"/>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -6239,7 +6239,7 @@
       <c r="U88" s="8"/>
       <c r="W88" s="8"/>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -6254,7 +6254,7 @@
       <c r="U89" s="8"/>
       <c r="W89" s="8"/>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -6269,22 +6269,22 @@
       <c r="U90" s="8"/>
       <c r="W90" s="8"/>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="J94" s="5"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -6315,27 +6315,27 @@
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="6" width="32.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="6" width="32.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6360,7 +6360,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -6407,7 +6407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>38</v>
@@ -6427,7 +6427,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>45</v>
@@ -6450,7 +6450,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>49</v>
@@ -6473,7 +6473,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -6497,7 +6497,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -6520,7 +6520,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -6544,7 +6544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>63</v>
@@ -6564,7 +6564,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>69</v>
@@ -6584,7 +6584,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>91</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
         <v>97</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>104</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>99</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>111</v>
       </c>
@@ -6668,7 +6668,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>27</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>35</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>19</v>
       </c>
@@ -6732,7 +6732,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -6742,7 +6742,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -6752,7 +6752,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>176</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24">
         <v>114</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="24">
         <v>101</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -6904,7 +6904,7 @@
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -6914,7 +6914,7 @@
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -6924,7 +6924,7 @@
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -6934,7 +6934,7 @@
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -6944,7 +6944,7 @@
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -6954,7 +6954,7 @@
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -6964,7 +6964,7 @@
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -6974,7 +6974,7 @@
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -6984,7 +6984,7 @@
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -6994,7 +6994,7 @@
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -7004,129 +7004,129 @@
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G42" s="4"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G43" s="4"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G44" s="4"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G45" s="4"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G46" s="4"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G47" s="4"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G48" s="4"/>
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G49" s="4"/>
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G50" s="4"/>
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G51" s="4"/>
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G52" s="4"/>
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G53" s="4"/>
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G54" s="4"/>
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G55" s="4"/>
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G56" s="4"/>
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G57" s="4"/>
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G58" s="4"/>
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J62"/>
       <c r="K62"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J63"/>
       <c r="K63"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="G64" s="4"/>
       <c r="O64" s="4"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="O65" s="4"/>
     </row>
-    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="J66" s="8"/>
       <c r="K66" s="5"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="F67" s="4"/>
@@ -7134,119 +7134,119 @@
       <c r="I67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="G68" s="4"/>
       <c r="I68" s="4"/>
       <c r="O68" s="4"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="O70" s="4"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="O71" s="4"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="O72" s="4"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="O73" s="4"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="O74" s="4"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="G75" s="4"/>
       <c r="O75" s="4"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="G76" s="4"/>
       <c r="O76" s="4"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="G77" s="4"/>
       <c r="O77" s="4"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="G78" s="4"/>
       <c r="O78" s="4"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="G79" s="4"/>
       <c r="O79" s="4"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="G80" s="4"/>
       <c r="O80" s="4"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="G81" s="4"/>
       <c r="O81" s="4"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="O82" s="4"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="G83" s="4"/>
       <c r="O83" s="4"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="G84" s="4"/>
       <c r="O84" s="4"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="G85" s="4"/>
@@ -7255,7 +7255,7 @@
       <c r="K85" s="8"/>
       <c r="O85" s="4"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="G86" s="4"/>
@@ -7264,7 +7264,7 @@
       <c r="K86" s="8"/>
       <c r="O86" s="4"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="G87" s="4"/>
@@ -7273,7 +7273,7 @@
       <c r="K87" s="8"/>
       <c r="O87" s="4"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -7291,21 +7291,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="4"/>
+    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>176</v>
       </c>
@@ -7315,11 +7315,11 @@
       <c r="C1" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -7329,11 +7329,11 @@
       <c r="C2" s="8">
         <v>10140</v>
       </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -7343,11 +7343,11 @@
       <c r="C3" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -7357,11 +7357,11 @@
       <c r="C4" s="8">
         <v>3838</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -7371,11 +7371,11 @@
       <c r="C5" s="8">
         <v>10452</v>
       </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -7385,11 +7385,11 @@
       <c r="C6" s="8">
         <v>10109</v>
       </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>7</v>
       </c>
@@ -7399,11 +7399,11 @@
       <c r="C7" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>8</v>
       </c>
@@ -7413,11 +7413,11 @@
       <c r="C8" s="8">
         <v>7456</v>
       </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>14</v>
       </c>
@@ -7427,11 +7427,11 @@
       <c r="C9" s="8">
         <v>8857</v>
       </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>15</v>
       </c>
@@ -7441,11 +7441,11 @@
       <c r="C10" s="8">
         <v>10577</v>
       </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>16</v>
       </c>
@@ -7455,11 +7455,11 @@
       <c r="C11" s="8">
         <v>4379</v>
       </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>17</v>
       </c>
@@ -7469,11 +7469,11 @@
       <c r="C12" s="8">
         <v>4089</v>
       </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>18</v>
       </c>
@@ -7483,11 +7483,11 @@
       <c r="C13" s="8">
         <v>10126</v>
       </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>19</v>
       </c>
@@ -7497,11 +7497,11 @@
       <c r="C14" s="8">
         <v>4213</v>
       </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>22</v>
       </c>
@@ -7511,11 +7511,11 @@
       <c r="C15" s="8">
         <v>10951</v>
       </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>25</v>
       </c>
@@ -7525,11 +7525,11 @@
       <c r="C16" s="8">
         <v>10416</v>
       </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>27</v>
       </c>
@@ -7539,11 +7539,11 @@
       <c r="C17" s="8">
         <v>10952</v>
       </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>29</v>
       </c>
@@ -7553,11 +7553,11 @@
       <c r="C18" s="8">
         <v>10507</v>
       </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>30</v>
       </c>
@@ -7567,11 +7567,11 @@
       <c r="C19" s="8">
         <v>10428</v>
       </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>31</v>
       </c>
@@ -7581,11 +7581,11 @@
       <c r="C20" s="8">
         <v>11003</v>
       </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>32</v>
       </c>
@@ -7595,11 +7595,11 @@
       <c r="C21" s="8">
         <v>10447</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>33</v>
       </c>
@@ -7609,11 +7609,11 @@
       <c r="C22" s="8">
         <v>8768</v>
       </c>
-      <c r="E22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>36</v>
       </c>
@@ -7623,11 +7623,11 @@
       <c r="C23" s="8">
         <v>3508</v>
       </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>102</v>
       </c>
@@ -7637,11 +7637,11 @@
       <c r="C24" s="8">
         <v>3737</v>
       </c>
-      <c r="E24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>104</v>
       </c>
@@ -7651,11 +7651,11 @@
       <c r="C25" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="E25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>105</v>
       </c>
@@ -7665,11 +7665,11 @@
       <c r="C26" s="8">
         <v>3994</v>
       </c>
-      <c r="E26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>106</v>
       </c>
@@ -7679,11 +7679,11 @@
       <c r="C27" s="8">
         <v>10431</v>
       </c>
-      <c r="E27" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>107</v>
       </c>
@@ -7693,11 +7693,11 @@
       <c r="C28" s="8">
         <v>4394</v>
       </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>108</v>
       </c>
@@ -7707,11 +7707,11 @@
       <c r="C29" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>109</v>
       </c>
@@ -7721,11 +7721,11 @@
       <c r="C30" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="E30" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>110</v>
       </c>
@@ -7735,11 +7735,11 @@
       <c r="C31" s="8">
         <v>5321</v>
       </c>
-      <c r="E31" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>111</v>
       </c>
@@ -7749,11 +7749,11 @@
       <c r="C32" s="8">
         <v>8735</v>
       </c>
-      <c r="E32" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>112</v>
       </c>
@@ -7763,11 +7763,11 @@
       <c r="C33" s="8">
         <v>10420</v>
       </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>113</v>
       </c>
@@ -7777,11 +7777,11 @@
       <c r="C34" s="8">
         <v>10421</v>
       </c>
-      <c r="E34" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>115</v>
       </c>
@@ -7791,11 +7791,11 @@
       <c r="C35" s="8">
         <v>4071</v>
       </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>116</v>
       </c>
@@ -7805,11 +7805,11 @@
       <c r="C36" s="8">
         <v>10456</v>
       </c>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>117</v>
       </c>
@@ -7819,11 +7819,11 @@
       <c r="C37" s="8">
         <v>10490</v>
       </c>
-      <c r="E37" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>120</v>
       </c>
@@ -7833,7 +7833,7 @@
       <c r="C38" s="8">
         <v>9870</v>
       </c>
-      <c r="E38" s="4">
+      <c r="D38" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change proj 5 description from new location to widening
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="249">
   <si>
     <t>Cost</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>4. Paste the "ProjID" field into the "ProjectList.csv" included in the model scenario's "Inputs" folder</t>
-  </si>
-  <si>
-    <t>New Capacity</t>
   </si>
   <si>
     <t>Widening</t>
@@ -2104,7 +2101,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,28 +2196,28 @@
     </row>
     <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>0</v>
@@ -2229,43 +2226,43 @@
         <v>1</v>
       </c>
       <c r="K9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="O9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P9" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="P9" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="Q9" s="15" t="s">
         <v>2</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S9" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T9" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="U9" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="V9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -2277,16 +2274,16 @@
         <v>205</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="4"/>
       <c r="J10" s="27">
@@ -2335,16 +2332,16 @@
         <v>351</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="4"/>
       <c r="J11" s="27">
@@ -2394,16 +2391,16 @@
         <v>356</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" s="4"/>
       <c r="J12" s="27">
@@ -2443,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="Z12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AJ12" s="24"/>
     </row>
@@ -2456,16 +2453,16 @@
         <v>251</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H13" s="4"/>
       <c r="J13" s="27">
@@ -2515,16 +2512,16 @@
         <v>353</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>149</v>
+        <v>8</v>
       </c>
       <c r="H14" s="4"/>
       <c r="J14" s="27">
@@ -2573,19 +2570,19 @@
         <v>853</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
         <v>29</v>
       </c>
-      <c r="G15" t="s">
-        <v>30</v>
-      </c>
       <c r="H15" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J15" s="27">
         <v>1.05</v>
@@ -2634,16 +2631,16 @@
         <v>306</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" t="s">
         <v>150</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>151</v>
-      </c>
-      <c r="G16" t="s">
-        <v>152</v>
       </c>
       <c r="H16" s="4"/>
       <c r="J16" s="27">
@@ -2693,16 +2690,16 @@
         <v>208</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H17" s="4"/>
       <c r="J17" s="27">
@@ -2748,19 +2745,19 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18">
         <v>854</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J18" s="27">
         <v>0.01</v>
@@ -2800,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="AD18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AJ18" s="24"/>
     </row>
@@ -2812,19 +2809,19 @@
         <v>855</v>
       </c>
       <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
       <c r="G19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J19" s="27">
         <v>4.18</v>
@@ -2866,7 +2863,7 @@
         <v>2012</v>
       </c>
       <c r="AE19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AJ19" s="24"/>
     </row>
@@ -2878,19 +2875,19 @@
         <v>856</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J20" s="27">
         <v>1.08</v>
@@ -2932,7 +2929,7 @@
         <v>2020</v>
       </c>
       <c r="AE20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AJ20" s="24"/>
     </row>
@@ -2944,19 +2941,19 @@
         <v>802</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F21" t="s">
-        <v>117</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>119</v>
-      </c>
       <c r="H21" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J21" s="27">
         <v>1.36</v>
@@ -2998,7 +2995,7 @@
         <v>2030</v>
       </c>
       <c r="AE21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AJ21" s="24"/>
     </row>
@@ -3010,25 +3007,25 @@
         <v>902</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
         <v>120</v>
       </c>
-      <c r="F22" t="s">
-        <v>121</v>
-      </c>
       <c r="G22" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J22" s="27"/>
       <c r="K22" s="12"/>
       <c r="L22" s="7"/>
       <c r="P22" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q22" s="8">
         <v>0</v>
@@ -3062,12 +3059,12 @@
         <v>308</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" s="4"/>
       <c r="J23" s="27">
@@ -3116,16 +3113,16 @@
         <v>301</v>
       </c>
       <c r="D24" t="s">
+        <v>171</v>
+      </c>
+      <c r="E24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" t="s">
         <v>172</v>
       </c>
-      <c r="E24" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>174</v>
       </c>
       <c r="H24" s="4"/>
       <c r="J24" s="27">
@@ -3175,16 +3172,16 @@
         <v>211</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H25" s="4"/>
       <c r="J25" s="27">
@@ -3230,25 +3227,25 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26">
         <v>302</v>
       </c>
       <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" t="s">
         <v>108</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>109</v>
       </c>
-      <c r="F26" t="s">
-        <v>110</v>
-      </c>
       <c r="G26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J26" s="27">
         <v>1.26</v>
@@ -3266,7 +3263,7 @@
         <v>3</v>
       </c>
       <c r="O26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q26" s="8">
         <v>0</v>
@@ -3300,16 +3297,16 @@
         <v>354</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>169</v>
-      </c>
       <c r="G27" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H27" s="4"/>
       <c r="J27" s="27">
@@ -3359,16 +3356,16 @@
         <v>207</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="G28" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" s="4"/>
       <c r="J28" s="27">
@@ -3417,19 +3414,19 @@
         <v>857</v>
       </c>
       <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
         <v>31</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>32</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>33</v>
       </c>
-      <c r="G29" t="s">
-        <v>34</v>
-      </c>
       <c r="H29" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J29" s="27">
         <v>0.43</v>
@@ -3477,19 +3474,19 @@
         <v>803</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="G30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J30" s="27">
         <v>0.19</v>
@@ -3538,16 +3535,16 @@
         <v>352</v>
       </c>
       <c r="D31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="G31" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H31" s="4"/>
       <c r="J31" s="27">
@@ -3596,19 +3593,19 @@
         <v>804</v>
       </c>
       <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" t="s">
         <v>89</v>
       </c>
-      <c r="E32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" t="s">
-        <v>90</v>
-      </c>
       <c r="G32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J32" s="27">
         <v>2.2999999999999998</v>
@@ -3626,7 +3623,7 @@
         <v>3</v>
       </c>
       <c r="O32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q32" s="5">
         <v>1</v>
@@ -3656,19 +3653,19 @@
         <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33">
         <v>204</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J33" s="27">
         <v>0.43</v>
@@ -3717,16 +3714,16 @@
         <v>303</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="G34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H34" s="4"/>
       <c r="J34" s="27">
@@ -3776,19 +3773,19 @@
         <v>801</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E35" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" t="s">
         <v>83</v>
       </c>
-      <c r="F35" t="s">
-        <v>84</v>
-      </c>
       <c r="G35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J35" s="27">
         <v>1.43</v>
@@ -3837,16 +3834,16 @@
         <v>305</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" t="s">
         <v>148</v>
-      </c>
-      <c r="G36" t="s">
-        <v>149</v>
       </c>
       <c r="H36" s="4"/>
       <c r="J36" s="27">
@@ -3895,19 +3892,19 @@
         <v>858</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="H37" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J37" s="27">
         <v>1</v>
@@ -3956,16 +3953,16 @@
         <v>304</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H38" s="4"/>
       <c r="J38" s="27">
@@ -4011,25 +4008,25 @@
         <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>206</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" t="s">
         <v>78</v>
       </c>
-      <c r="F39" t="s">
-        <v>79</v>
-      </c>
       <c r="G39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J39" s="27">
         <v>0.35</v>
@@ -4077,16 +4074,16 @@
         <v>304</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E40" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" t="s">
         <v>78</v>
       </c>
-      <c r="F40" t="s">
-        <v>79</v>
-      </c>
       <c r="G40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H40" s="4"/>
       <c r="J40" s="27">
@@ -4132,25 +4129,25 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41">
         <v>210</v>
       </c>
       <c r="D41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J41" s="27">
         <v>2.48</v>
@@ -4168,7 +4165,7 @@
         <v>4</v>
       </c>
       <c r="O41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q41" s="8">
         <v>0</v>
@@ -4201,19 +4198,19 @@
         <v>709</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="H42" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J42" s="27">
         <v>0.54</v>
@@ -4261,19 +4258,19 @@
         <v>859</v>
       </c>
       <c r="D43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G43" t="s">
         <v>8</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J43" s="27">
         <v>0.47</v>
@@ -4318,23 +4315,23 @@
         <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H44" s="4"/>
       <c r="J44" s="27">
         <v>0.51</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M44">
         <v>8</v>
@@ -4374,16 +4371,16 @@
         <v>209</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="G45" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H45" s="4"/>
       <c r="J45" s="27">
@@ -4432,19 +4429,19 @@
         <v>805</v>
       </c>
       <c r="D46" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" t="s">
         <v>94</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>95</v>
       </c>
-      <c r="F46" t="s">
-        <v>96</v>
-      </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J46" s="27">
         <v>0.89</v>
@@ -4462,7 +4459,7 @@
         <v>3</v>
       </c>
       <c r="O46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q46" s="5">
         <v>1</v>
@@ -4496,12 +4493,12 @@
         <v>307</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H47" s="4"/>
       <c r="J47" s="27">
@@ -4550,19 +4547,19 @@
         <v>806</v>
       </c>
       <c r="D48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" t="s">
         <v>87</v>
       </c>
-      <c r="E48" t="s">
-        <v>85</v>
-      </c>
-      <c r="F48" t="s">
-        <v>86</v>
-      </c>
-      <c r="G48" t="s">
-        <v>88</v>
-      </c>
       <c r="H48" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J48" s="27">
         <v>0.28999999999999998</v>
@@ -4580,7 +4577,7 @@
         <v>4</v>
       </c>
       <c r="O48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q48" s="5">
         <v>1</v>
@@ -4610,16 +4607,16 @@
         <v>40</v>
       </c>
       <c r="D49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J49" s="27">
         <v>19.809999999999999</v>
@@ -4664,16 +4661,16 @@
         <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H50" s="4"/>
       <c r="J50" s="27">
@@ -4719,10 +4716,10 @@
         <v>42</v>
       </c>
       <c r="D51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H51" s="4"/>
       <c r="J51" s="27">
@@ -4768,10 +4765,10 @@
         <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H52" s="4"/>
       <c r="J52" s="27">
@@ -4817,16 +4814,16 @@
         <v>44</v>
       </c>
       <c r="D53" t="s">
+        <v>192</v>
+      </c>
+      <c r="E53" t="s">
+        <v>116</v>
+      </c>
+      <c r="F53" t="s">
         <v>193</v>
       </c>
-      <c r="E53" t="s">
-        <v>117</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>194</v>
-      </c>
-      <c r="G53" t="s">
-        <v>195</v>
       </c>
       <c r="H53" s="4"/>
       <c r="J53" s="27">
@@ -4845,7 +4842,7 @@
         <v>1</v>
       </c>
       <c r="O53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q53" s="8">
         <v>0</v>
@@ -4875,16 +4872,16 @@
         <v>45</v>
       </c>
       <c r="D54" t="s">
+        <v>196</v>
+      </c>
+      <c r="E54" t="s">
         <v>197</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" t="s">
         <v>198</v>
-      </c>
-      <c r="F54" t="s">
-        <v>117</v>
-      </c>
-      <c r="G54" t="s">
-        <v>199</v>
       </c>
       <c r="H54" s="4"/>
       <c r="J54" s="27">
@@ -4930,16 +4927,16 @@
         <v>46</v>
       </c>
       <c r="D55" t="s">
+        <v>199</v>
+      </c>
+      <c r="E55" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" t="s">
         <v>200</v>
       </c>
-      <c r="E55" t="s">
-        <v>117</v>
-      </c>
-      <c r="F55" t="s">
-        <v>201</v>
-      </c>
       <c r="G55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H55" s="4"/>
       <c r="J55" s="27">
@@ -4985,16 +4982,16 @@
         <v>47</v>
       </c>
       <c r="D56" t="s">
+        <v>201</v>
+      </c>
+      <c r="E56" t="s">
+        <v>60</v>
+      </c>
+      <c r="F56" t="s">
         <v>202</v>
       </c>
-      <c r="E56" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" t="s">
-        <v>203</v>
-      </c>
       <c r="G56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H56" s="4"/>
       <c r="J56" s="27">
@@ -5040,16 +5037,16 @@
         <v>48</v>
       </c>
       <c r="D57" t="s">
+        <v>203</v>
+      </c>
+      <c r="E57" t="s">
         <v>204</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>205</v>
       </c>
-      <c r="F57" t="s">
-        <v>206</v>
-      </c>
       <c r="G57" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H57" s="4"/>
       <c r="J57" s="27">
@@ -5095,10 +5092,10 @@
         <v>102</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H58" s="4"/>
       <c r="J58" s="27">
@@ -5144,10 +5141,10 @@
         <v>103</v>
       </c>
       <c r="D59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H59" s="4"/>
       <c r="J59" s="27">
@@ -5193,16 +5190,16 @@
         <v>104</v>
       </c>
       <c r="D60" t="s">
+        <v>210</v>
+      </c>
+      <c r="E60" t="s">
+        <v>149</v>
+      </c>
+      <c r="F60" t="s">
         <v>211</v>
       </c>
-      <c r="E60" t="s">
-        <v>150</v>
-      </c>
-      <c r="F60" t="s">
-        <v>212</v>
-      </c>
       <c r="G60" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H60" s="4"/>
       <c r="J60" s="27">
@@ -5248,16 +5245,16 @@
         <v>105</v>
       </c>
       <c r="D61" t="s">
+        <v>212</v>
+      </c>
+      <c r="E61" t="s">
         <v>213</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>214</v>
       </c>
-      <c r="F61" t="s">
-        <v>215</v>
-      </c>
       <c r="G61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H61" s="4"/>
       <c r="J61" s="27">
@@ -5303,10 +5300,10 @@
         <v>106</v>
       </c>
       <c r="D62" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G62" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H62" s="4"/>
       <c r="J62" s="27">
@@ -5352,16 +5349,16 @@
         <v>107</v>
       </c>
       <c r="D63" t="s">
+        <v>216</v>
+      </c>
+      <c r="E63" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" t="s">
         <v>217</v>
       </c>
-      <c r="E63" t="s">
-        <v>31</v>
-      </c>
-      <c r="F63" t="s">
-        <v>218</v>
-      </c>
       <c r="G63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H63" s="4"/>
       <c r="J63" s="27">
@@ -5407,16 +5404,16 @@
         <v>108</v>
       </c>
       <c r="D64" t="s">
+        <v>218</v>
+      </c>
+      <c r="E64" t="s">
+        <v>207</v>
+      </c>
+      <c r="F64" t="s">
         <v>219</v>
       </c>
-      <c r="E64" t="s">
-        <v>208</v>
-      </c>
-      <c r="F64" t="s">
-        <v>220</v>
-      </c>
       <c r="G64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J64" s="27">
         <v>3.24</v>
@@ -5461,10 +5458,10 @@
         <v>109</v>
       </c>
       <c r="D65" t="s">
+        <v>220</v>
+      </c>
+      <c r="G65" t="s">
         <v>221</v>
-      </c>
-      <c r="G65" t="s">
-        <v>222</v>
       </c>
       <c r="J65" s="27">
         <v>3.81</v>
@@ -5509,16 +5506,16 @@
         <v>110</v>
       </c>
       <c r="D66" t="s">
+        <v>222</v>
+      </c>
+      <c r="E66" t="s">
         <v>223</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>224</v>
       </c>
-      <c r="F66" t="s">
-        <v>225</v>
-      </c>
       <c r="G66" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J66" s="27">
         <v>0.69</v>
@@ -5563,16 +5560,16 @@
         <v>111</v>
       </c>
       <c r="D67" t="s">
+        <v>225</v>
+      </c>
+      <c r="E67" t="s">
         <v>226</v>
       </c>
-      <c r="E67" t="s">
-        <v>227</v>
-      </c>
       <c r="F67" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G67" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J67" s="27">
         <v>16.190000000000001</v>
@@ -5617,16 +5614,16 @@
         <v>112</v>
       </c>
       <c r="D68" t="s">
+        <v>227</v>
+      </c>
+      <c r="E68" t="s">
         <v>228</v>
       </c>
-      <c r="E68" t="s">
-        <v>229</v>
-      </c>
       <c r="F68" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G68" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J68" s="27">
         <v>3.25</v>
@@ -5674,16 +5671,16 @@
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" t="s">
+        <v>229</v>
+      </c>
+      <c r="E69" t="s">
+        <v>142</v>
+      </c>
+      <c r="F69" t="s">
         <v>230</v>
       </c>
-      <c r="E69" t="s">
-        <v>143</v>
-      </c>
-      <c r="F69" t="s">
-        <v>231</v>
-      </c>
       <c r="G69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H69" s="4"/>
       <c r="J69" s="27">
@@ -5732,16 +5729,16 @@
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E70" s="4" t="s">
-        <v>235</v>
-      </c>
       <c r="F70" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -5791,10 +5788,10 @@
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H71" s="4"/>
       <c r="J71" s="27">
@@ -5843,10 +5840,10 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H72" s="4"/>
       <c r="J72" s="27">
@@ -5895,10 +5892,10 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
@@ -5948,16 +5945,16 @@
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
@@ -6007,16 +6004,16 @@
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E75" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -6365,23 +6362,23 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="H9" s="3" t="s">
         <v>0</v>
       </c>
@@ -6389,342 +6386,342 @@
         <v>1</v>
       </c>
       <c r="J9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="N9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
       <c r="O10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
       <c r="O11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
         <v>46</v>
       </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
       <c r="G12" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12"/>
       <c r="K12"/>
       <c r="O12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>56</v>
       </c>
       <c r="J13"/>
       <c r="K13" s="10"/>
       <c r="O13" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>58</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>59</v>
       </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
       <c r="G14" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J14"/>
       <c r="O14" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J15"/>
       <c r="K15"/>
       <c r="O15" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
         <v>63</v>
       </c>
-      <c r="C16" t="s">
-        <v>64</v>
-      </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16"/>
       <c r="K16"/>
       <c r="O16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>70</v>
       </c>
-      <c r="F17" t="s">
-        <v>71</v>
-      </c>
       <c r="G17" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J17"/>
       <c r="K17"/>
       <c r="O17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
         <v>91</v>
       </c>
-      <c r="D18" t="s">
-        <v>92</v>
-      </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G18" s="4"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="N18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
         <v>97</v>
       </c>
-      <c r="D19" t="s">
-        <v>98</v>
-      </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G19" s="4"/>
       <c r="J19"/>
       <c r="K19"/>
       <c r="N19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="G20" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="N20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G21" s="4"/>
       <c r="J21"/>
       <c r="K21" s="10"/>
       <c r="N21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G22" s="4"/>
       <c r="J22"/>
       <c r="K22"/>
       <c r="N22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="F23" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J23"/>
       <c r="O23" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J24"/>
       <c r="O24" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
         <v>19</v>
       </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
       <c r="F25" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J25"/>
       <c r="K25"/>
       <c r="O25" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
@@ -6754,28 +6751,28 @@
     </row>
     <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>0</v>
@@ -6784,40 +6781,40 @@
         <v>1</v>
       </c>
       <c r="K28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="N28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N28" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="O28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P28" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="P28" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="Q28" s="15" t="s">
         <v>2</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S28" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="T28" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="T28" s="3" t="s">
+      <c r="U28" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="U28" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="V28" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -6825,12 +6822,12 @@
         <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I29"/>
       <c r="J29" s="27"/>
@@ -6859,16 +6856,16 @@
         <v>101</v>
       </c>
       <c r="D30" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" t="s">
         <v>207</v>
       </c>
-      <c r="E30" t="s">
-        <v>208</v>
-      </c>
       <c r="F30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H30" s="4"/>
       <c r="J30" s="27"/>
@@ -7307,16 +7304,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7324,7 +7321,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="8">
         <v>10140</v>
@@ -7338,10 +7335,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -7352,7 +7349,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="8">
         <v>3838</v>
@@ -7366,7 +7363,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="8">
         <v>10452</v>
@@ -7380,7 +7377,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="8">
         <v>10109</v>
@@ -7394,10 +7391,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -7408,7 +7405,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="8">
         <v>7456</v>
@@ -7422,7 +7419,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" s="8">
         <v>8857</v>
@@ -7436,7 +7433,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" s="8">
         <v>10577</v>
@@ -7450,7 +7447,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" s="8">
         <v>4379</v>
@@ -7464,7 +7461,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="8">
         <v>4089</v>
@@ -7478,7 +7475,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="8">
         <v>10126</v>
@@ -7492,7 +7489,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C14" s="8">
         <v>4213</v>
@@ -7506,7 +7503,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" s="8">
         <v>10951</v>
@@ -7520,7 +7517,7 @@
         <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" s="8">
         <v>10416</v>
@@ -7534,7 +7531,7 @@
         <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" s="8">
         <v>10952</v>
@@ -7548,7 +7545,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="8">
         <v>10507</v>
@@ -7562,7 +7559,7 @@
         <v>30</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="8">
         <v>10428</v>
@@ -7576,7 +7573,7 @@
         <v>31</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="8">
         <v>11003</v>
@@ -7590,7 +7587,7 @@
         <v>32</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" s="8">
         <v>10447</v>
@@ -7604,7 +7601,7 @@
         <v>33</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22" s="8">
         <v>8768</v>
@@ -7618,7 +7615,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C23" s="8">
         <v>3508</v>
@@ -7632,7 +7629,7 @@
         <v>102</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C24" s="8">
         <v>3737</v>
@@ -7646,10 +7643,10 @@
         <v>104</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
@@ -7660,7 +7657,7 @@
         <v>105</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C26" s="8">
         <v>3994</v>
@@ -7674,7 +7671,7 @@
         <v>106</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C27" s="8">
         <v>10431</v>
@@ -7688,7 +7685,7 @@
         <v>107</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" s="8">
         <v>4394</v>
@@ -7702,10 +7699,10 @@
         <v>108</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
@@ -7716,10 +7713,10 @@
         <v>109</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -7730,7 +7727,7 @@
         <v>110</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C31" s="8">
         <v>5321</v>
@@ -7744,7 +7741,7 @@
         <v>111</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" s="8">
         <v>8735</v>
@@ -7758,7 +7755,7 @@
         <v>112</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C33" s="8">
         <v>10420</v>
@@ -7772,7 +7769,7 @@
         <v>113</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C34" s="8">
         <v>10421</v>
@@ -7786,7 +7783,7 @@
         <v>115</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C35" s="8">
         <v>4071</v>
@@ -7800,7 +7797,7 @@
         <v>116</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C36" s="8">
         <v>10456</v>
@@ -7814,7 +7811,7 @@
         <v>117</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C37" s="8">
         <v>10490</v>
@@ -7828,7 +7825,7 @@
         <v>120</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C38" s="8">
         <v>9870</v>

</xml_diff>

<commit_message>
Add some cost info
Added a few project costs in manually. Waiting
on the project cost XLSX from the ORTP to
perform a join for all projects.
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -1479,8 +1479,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2182091" y="0"/>
-          <a:ext cx="10021727" cy="1366683"/>
+          <a:off x="2178326" y="0"/>
+          <a:ext cx="10042810" cy="1366683"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -2097,7 +2097,7 @@
   </sheetPr>
   <dimension ref="A1:AJ97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -2286,6 +2286,9 @@
         <v>8</v>
       </c>
       <c r="H10" s="4"/>
+      <c r="I10">
+        <v>100000000</v>
+      </c>
       <c r="J10" s="27">
         <v>2.5</v>
       </c>
@@ -2702,6 +2705,9 @@
         <v>156</v>
       </c>
       <c r="H17" s="4"/>
+      <c r="I17">
+        <v>90000000</v>
+      </c>
       <c r="J17" s="27">
         <v>2.0299999999999998</v>
       </c>
@@ -3368,6 +3374,9 @@
         <v>8</v>
       </c>
       <c r="H28" s="4"/>
+      <c r="I28">
+        <v>300000000</v>
+      </c>
       <c r="J28" s="27">
         <v>1.9</v>
       </c>
@@ -3667,6 +3676,9 @@
       <c r="H33" s="22" t="s">
         <v>39</v>
       </c>
+      <c r="I33">
+        <v>116000000</v>
+      </c>
       <c r="J33" s="27">
         <v>0.43</v>
       </c>
@@ -4028,6 +4040,9 @@
       <c r="H39" s="21" t="s">
         <v>72</v>
       </c>
+      <c r="I39">
+        <v>20000000</v>
+      </c>
       <c r="J39" s="27">
         <v>0.35</v>
       </c>
@@ -4383,6 +4398,9 @@
         <v>8</v>
       </c>
       <c r="H45" s="4"/>
+      <c r="I45">
+        <v>80000000</v>
+      </c>
       <c r="J45" s="27">
         <v>1.46</v>
       </c>

</xml_diff>

<commit_message>
Add cost info to project management xlsx
Joined from the 2040 ORTP project table
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -2347,6 +2347,9 @@
         <v>8</v>
       </c>
       <c r="H11" s="4"/>
+      <c r="I11">
+        <v>252000000</v>
+      </c>
       <c r="J11" s="27">
         <v>7.2</v>
       </c>
@@ -2406,6 +2409,9 @@
         <v>8</v>
       </c>
       <c r="H12" s="4"/>
+      <c r="I12">
+        <v>142000000</v>
+      </c>
       <c r="J12" s="27">
         <v>2.75</v>
       </c>
@@ -2468,6 +2474,9 @@
         <v>8</v>
       </c>
       <c r="H13" s="4"/>
+      <c r="I13">
+        <v>50000000</v>
+      </c>
       <c r="J13" s="27">
         <v>1.25</v>
       </c>
@@ -2527,6 +2536,9 @@
         <v>8</v>
       </c>
       <c r="H14" s="4"/>
+      <c r="I14">
+        <v>12000000</v>
+      </c>
       <c r="J14" s="27">
         <v>0.28000000000000003</v>
       </c>
@@ -2646,6 +2658,9 @@
         <v>151</v>
       </c>
       <c r="H16" s="4"/>
+      <c r="I16">
+        <v>50000000</v>
+      </c>
       <c r="J16" s="27">
         <v>1.75</v>
       </c>
@@ -2764,6 +2779,9 @@
       </c>
       <c r="H18" s="21" t="s">
         <v>72</v>
+      </c>
+      <c r="I18">
+        <v>5000000</v>
       </c>
       <c r="J18" s="27">
         <v>0.01</v>
@@ -3073,6 +3091,9 @@
         <v>102</v>
       </c>
       <c r="H23" s="4"/>
+      <c r="I23">
+        <v>111000000</v>
+      </c>
       <c r="J23" s="27">
         <v>5.57</v>
       </c>
@@ -3131,6 +3152,9 @@
         <v>173</v>
       </c>
       <c r="H24" s="4"/>
+      <c r="I24">
+        <v>130000000</v>
+      </c>
       <c r="J24" s="27">
         <v>2.72</v>
       </c>
@@ -3190,6 +3214,9 @@
         <v>8</v>
       </c>
       <c r="H25" s="4"/>
+      <c r="I25">
+        <v>103000000</v>
+      </c>
       <c r="J25" s="27">
         <v>3.32</v>
       </c>
@@ -3253,6 +3280,9 @@
       <c r="H26" s="22" t="s">
         <v>39</v>
       </c>
+      <c r="I26">
+        <v>32000000</v>
+      </c>
       <c r="J26" s="27">
         <v>1.26</v>
       </c>
@@ -3315,6 +3345,9 @@
         <v>148</v>
       </c>
       <c r="H27" s="4"/>
+      <c r="I27">
+        <v>293000000</v>
+      </c>
       <c r="J27" s="27">
         <v>3.99</v>
       </c>
@@ -3497,6 +3530,9 @@
       <c r="H30" s="21" t="s">
         <v>114</v>
       </c>
+      <c r="I30">
+        <v>1350000</v>
+      </c>
       <c r="J30" s="27">
         <v>0.19</v>
       </c>
@@ -3556,6 +3592,9 @@
         <v>148</v>
       </c>
       <c r="H31" s="4"/>
+      <c r="I31">
+        <v>26000000</v>
+      </c>
       <c r="J31" s="27">
         <v>0.65</v>
       </c>
@@ -3616,6 +3655,9 @@
       <c r="H32" s="21" t="s">
         <v>114</v>
       </c>
+      <c r="I32">
+        <v>77000</v>
+      </c>
       <c r="J32" s="27">
         <v>2.2999999999999998</v>
       </c>
@@ -3738,6 +3780,9 @@
         <v>143</v>
       </c>
       <c r="H34" s="4"/>
+      <c r="I34">
+        <v>48000000</v>
+      </c>
       <c r="J34" s="27">
         <v>1.28</v>
       </c>
@@ -3799,6 +3844,9 @@
       <c r="H35" s="22" t="s">
         <v>39</v>
       </c>
+      <c r="I35">
+        <v>13300000</v>
+      </c>
       <c r="J35" s="27">
         <v>1.43</v>
       </c>
@@ -3858,6 +3906,9 @@
         <v>148</v>
       </c>
       <c r="H36" s="4"/>
+      <c r="I36">
+        <v>227000000</v>
+      </c>
       <c r="J36" s="27">
         <v>2.19</v>
       </c>
@@ -3918,6 +3969,9 @@
       <c r="H37" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I37">
+        <v>500000</v>
+      </c>
       <c r="J37" s="27">
         <v>1</v>
       </c>
@@ -3977,6 +4031,9 @@
         <v>8</v>
       </c>
       <c r="H38" s="4"/>
+      <c r="I38">
+        <v>180000000</v>
+      </c>
       <c r="J38" s="27">
         <v>2.36</v>
       </c>
@@ -4101,6 +4158,9 @@
         <v>8</v>
       </c>
       <c r="H40" s="4"/>
+      <c r="I40">
+        <v>180000000</v>
+      </c>
       <c r="J40" s="27">
         <v>0.35</v>
       </c>
@@ -4164,6 +4224,9 @@
       <c r="H41" s="22" t="s">
         <v>72</v>
       </c>
+      <c r="I41">
+        <v>76000000</v>
+      </c>
       <c r="J41" s="27">
         <v>2.48</v>
       </c>
@@ -4226,6 +4289,9 @@
       </c>
       <c r="H42" s="22" t="s">
         <v>16</v>
+      </c>
+      <c r="I42">
+        <v>18200000</v>
       </c>
       <c r="J42" s="27">
         <v>0.54</v>
@@ -4519,6 +4585,9 @@
         <v>8</v>
       </c>
       <c r="H47" s="4"/>
+      <c r="I47">
+        <v>33000000</v>
+      </c>
       <c r="J47" s="27">
         <v>1.25</v>
       </c>
@@ -4578,6 +4647,9 @@
       </c>
       <c r="H48" s="21" t="s">
         <v>114</v>
+      </c>
+      <c r="I48">
+        <v>77000</v>
       </c>
       <c r="J48" s="27">
         <v>0.28999999999999998</v>

</xml_diff>

<commit_message>
Make minor updates to project list and network to conform with TIP
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEECCA3F-19A9-4621-84FD-64BFB48EE32B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="450" windowWidth="18510" windowHeight="12015"/>
+    <workbookView xWindow="4305" yWindow="450" windowWidth="18510" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proj Attributes and Scenarios" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="252">
   <si>
     <t>Cost</t>
   </si>
@@ -768,12 +769,21 @@
   </si>
   <si>
     <t>congested corridor?</t>
+  </si>
+  <si>
+    <t>OC23</t>
+  </si>
+  <si>
+    <t>OC6</t>
+  </si>
+  <si>
+    <t>OC27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1372,9 +1382,9 @@
     <cellStyle name="Linked Cell" xfId="15" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="11" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2 6" xfId="1"/>
-    <cellStyle name="Normal 31" xfId="3"/>
-    <cellStyle name="Normal 9" xfId="2"/>
+    <cellStyle name="Normal 2 2 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 31" xfId="3" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 9" xfId="2" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
     <cellStyle name="Note" xfId="18" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="13" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="4" builtinId="15" customBuiltin="1"/>
@@ -1414,7 +1424,13 @@
     <xdr:ext cx="1288045" cy="357790"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1474,7 +1490,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="11" name="Group 10"/>
+        <xdr:cNvPr id="11" name="Group 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -1487,7 +1509,13 @@
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="12" name="Group 11"/>
+          <xdr:cNvPr id="12" name="Group 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
@@ -1500,7 +1528,13 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="14" name="Picture 13"/>
+            <xdr:cNvPr id="14" name="Picture 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvPicPr>
               <a:picLocks noChangeAspect="1"/>
             </xdr:cNvPicPr>
@@ -1529,7 +1563,13 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="15" name="Picture 14"/>
+            <xdr:cNvPr id="15" name="Picture 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvPicPr>
               <a:picLocks noChangeAspect="1"/>
             </xdr:cNvPicPr>
@@ -1559,7 +1599,13 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="TextBox 12"/>
+          <xdr:cNvPr id="13" name="TextBox 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1621,7 +1667,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Screen Clipping"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Screen Clipping">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1670,7 +1722,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="3" name="Group 2"/>
+        <xdr:cNvPr id="3" name="Group 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -1683,7 +1741,13 @@
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="4" name="Group 3"/>
+          <xdr:cNvPr id="4" name="Group 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
@@ -1696,7 +1760,13 @@
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="6" name="Picture 5"/>
+            <xdr:cNvPr id="6" name="Picture 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvPicPr>
               <a:picLocks noChangeAspect="1"/>
             </xdr:cNvPicPr>
@@ -1725,7 +1795,13 @@
         </xdr:pic>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="7" name="Picture 6"/>
+            <xdr:cNvPr id="7" name="Picture 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvPicPr>
               <a:picLocks noChangeAspect="1"/>
             </xdr:cNvPicPr>
@@ -1755,7 +1831,13 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="TextBox 4"/>
+          <xdr:cNvPr id="5" name="TextBox 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1881,6 +1963,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1916,6 +2015,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2091,7 +2207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2269,7 +2385,9 @@
       <c r="A10" s="4">
         <v>1</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>251</v>
+      </c>
       <c r="C10" s="4">
         <v>205</v>
       </c>
@@ -3825,7 +3943,9 @@
       <c r="A35" s="4">
         <v>26</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="C35" s="4">
         <v>801</v>
       </c>
@@ -4447,7 +4567,9 @@
       <c r="A45" s="4">
         <v>36</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="C45" s="4">
         <v>209</v>
       </c>
@@ -4465,10 +4587,10 @@
       </c>
       <c r="H45" s="4"/>
       <c r="I45">
-        <v>80000000</v>
+        <v>87280000</v>
       </c>
       <c r="J45" s="27">
-        <v>1.46</v>
+        <v>0.99</v>
       </c>
       <c r="K45" s="4">
         <v>2</v>
@@ -6378,9 +6500,9 @@
       <c r="D97" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:W75"/>
+  <autoFilter ref="A9:W75" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I89:I91"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I89:I91" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="40" orientation="landscape" r:id="rId1"/>
@@ -6389,7 +6511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7367,8 +7489,8 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If complete, input the year. Otherwise:_x000a_Committed_x000a_Consideration" sqref="G9"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="H12 H10 H85:H87"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If complete, input the year. Otherwise:_x000a_Committed_x000a_Consideration" sqref="G9" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="H12 H10 H85:H87" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="56" orientation="landscape" r:id="rId1"/>
@@ -7377,7 +7499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Update the project management sheet for TIP analysis
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEECCA3F-19A9-4621-84FD-64BFB48EE32B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46A0B94-B8F4-0A40-B267-2DEE9731E512}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="450" windowWidth="18510" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proj Attributes and Scenarios" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$64:$O$84</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$W$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$V$75</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="251">
   <si>
     <t>Cost</t>
   </si>
@@ -567,21 +567,6 @@
     <t>2040 LRTP w/o Dev Proj</t>
   </si>
   <si>
-    <t>Plan Scenarios to Run</t>
-  </si>
-  <si>
-    <t>transit</t>
-  </si>
-  <si>
-    <t>no bus/rail integration</t>
-  </si>
-  <si>
-    <t>bus/rail integration</t>
-  </si>
-  <si>
-    <t>bus/rail integration + HUB</t>
-  </si>
-  <si>
     <t>2040 LRTP</t>
   </si>
   <si>
@@ -778,6 +763,18 @@
   </si>
   <si>
     <t>OC27</t>
+  </si>
+  <si>
+    <t>TIP</t>
+  </si>
+  <si>
+    <t>OS59</t>
+  </si>
+  <si>
+    <t>EC 4 TIP</t>
+  </si>
+  <si>
+    <t>For 2040 ORTP:</t>
   </si>
 </sst>
 </file>
@@ -1501,8 +1498,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2178326" y="0"/>
-          <a:ext cx="10042810" cy="1366683"/>
+          <a:off x="2497667" y="0"/>
+          <a:ext cx="11268636" cy="1366683"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -1654,16 +1651,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148166</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>343458</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85843</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>301124</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>37794</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1692,8 +1689,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27974925" y="2286000"/>
-          <a:ext cx="4001058" cy="847843"/>
+          <a:off x="29633333" y="2815166"/>
+          <a:ext cx="4407458" cy="842128"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1733,8 +1730,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1181100" y="0"/>
-          <a:ext cx="10049436" cy="1366683"/>
+          <a:off x="1346200" y="0"/>
+          <a:ext cx="11268636" cy="1366683"/>
           <a:chOff x="3473823" y="78441"/>
           <a:chExt cx="10058400" cy="1366683"/>
         </a:xfrm>
@@ -2211,73 +2208,70 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ97"/>
+  <dimension ref="A1:AG97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="7" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="5" customWidth="1"/>
-    <col min="13" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="7" width="32.5" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" style="5" customWidth="1"/>
+    <col min="13" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="18" customWidth="1"/>
     <col min="17" max="17" width="18" style="5" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
-    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="24" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="P1" s="16"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="P2" s="16"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="P3" s="16"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="P4" s="16"/>
       <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="P5" s="16"/>
       <c r="Q5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="P6" s="16"/>
       <c r="Q6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="P7" s="16"/>
       <c r="Q7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2306,11 +2300,8 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-    </row>
-    <row r="9" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>175</v>
       </c>
@@ -2366,27 +2357,24 @@
         <v>71</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>179</v>
+        <v>236</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>180</v>
+        <v>249</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C10" s="4">
         <v>205</v>
@@ -2431,20 +2419,17 @@
       <c r="S10">
         <v>1</v>
       </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10">
-        <v>1</v>
+      <c r="T10" s="24">
+        <v>1</v>
+      </c>
+      <c r="U10" s="24">
+        <v>0</v>
       </c>
       <c r="V10">
         <v>1</v>
       </c>
-      <c r="W10" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -2490,23 +2475,20 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-      <c r="W11" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="24"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T11" s="24">
+        <v>1</v>
+      </c>
+      <c r="U11" s="24">
+        <v>0</v>
+      </c>
+      <c r="V11" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="24"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -2552,26 +2534,28 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
-      <c r="W12" s="24">
-        <v>1</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>181</v>
-      </c>
-      <c r="AJ12" s="24"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T12" s="24">
+        <v>1</v>
+      </c>
+      <c r="U12" s="24">
+        <v>0</v>
+      </c>
+      <c r="V12" s="8">
+        <v>0</v>
+      </c>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AG12" s="24"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2617,23 +2601,28 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-      <c r="V13">
-        <v>1</v>
-      </c>
-      <c r="W13" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="24"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T13" s="24">
+        <v>1</v>
+      </c>
+      <c r="U13" s="24">
+        <v>0</v>
+      </c>
+      <c r="V13" s="8">
+        <v>0</v>
+      </c>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="24"/>
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="24"/>
+      <c r="AD13" s="24"/>
+      <c r="AG13" s="24"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>5</v>
       </c>
@@ -2679,23 +2668,30 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-      <c r="W14" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ14" s="24"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T14" s="24">
+        <v>1</v>
+      </c>
+      <c r="U14" s="24">
+        <v>0</v>
+      </c>
+      <c r="V14" s="8">
+        <v>0</v>
+      </c>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="24"/>
+      <c r="AB14" s="24"/>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+      <c r="AG14" s="24"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2741,21 +2737,26 @@
       <c r="S15">
         <v>1</v>
       </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="24"/>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T15" s="24">
+        <v>0</v>
+      </c>
+      <c r="U15" s="24">
+        <v>1</v>
+      </c>
+      <c r="V15" s="8">
+        <v>0</v>
+      </c>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="24"/>
+      <c r="AG15" s="24"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>7</v>
       </c>
@@ -2801,27 +2802,34 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ16" s="24"/>
-    </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T16" s="24">
+        <v>1</v>
+      </c>
+      <c r="U16" s="24">
+        <v>0</v>
+      </c>
+      <c r="V16" s="8">
+        <v>0</v>
+      </c>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="24"/>
+      <c r="AG16" s="24"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>8</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="C17" s="4">
         <v>208</v>
       </c>
@@ -2865,21 +2873,26 @@
       <c r="S17">
         <v>1</v>
       </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17">
-        <v>1</v>
+      <c r="T17" s="24">
+        <v>1</v>
+      </c>
+      <c r="U17" s="24">
+        <v>0</v>
       </c>
       <c r="V17">
         <v>1</v>
       </c>
-      <c r="W17" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ17" s="24"/>
-    </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24"/>
+      <c r="AG17" s="24"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -2926,24 +2939,26 @@
       <c r="S18">
         <v>1</v>
       </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
-      <c r="U18">
-        <v>1</v>
+      <c r="T18" s="24">
+        <v>0</v>
+      </c>
+      <c r="U18" s="24">
+        <v>0</v>
       </c>
       <c r="V18">
         <v>1</v>
       </c>
-      <c r="W18" s="24">
-        <v>0</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>182</v>
-      </c>
-      <c r="AJ18" s="24"/>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AG18" s="24"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10</v>
       </c>
@@ -2989,27 +3004,26 @@
       <c r="S19">
         <v>1</v>
       </c>
-      <c r="T19">
-        <v>1</v>
-      </c>
-      <c r="U19">
-        <v>1</v>
-      </c>
-      <c r="V19">
-        <v>1</v>
-      </c>
-      <c r="W19" s="24">
-        <v>0</v>
-      </c>
-      <c r="AD19">
-        <v>2012</v>
-      </c>
-      <c r="AE19" t="s">
-        <v>183</v>
-      </c>
-      <c r="AJ19" s="24"/>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T19" s="24">
+        <v>0</v>
+      </c>
+      <c r="U19" s="24">
+        <v>1</v>
+      </c>
+      <c r="V19" s="8">
+        <v>0</v>
+      </c>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="24"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="24"/>
+      <c r="AD19" s="24"/>
+      <c r="AG19" s="24"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>11</v>
       </c>
@@ -3055,27 +3069,26 @@
       <c r="S20">
         <v>1</v>
       </c>
-      <c r="T20">
-        <v>1</v>
-      </c>
-      <c r="U20">
-        <v>1</v>
-      </c>
-      <c r="V20">
-        <v>1</v>
-      </c>
-      <c r="W20" s="24">
-        <v>0</v>
-      </c>
-      <c r="AD20">
-        <v>2020</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>184</v>
-      </c>
-      <c r="AJ20" s="24"/>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T20" s="24">
+        <v>0</v>
+      </c>
+      <c r="U20" s="24">
+        <v>1</v>
+      </c>
+      <c r="V20" s="8">
+        <v>0</v>
+      </c>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
+      <c r="AD20" s="24"/>
+      <c r="AG20" s="24"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>12</v>
       </c>
@@ -3121,27 +3134,26 @@
       <c r="S21">
         <v>1</v>
       </c>
-      <c r="T21">
-        <v>1</v>
-      </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
-      <c r="V21">
-        <v>1</v>
-      </c>
-      <c r="W21" s="24">
-        <v>0</v>
-      </c>
-      <c r="AD21">
-        <v>2030</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>185</v>
-      </c>
-      <c r="AJ21" s="24"/>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T21" s="24">
+        <v>0</v>
+      </c>
+      <c r="U21" s="24">
+        <v>1</v>
+      </c>
+      <c r="V21" s="8">
+        <v>0</v>
+      </c>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="24"/>
+      <c r="AD21" s="24"/>
+      <c r="AG21" s="24"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>13</v>
       </c>
@@ -3178,21 +3190,18 @@
       <c r="S22">
         <v>0</v>
       </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="24"/>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T22" s="24">
+        <v>0</v>
+      </c>
+      <c r="U22" s="24">
+        <v>0</v>
+      </c>
+      <c r="V22" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="24"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>14</v>
       </c>
@@ -3234,23 +3243,20 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>1</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>1</v>
-      </c>
-      <c r="W23" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ23" s="24"/>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T23" s="24">
+        <v>1</v>
+      </c>
+      <c r="U23" s="24">
+        <v>0</v>
+      </c>
+      <c r="V23" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG23" s="24"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>15</v>
       </c>
@@ -3295,23 +3301,20 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-      <c r="V24">
-        <v>1</v>
-      </c>
-      <c r="W24" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ24" s="24"/>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T24" s="24">
+        <v>1</v>
+      </c>
+      <c r="U24" s="24">
+        <v>0</v>
+      </c>
+      <c r="V24" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="24"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>16</v>
       </c>
@@ -3359,21 +3362,18 @@
       <c r="S25">
         <v>1</v>
       </c>
-      <c r="T25">
-        <v>1</v>
-      </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-      <c r="V25">
-        <v>1</v>
-      </c>
-      <c r="W25" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ25" s="24"/>
-    </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T25" s="24">
+        <v>1</v>
+      </c>
+      <c r="U25" s="24">
+        <v>0</v>
+      </c>
+      <c r="V25" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG25" s="24"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>17</v>
       </c>
@@ -3423,26 +3423,23 @@
         <v>0</v>
       </c>
       <c r="R26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="T26" s="24">
+        <v>1</v>
+      </c>
+      <c r="U26" s="24">
         <v>0</v>
       </c>
       <c r="V26">
         <v>1</v>
       </c>
-      <c r="W26" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ26" s="24"/>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG26" s="24"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>18</v>
       </c>
@@ -3488,23 +3485,20 @@
         <v>0</v>
       </c>
       <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
-      <c r="W27" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ27" s="24"/>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T27" s="24">
+        <v>1</v>
+      </c>
+      <c r="U27" s="24">
+        <v>0</v>
+      </c>
+      <c r="V27" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="24"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>19</v>
       </c>
@@ -3552,21 +3546,18 @@
       <c r="S28">
         <v>1</v>
       </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
-      <c r="W28" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ28" s="24"/>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T28" s="24">
+        <v>1</v>
+      </c>
+      <c r="U28" s="24">
+        <v>0</v>
+      </c>
+      <c r="V28" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="24"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -3612,21 +3603,18 @@
       <c r="S29">
         <v>1</v>
       </c>
-      <c r="T29">
-        <v>1</v>
-      </c>
-      <c r="U29">
-        <v>1</v>
-      </c>
-      <c r="V29">
-        <v>1</v>
-      </c>
-      <c r="W29" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ29" s="24"/>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T29" s="24">
+        <v>0</v>
+      </c>
+      <c r="U29" s="24">
+        <v>1</v>
+      </c>
+      <c r="V29" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG29" s="24"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>21</v>
       </c>
@@ -3675,21 +3663,18 @@
       <c r="S30">
         <v>1</v>
       </c>
-      <c r="T30">
-        <v>1</v>
-      </c>
-      <c r="U30">
-        <v>1</v>
-      </c>
-      <c r="V30">
-        <v>1</v>
-      </c>
-      <c r="W30" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="24"/>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T30" s="24">
+        <v>0</v>
+      </c>
+      <c r="U30" s="24">
+        <v>1</v>
+      </c>
+      <c r="V30" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG30" s="24"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>22</v>
       </c>
@@ -3735,23 +3720,20 @@
         <v>0</v>
       </c>
       <c r="S31">
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-      <c r="V31">
-        <v>1</v>
-      </c>
-      <c r="W31" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="24"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T31" s="24">
+        <v>1</v>
+      </c>
+      <c r="U31" s="24">
+        <v>0</v>
+      </c>
+      <c r="V31" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG31" s="24"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>23</v>
       </c>
@@ -3803,21 +3785,18 @@
       <c r="S32">
         <v>1</v>
       </c>
-      <c r="T32">
-        <v>1</v>
-      </c>
-      <c r="U32">
-        <v>1</v>
-      </c>
-      <c r="V32">
-        <v>1</v>
-      </c>
-      <c r="W32" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ32" s="24"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T32" s="24">
+        <v>0</v>
+      </c>
+      <c r="U32" s="24">
+        <v>1</v>
+      </c>
+      <c r="V32" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="24"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>24</v>
       </c>
@@ -3863,21 +3842,18 @@
       <c r="S33">
         <v>1</v>
       </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
-      <c r="U33">
-        <v>1</v>
+      <c r="T33" s="24">
+        <v>0</v>
+      </c>
+      <c r="U33" s="24">
+        <v>0</v>
       </c>
       <c r="V33">
         <v>1</v>
       </c>
-      <c r="W33" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ33" s="24"/>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG33" s="24"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -3923,28 +3899,25 @@
         <v>0</v>
       </c>
       <c r="S34">
-        <v>0</v>
-      </c>
-      <c r="T34">
-        <v>1</v>
-      </c>
-      <c r="U34">
-        <v>0</v>
-      </c>
-      <c r="V34">
-        <v>1</v>
-      </c>
-      <c r="W34" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ34" s="24"/>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T34" s="24">
+        <v>1</v>
+      </c>
+      <c r="U34" s="24">
+        <v>0</v>
+      </c>
+      <c r="V34" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="24"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>26</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C35" s="4">
         <v>801</v>
@@ -3991,21 +3964,18 @@
       <c r="S35">
         <v>1</v>
       </c>
-      <c r="T35">
-        <v>1</v>
-      </c>
-      <c r="U35">
-        <v>1</v>
+      <c r="T35" s="24">
+        <v>0</v>
+      </c>
+      <c r="U35" s="24">
+        <v>0</v>
       </c>
       <c r="V35">
         <v>1</v>
       </c>
-      <c r="W35" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ35" s="24"/>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG35" s="24"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>27</v>
       </c>
@@ -4051,23 +4021,20 @@
         <v>0</v>
       </c>
       <c r="S36">
-        <v>0</v>
-      </c>
-      <c r="T36">
-        <v>1</v>
-      </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-      <c r="V36">
-        <v>1</v>
-      </c>
-      <c r="W36" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ36" s="24"/>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T36" s="24">
+        <v>1</v>
+      </c>
+      <c r="U36" s="24">
+        <v>0</v>
+      </c>
+      <c r="V36" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG36" s="24"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>28</v>
       </c>
@@ -4116,21 +4083,18 @@
       <c r="S37">
         <v>1</v>
       </c>
-      <c r="T37">
-        <v>1</v>
-      </c>
-      <c r="U37">
-        <v>1</v>
-      </c>
-      <c r="V37">
-        <v>1</v>
-      </c>
-      <c r="W37" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ37" s="24"/>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T37" s="24">
+        <v>0</v>
+      </c>
+      <c r="U37" s="24">
+        <v>1</v>
+      </c>
+      <c r="V37" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG37" s="24"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>29</v>
       </c>
@@ -4176,23 +4140,20 @@
         <v>0</v>
       </c>
       <c r="S38">
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <v>1</v>
-      </c>
-      <c r="U38">
-        <v>0</v>
-      </c>
-      <c r="V38">
-        <v>1</v>
-      </c>
-      <c r="W38" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ38" s="24"/>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T38" s="24">
+        <v>1</v>
+      </c>
+      <c r="U38" s="24">
+        <v>0</v>
+      </c>
+      <c r="V38" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="24"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>30</v>
       </c>
@@ -4244,21 +4205,18 @@
       <c r="S39">
         <v>1</v>
       </c>
-      <c r="T39">
-        <v>1</v>
-      </c>
-      <c r="U39">
-        <v>1</v>
+      <c r="T39" s="24">
+        <v>1</v>
+      </c>
+      <c r="U39" s="24">
+        <v>0</v>
       </c>
       <c r="V39">
         <v>1</v>
       </c>
-      <c r="W39" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ39" s="24"/>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG39" s="24"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>31</v>
       </c>
@@ -4303,23 +4261,20 @@
         <v>0</v>
       </c>
       <c r="S40">
-        <v>0</v>
-      </c>
-      <c r="T40">
-        <v>1</v>
-      </c>
-      <c r="U40">
-        <v>0</v>
-      </c>
-      <c r="V40">
-        <v>1</v>
-      </c>
-      <c r="W40" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ40" s="24"/>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T40" s="24">
+        <v>1</v>
+      </c>
+      <c r="U40" s="24">
+        <v>0</v>
+      </c>
+      <c r="V40" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG40" s="24"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>32</v>
       </c>
@@ -4374,21 +4329,18 @@
       <c r="S41">
         <v>1</v>
       </c>
-      <c r="T41">
-        <v>1</v>
-      </c>
-      <c r="U41">
-        <v>1</v>
+      <c r="T41" s="24">
+        <v>1</v>
+      </c>
+      <c r="U41" s="24">
+        <v>0</v>
       </c>
       <c r="V41">
         <v>1</v>
       </c>
-      <c r="W41" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ41" s="24"/>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG41" s="24"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>33</v>
       </c>
@@ -4437,21 +4389,18 @@
       <c r="S42">
         <v>0</v>
       </c>
-      <c r="T42">
-        <v>0</v>
-      </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
-      <c r="V42">
-        <v>0</v>
-      </c>
-      <c r="W42" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ42" s="24"/>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T42" s="24">
+        <v>1</v>
+      </c>
+      <c r="U42" s="24">
+        <v>0</v>
+      </c>
+      <c r="V42" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="24"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>34</v>
       </c>
@@ -4497,21 +4446,18 @@
       <c r="S43">
         <v>1</v>
       </c>
-      <c r="T43">
-        <v>1</v>
-      </c>
-      <c r="U43">
-        <v>1</v>
-      </c>
-      <c r="V43">
-        <v>1</v>
-      </c>
-      <c r="W43" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ43" s="24"/>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T43" s="24">
+        <v>0</v>
+      </c>
+      <c r="U43" s="24">
+        <v>1</v>
+      </c>
+      <c r="V43" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG43" s="24"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>35</v>
       </c>
@@ -4522,17 +4468,17 @@
         <v>113</v>
       </c>
       <c r="G44" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H44" s="4"/>
       <c r="J44" s="27">
         <v>0.51</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="M44">
         <v>8</v>
@@ -4549,26 +4495,23 @@
       <c r="S44">
         <v>1</v>
       </c>
-      <c r="T44">
-        <v>1</v>
-      </c>
-      <c r="U44">
-        <v>1</v>
-      </c>
-      <c r="V44">
-        <v>1</v>
-      </c>
-      <c r="W44" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ44" s="24"/>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T44" s="24">
+        <v>0</v>
+      </c>
+      <c r="U44" s="24">
+        <v>1</v>
+      </c>
+      <c r="V44" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG44" s="24"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>36</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C45" s="4">
         <v>209</v>
@@ -4613,21 +4556,18 @@
       <c r="S45">
         <v>1</v>
       </c>
-      <c r="T45">
-        <v>1</v>
-      </c>
-      <c r="U45">
-        <v>1</v>
+      <c r="T45" s="24">
+        <v>1</v>
+      </c>
+      <c r="U45" s="24">
+        <v>0</v>
       </c>
       <c r="V45">
         <v>1</v>
       </c>
-      <c r="W45" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ45" s="24"/>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG45" s="24"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>37</v>
       </c>
@@ -4676,21 +4616,18 @@
       <c r="S46">
         <v>1</v>
       </c>
-      <c r="T46">
-        <v>1</v>
-      </c>
-      <c r="U46">
-        <v>1</v>
-      </c>
-      <c r="V46">
-        <v>1</v>
-      </c>
-      <c r="W46" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ46" s="24"/>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T46" s="24">
+        <v>0</v>
+      </c>
+      <c r="U46" s="24">
+        <v>1</v>
+      </c>
+      <c r="V46" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG46" s="24"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>38</v>
       </c>
@@ -4732,23 +4669,20 @@
         <v>0</v>
       </c>
       <c r="S47">
-        <v>0</v>
-      </c>
-      <c r="T47">
-        <v>1</v>
-      </c>
-      <c r="U47">
-        <v>0</v>
-      </c>
-      <c r="V47">
-        <v>1</v>
-      </c>
-      <c r="W47" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ47" s="24"/>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="T47" s="24">
+        <v>0</v>
+      </c>
+      <c r="U47" s="24">
+        <v>0</v>
+      </c>
+      <c r="V47" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG47" s="24"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>39</v>
       </c>
@@ -4800,26 +4734,23 @@
       <c r="S48">
         <v>1</v>
       </c>
-      <c r="T48">
-        <v>1</v>
-      </c>
-      <c r="U48">
-        <v>1</v>
-      </c>
-      <c r="V48">
-        <v>1</v>
-      </c>
-      <c r="W48" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ48" s="24"/>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="T48" s="24">
+        <v>0</v>
+      </c>
+      <c r="U48" s="24">
+        <v>1</v>
+      </c>
+      <c r="V48" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG48" s="24"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>40</v>
       </c>
       <c r="D49" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E49" t="s">
         <v>142</v>
@@ -4854,26 +4785,23 @@
       <c r="S49" s="8">
         <v>1</v>
       </c>
-      <c r="T49" s="8">
-        <v>1</v>
+      <c r="T49" s="24">
+        <v>0</v>
       </c>
       <c r="U49" s="8">
         <v>1</v>
       </c>
       <c r="V49" s="8">
-        <v>1</v>
-      </c>
-      <c r="W49" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ49" s="24"/>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="24"/>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E50" t="s">
         <v>142</v>
@@ -4909,26 +4837,23 @@
       <c r="S50" s="8">
         <v>1</v>
       </c>
-      <c r="T50" s="8">
-        <v>1</v>
+      <c r="T50" s="24">
+        <v>0</v>
       </c>
       <c r="U50" s="8">
         <v>1</v>
       </c>
       <c r="V50" s="8">
-        <v>1</v>
-      </c>
-      <c r="W50" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ50" s="24"/>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG50" s="24"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>42</v>
       </c>
       <c r="D51" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G51" t="s">
         <v>148</v>
@@ -4958,26 +4883,23 @@
       <c r="S51" s="8">
         <v>1</v>
       </c>
-      <c r="T51" s="8">
-        <v>1</v>
+      <c r="T51" s="24">
+        <v>0</v>
       </c>
       <c r="U51" s="8">
         <v>1</v>
       </c>
       <c r="V51" s="8">
-        <v>1</v>
-      </c>
-      <c r="W51" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ51" s="24"/>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="24"/>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G52" t="s">
         <v>148</v>
@@ -5007,35 +4929,32 @@
       <c r="S52" s="8">
         <v>1</v>
       </c>
-      <c r="T52" s="8">
-        <v>1</v>
+      <c r="T52" s="24">
+        <v>0</v>
       </c>
       <c r="U52" s="8">
         <v>1</v>
       </c>
       <c r="V52" s="8">
-        <v>1</v>
-      </c>
-      <c r="W52" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ52" s="24"/>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG52" s="24"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>44</v>
       </c>
       <c r="D53" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E53" t="s">
         <v>116</v>
       </c>
       <c r="F53" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G53" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H53" s="4"/>
       <c r="J53" s="27">
@@ -5054,7 +4973,7 @@
         <v>1</v>
       </c>
       <c r="O53" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="Q53" s="8">
         <v>0</v>
@@ -5065,35 +4984,32 @@
       <c r="S53" s="8">
         <v>1</v>
       </c>
-      <c r="T53" s="8">
-        <v>1</v>
+      <c r="T53" s="24">
+        <v>0</v>
       </c>
       <c r="U53" s="8">
         <v>1</v>
       </c>
       <c r="V53" s="8">
-        <v>1</v>
-      </c>
-      <c r="W53" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ53" s="24"/>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG53" s="24"/>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>45</v>
       </c>
       <c r="D54" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E54" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F54" t="s">
         <v>116</v>
       </c>
       <c r="G54" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H54" s="4"/>
       <c r="J54" s="27">
@@ -5120,35 +5036,32 @@
       <c r="S54" s="8">
         <v>1</v>
       </c>
-      <c r="T54" s="8">
-        <v>1</v>
+      <c r="T54" s="24">
+        <v>0</v>
       </c>
       <c r="U54" s="8">
         <v>1</v>
       </c>
       <c r="V54" s="8">
-        <v>1</v>
-      </c>
-      <c r="W54" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ54" s="24"/>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG54" s="24"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>46</v>
       </c>
       <c r="D55" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E55" t="s">
         <v>116</v>
       </c>
       <c r="F55" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G55" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H55" s="4"/>
       <c r="J55" s="27">
@@ -5175,35 +5088,32 @@
       <c r="S55" s="8">
         <v>1</v>
       </c>
-      <c r="T55" s="8">
-        <v>1</v>
+      <c r="T55" s="24">
+        <v>0</v>
       </c>
       <c r="U55" s="8">
         <v>1</v>
       </c>
       <c r="V55" s="8">
-        <v>1</v>
-      </c>
-      <c r="W55" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ55" s="24"/>
-    </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG55" s="24"/>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>47</v>
       </c>
       <c r="D56" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E56" t="s">
         <v>60</v>
       </c>
       <c r="F56" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G56" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H56" s="4"/>
       <c r="J56" s="27">
@@ -5230,35 +5140,32 @@
       <c r="S56" s="8">
         <v>1</v>
       </c>
-      <c r="T56" s="8">
-        <v>1</v>
+      <c r="T56" s="24">
+        <v>0</v>
       </c>
       <c r="U56" s="8">
         <v>1</v>
       </c>
       <c r="V56" s="8">
-        <v>1</v>
-      </c>
-      <c r="W56" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ56" s="24"/>
-    </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG56" s="24"/>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>48</v>
       </c>
       <c r="D57" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E57" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F57" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G57" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H57" s="4"/>
       <c r="J57" s="27">
@@ -5285,29 +5192,26 @@
       <c r="S57" s="8">
         <v>1</v>
       </c>
-      <c r="T57" s="8">
-        <v>1</v>
+      <c r="T57" s="24">
+        <v>0</v>
       </c>
       <c r="U57" s="8">
         <v>1</v>
       </c>
       <c r="V57" s="8">
-        <v>1</v>
-      </c>
-      <c r="W57" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ57" s="24"/>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG57" s="24"/>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58" s="24">
         <v>102</v>
       </c>
       <c r="D58" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G58" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H58" s="4"/>
       <c r="J58" s="27">
@@ -5334,8 +5238,8 @@
       <c r="S58" s="8">
         <v>0</v>
       </c>
-      <c r="T58" s="8">
-        <v>0</v>
+      <c r="T58" s="24">
+        <v>1</v>
       </c>
       <c r="U58" s="8">
         <v>0</v>
@@ -5343,17 +5247,14 @@
       <c r="V58" s="8">
         <v>0</v>
       </c>
-      <c r="W58" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ58" s="24"/>
-    </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG58" s="24"/>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A59" s="24">
         <v>103</v>
       </c>
       <c r="D59" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G59" t="s">
         <v>101</v>
@@ -5383,7 +5284,7 @@
       <c r="S59" s="8">
         <v>0</v>
       </c>
-      <c r="T59" s="8">
+      <c r="T59" s="24">
         <v>0</v>
       </c>
       <c r="U59" s="8">
@@ -5392,26 +5293,23 @@
       <c r="V59" s="8">
         <v>0</v>
       </c>
-      <c r="W59" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ59" s="24"/>
-    </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG59" s="24"/>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A60" s="24">
         <v>104</v>
       </c>
       <c r="D60" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E60" t="s">
         <v>149</v>
       </c>
       <c r="F60" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G60" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H60" s="4"/>
       <c r="J60" s="27">
@@ -5438,8 +5336,8 @@
       <c r="S60" s="8">
         <v>0</v>
       </c>
-      <c r="T60" s="8">
-        <v>0</v>
+      <c r="T60" s="24">
+        <v>1</v>
       </c>
       <c r="U60" s="8">
         <v>0</v>
@@ -5447,26 +5345,23 @@
       <c r="V60" s="8">
         <v>0</v>
       </c>
-      <c r="W60" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ60" s="24"/>
-    </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG60" s="24"/>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A61" s="24">
         <v>105</v>
       </c>
       <c r="D61" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E61" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="F61" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G61" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H61" s="4"/>
       <c r="J61" s="27">
@@ -5493,8 +5388,8 @@
       <c r="S61" s="8">
         <v>0</v>
       </c>
-      <c r="T61" s="8">
-        <v>0</v>
+      <c r="T61" s="24">
+        <v>1</v>
       </c>
       <c r="U61" s="8">
         <v>0</v>
@@ -5502,20 +5397,17 @@
       <c r="V61" s="8">
         <v>0</v>
       </c>
-      <c r="W61" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ61" s="24"/>
-    </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG61" s="24"/>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A62" s="24">
         <v>106</v>
       </c>
       <c r="D62" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G62" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H62" s="4"/>
       <c r="J62" s="27">
@@ -5542,8 +5434,8 @@
       <c r="S62" s="8">
         <v>0</v>
       </c>
-      <c r="T62" s="8">
-        <v>0</v>
+      <c r="T62" s="24">
+        <v>1</v>
       </c>
       <c r="U62" s="8">
         <v>0</v>
@@ -5551,26 +5443,23 @@
       <c r="V62" s="8">
         <v>0</v>
       </c>
-      <c r="W62" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ62" s="24"/>
-    </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG62" s="24"/>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A63" s="24">
         <v>107</v>
       </c>
       <c r="D63" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E63" t="s">
         <v>30</v>
       </c>
       <c r="F63" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G63" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H63" s="4"/>
       <c r="J63" s="27">
@@ -5597,8 +5486,8 @@
       <c r="S63" s="8">
         <v>0</v>
       </c>
-      <c r="T63" s="8">
-        <v>0</v>
+      <c r="T63" s="24">
+        <v>1</v>
       </c>
       <c r="U63" s="8">
         <v>0</v>
@@ -5606,26 +5495,23 @@
       <c r="V63" s="8">
         <v>0</v>
       </c>
-      <c r="W63" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ63" s="24"/>
-    </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG63" s="24"/>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A64" s="24">
         <v>108</v>
       </c>
       <c r="D64" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E64" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F64" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G64" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J64" s="27">
         <v>3.24</v>
@@ -5651,8 +5537,8 @@
       <c r="S64" s="8">
         <v>0</v>
       </c>
-      <c r="T64" s="8">
-        <v>0</v>
+      <c r="T64" s="24">
+        <v>1</v>
       </c>
       <c r="U64" s="8">
         <v>0</v>
@@ -5660,20 +5546,17 @@
       <c r="V64" s="8">
         <v>0</v>
       </c>
-      <c r="W64" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ64" s="24"/>
-    </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG64" s="24"/>
+    </row>
+    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A65" s="24">
         <v>109</v>
       </c>
       <c r="D65" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G65" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J65" s="27">
         <v>3.81</v>
@@ -5699,8 +5582,8 @@
       <c r="S65" s="8">
         <v>0</v>
       </c>
-      <c r="T65" s="8">
-        <v>0</v>
+      <c r="T65" s="24">
+        <v>1</v>
       </c>
       <c r="U65" s="8">
         <v>0</v>
@@ -5708,26 +5591,23 @@
       <c r="V65" s="8">
         <v>0</v>
       </c>
-      <c r="W65" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ65" s="24"/>
-    </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG65" s="24"/>
+    </row>
+    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A66" s="24">
         <v>110</v>
       </c>
       <c r="D66" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E66" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F66" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G66" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J66" s="27">
         <v>0.69</v>
@@ -5753,8 +5633,8 @@
       <c r="S66" s="8">
         <v>0</v>
       </c>
-      <c r="T66" s="8">
-        <v>0</v>
+      <c r="T66" s="24">
+        <v>1</v>
       </c>
       <c r="U66" s="8">
         <v>0</v>
@@ -5762,26 +5642,23 @@
       <c r="V66" s="8">
         <v>0</v>
       </c>
-      <c r="W66" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ66" s="24"/>
-    </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG66" s="24"/>
+    </row>
+    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A67" s="24">
         <v>111</v>
       </c>
       <c r="D67" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E67" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F67" t="s">
         <v>119</v>
       </c>
       <c r="G67" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J67" s="27">
         <v>16.190000000000001</v>
@@ -5807,8 +5684,8 @@
       <c r="S67" s="8">
         <v>0</v>
       </c>
-      <c r="T67" s="8">
-        <v>0</v>
+      <c r="T67" s="24">
+        <v>1</v>
       </c>
       <c r="U67" s="8">
         <v>0</v>
@@ -5816,26 +5693,23 @@
       <c r="V67" s="8">
         <v>0</v>
       </c>
-      <c r="W67" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ67" s="24"/>
-    </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG67" s="24"/>
+    </row>
+    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A68" s="24">
         <v>112</v>
       </c>
       <c r="D68" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E68" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F68" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G68" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J68" s="27">
         <v>3.25</v>
@@ -5862,8 +5736,8 @@
       <c r="S68" s="8">
         <v>0</v>
       </c>
-      <c r="T68" s="8">
-        <v>0</v>
+      <c r="T68" s="24">
+        <v>1</v>
       </c>
       <c r="U68" s="8">
         <v>0</v>
@@ -5871,28 +5745,25 @@
       <c r="V68" s="8">
         <v>0</v>
       </c>
-      <c r="W68" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ68" s="24"/>
-    </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG68" s="24"/>
+    </row>
+    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A69" s="24">
         <v>113</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E69" t="s">
         <v>142</v>
       </c>
       <c r="F69" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G69" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H69" s="4"/>
       <c r="J69" s="27">
@@ -5920,8 +5791,8 @@
       <c r="S69" s="8">
         <v>0</v>
       </c>
-      <c r="T69" s="8">
-        <v>0</v>
+      <c r="T69" s="24">
+        <v>1</v>
       </c>
       <c r="U69" s="8">
         <v>0</v>
@@ -5929,28 +5800,25 @@
       <c r="V69" s="8">
         <v>0</v>
       </c>
-      <c r="W69" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ69" s="24"/>
-    </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG69" s="24"/>
+    </row>
+    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A70" s="24">
         <v>115</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>141</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -5979,8 +5847,8 @@
       <c r="S70" s="8">
         <v>0</v>
       </c>
-      <c r="T70" s="8">
-        <v>0</v>
+      <c r="T70" s="24">
+        <v>1</v>
       </c>
       <c r="U70" s="8">
         <v>0</v>
@@ -5988,22 +5856,19 @@
       <c r="V70" s="8">
         <v>0</v>
       </c>
-      <c r="W70" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ70" s="24"/>
-    </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG70" s="24"/>
+    </row>
+    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A71" s="24">
         <v>116</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H71" s="4"/>
       <c r="J71" s="27">
@@ -6031,8 +5896,8 @@
       <c r="S71" s="8">
         <v>0</v>
       </c>
-      <c r="T71" s="8">
-        <v>0</v>
+      <c r="T71" s="24">
+        <v>1</v>
       </c>
       <c r="U71" s="8">
         <v>0</v>
@@ -6040,22 +5905,19 @@
       <c r="V71" s="8">
         <v>0</v>
       </c>
-      <c r="W71" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ71" s="24"/>
-    </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG71" s="24"/>
+    </row>
+    <row r="72" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A72" s="24">
         <v>117</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H72" s="4"/>
       <c r="J72" s="27">
@@ -6083,8 +5945,8 @@
       <c r="S72" s="8">
         <v>0</v>
       </c>
-      <c r="T72" s="8">
-        <v>0</v>
+      <c r="T72" s="24">
+        <v>1</v>
       </c>
       <c r="U72" s="8">
         <v>0</v>
@@ -6092,22 +5954,19 @@
       <c r="V72" s="8">
         <v>0</v>
       </c>
-      <c r="W72" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ72" s="24"/>
-    </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG72" s="24"/>
+    </row>
+    <row r="73" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A73" s="24">
         <v>118</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
@@ -6136,28 +5995,25 @@
       <c r="S73" s="8">
         <v>1</v>
       </c>
-      <c r="T73" s="8">
-        <v>1</v>
+      <c r="T73" s="24">
+        <v>0</v>
       </c>
       <c r="U73" s="8">
         <v>1</v>
       </c>
       <c r="V73" s="8">
-        <v>1</v>
-      </c>
-      <c r="W73" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ73" s="24"/>
-    </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG73" s="24"/>
+    </row>
+    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>119</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E74" t="s">
         <v>28</v>
@@ -6166,7 +6022,7 @@
         <v>168</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
@@ -6195,37 +6051,34 @@
       <c r="S74" s="8">
         <v>1</v>
       </c>
-      <c r="T74" s="8">
-        <v>1</v>
+      <c r="T74" s="24">
+        <v>0</v>
       </c>
       <c r="U74" s="8">
         <v>1</v>
       </c>
       <c r="V74" s="8">
-        <v>1</v>
-      </c>
-      <c r="W74" s="24">
-        <v>0</v>
-      </c>
-      <c r="AJ74" s="24"/>
-    </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AG74" s="24"/>
+    </row>
+    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>120</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E75" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F75" t="s">
         <v>79</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -6254,8 +6107,8 @@
       <c r="S75" s="8">
         <v>0</v>
       </c>
-      <c r="T75" s="8">
-        <v>0</v>
+      <c r="T75" s="24">
+        <v>1</v>
       </c>
       <c r="U75" s="8">
         <v>0</v>
@@ -6263,12 +6116,9 @@
       <c r="V75" s="8">
         <v>0</v>
       </c>
-      <c r="W75" s="24">
-        <v>1</v>
-      </c>
-      <c r="AJ75" s="24"/>
-    </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG75" s="24"/>
+    </row>
+    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -6278,12 +6128,9 @@
       <c r="P76" s="19"/>
       <c r="Q76" s="8"/>
       <c r="R76" s="8"/>
-      <c r="S76" s="8"/>
       <c r="T76" s="8"/>
-      <c r="U76" s="8"/>
-      <c r="W76" s="8"/>
-    </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -6293,12 +6140,9 @@
       <c r="P77" s="19"/>
       <c r="Q77" s="8"/>
       <c r="R77" s="8"/>
-      <c r="S77" s="8"/>
       <c r="T77" s="8"/>
-      <c r="U77" s="8"/>
-      <c r="W77" s="8"/>
-    </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -6308,12 +6152,9 @@
       <c r="P78" s="19"/>
       <c r="Q78" s="8"/>
       <c r="R78" s="8"/>
-      <c r="S78" s="8"/>
       <c r="T78" s="8"/>
-      <c r="U78" s="8"/>
-      <c r="W78" s="8"/>
-    </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -6321,12 +6162,9 @@
       <c r="P79" s="19"/>
       <c r="Q79" s="8"/>
       <c r="R79" s="8"/>
-      <c r="S79" s="8"/>
       <c r="T79" s="8"/>
-      <c r="U79" s="8"/>
-      <c r="W79" s="8"/>
-    </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -6334,12 +6172,9 @@
       <c r="P80" s="19"/>
       <c r="Q80" s="8"/>
       <c r="R80" s="8"/>
-      <c r="S80" s="8"/>
       <c r="T80" s="8"/>
-      <c r="U80" s="8"/>
-      <c r="W80" s="8"/>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -6347,12 +6182,9 @@
       <c r="P81" s="19"/>
       <c r="Q81" s="8"/>
       <c r="R81" s="8"/>
-      <c r="S81" s="8"/>
       <c r="T81" s="8"/>
-      <c r="U81" s="8"/>
-      <c r="W81" s="8"/>
-    </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -6360,12 +6192,9 @@
       <c r="P82" s="19"/>
       <c r="Q82" s="8"/>
       <c r="R82" s="8"/>
-      <c r="S82" s="8"/>
       <c r="T82" s="8"/>
-      <c r="U82" s="8"/>
-      <c r="W82" s="8"/>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -6373,12 +6202,9 @@
       <c r="P83" s="19"/>
       <c r="Q83" s="8"/>
       <c r="R83" s="8"/>
-      <c r="S83" s="8"/>
       <c r="T83" s="8"/>
-      <c r="U83" s="8"/>
-      <c r="W83" s="8"/>
-    </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -6386,12 +6212,9 @@
       <c r="P84" s="19"/>
       <c r="Q84" s="8"/>
       <c r="R84" s="8"/>
-      <c r="S84" s="8"/>
       <c r="T84" s="8"/>
-      <c r="U84" s="8"/>
-      <c r="W84" s="8"/>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -6399,12 +6222,9 @@
       <c r="P85" s="19"/>
       <c r="Q85" s="8"/>
       <c r="R85" s="8"/>
-      <c r="S85" s="8"/>
       <c r="T85" s="8"/>
-      <c r="U85" s="8"/>
-      <c r="W85" s="8"/>
-    </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -6413,12 +6233,9 @@
       <c r="P86" s="19"/>
       <c r="Q86" s="8"/>
       <c r="R86" s="8"/>
-      <c r="S86" s="8"/>
       <c r="T86" s="8"/>
-      <c r="U86" s="8"/>
-      <c r="W86" s="8"/>
-    </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -6427,12 +6244,9 @@
       <c r="P87" s="19"/>
       <c r="Q87" s="8"/>
       <c r="R87" s="8"/>
-      <c r="S87" s="8"/>
       <c r="T87" s="8"/>
-      <c r="U87" s="8"/>
-      <c r="W87" s="8"/>
-    </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -6443,12 +6257,9 @@
       <c r="P88" s="19"/>
       <c r="Q88" s="8"/>
       <c r="R88" s="8"/>
-      <c r="S88" s="8"/>
       <c r="T88" s="8"/>
-      <c r="U88" s="8"/>
-      <c r="W88" s="8"/>
-    </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -6458,12 +6269,9 @@
       <c r="P89" s="19"/>
       <c r="Q89" s="8"/>
       <c r="R89" s="8"/>
-      <c r="S89" s="8"/>
       <c r="T89" s="8"/>
-      <c r="U89" s="8"/>
-      <c r="W89" s="8"/>
-    </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -6473,34 +6281,31 @@
       <c r="P90" s="19"/>
       <c r="Q90" s="8"/>
       <c r="R90" s="8"/>
-      <c r="S90" s="8"/>
       <c r="T90" s="8"/>
-      <c r="U90" s="8"/>
-      <c r="W90" s="8"/>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J94" s="5"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:W75" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A9:V75" xr:uid="{7020DE52-0B61-9644-93F1-364D58F6F3FB}"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I89:I91" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
@@ -6524,27 +6329,27 @@
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="6" width="32.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="6" width="32.5" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6569,7 +6374,7 @@
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -6616,7 +6421,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>37</v>
@@ -6636,7 +6441,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>44</v>
@@ -6659,7 +6464,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>48</v>
@@ -6682,7 +6487,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -6706,7 +6511,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -6729,7 +6534,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -6753,7 +6558,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>62</v>
@@ -6773,7 +6578,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>68</v>
@@ -6793,7 +6598,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>90</v>
       </c>
@@ -6816,7 +6621,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>96</v>
       </c>
@@ -6839,7 +6644,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>103</v>
       </c>
@@ -6855,7 +6660,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C21" s="4" t="s">
         <v>98</v>
       </c>
@@ -6866,7 +6671,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C22" s="4" t="s">
         <v>110</v>
       </c>
@@ -6877,7 +6682,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="4" t="s">
         <v>26</v>
       </c>
@@ -6898,7 +6703,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C24" s="4" t="s">
         <v>34</v>
       </c>
@@ -6917,7 +6722,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>18</v>
       </c>
@@ -6941,7 +6746,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -6951,7 +6756,7 @@
       <c r="J26"/>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -6961,7 +6766,7 @@
       <c r="J27"/>
       <c r="K27"/>
     </row>
-    <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>175</v>
       </c>
@@ -7026,20 +6831,20 @@
         <v>180</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="24">
         <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" s="4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I29"/>
       <c r="J29" s="27"/>
@@ -7063,21 +6868,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="24">
         <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E30" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F30" t="s">
         <v>150</v>
       </c>
       <c r="G30" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H30" s="4"/>
       <c r="J30" s="27"/>
@@ -7103,7 +6908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -7113,7 +6918,7 @@
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -7123,7 +6928,7 @@
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -7133,7 +6938,7 @@
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -7143,7 +6948,7 @@
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -7153,7 +6958,7 @@
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -7163,7 +6968,7 @@
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -7173,7 +6978,7 @@
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -7183,7 +6988,7 @@
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -7193,7 +6998,7 @@
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -7203,7 +7008,7 @@
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -7213,129 +7018,129 @@
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G42" s="4"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G43" s="4"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G44" s="4"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G45" s="4"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G46" s="4"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G47" s="4"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G48" s="4"/>
       <c r="J48"/>
       <c r="K48"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G49" s="4"/>
       <c r="J49"/>
       <c r="K49"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G50" s="4"/>
       <c r="J50"/>
       <c r="K50"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G51" s="4"/>
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G52" s="4"/>
       <c r="J52"/>
       <c r="K52"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G53" s="4"/>
       <c r="J53"/>
       <c r="K53"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G54" s="4"/>
       <c r="J54"/>
       <c r="K54"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G55" s="4"/>
       <c r="J55"/>
       <c r="K55"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G56" s="4"/>
       <c r="J56"/>
       <c r="K56"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G57" s="4"/>
       <c r="J57"/>
       <c r="K57"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G58" s="4"/>
       <c r="J58"/>
       <c r="K58"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J59"/>
       <c r="K59"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J60"/>
       <c r="K60"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J61"/>
       <c r="K61"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J62"/>
       <c r="K62"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J63"/>
       <c r="K63"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="G64" s="4"/>
       <c r="O64" s="4"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="O65" s="4"/>
     </row>
-    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="J66" s="8"/>
       <c r="K66" s="5"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="F67" s="4"/>
@@ -7343,119 +7148,119 @@
       <c r="I67" s="4"/>
       <c r="O67" s="4"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="G68" s="4"/>
       <c r="I68" s="4"/>
       <c r="O68" s="4"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="O70" s="4"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="O71" s="4"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="O72" s="4"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="O73" s="4"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="O74" s="4"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="G75" s="4"/>
       <c r="O75" s="4"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="G76" s="4"/>
       <c r="O76" s="4"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="G77" s="4"/>
       <c r="O77" s="4"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="G78" s="4"/>
       <c r="O78" s="4"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="G79" s="4"/>
       <c r="O79" s="4"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="G80" s="4"/>
       <c r="O80" s="4"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="G81" s="4"/>
       <c r="O81" s="4"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="O82" s="4"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="G83" s="4"/>
       <c r="O83" s="4"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="G84" s="4"/>
       <c r="O84" s="4"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="G85" s="4"/>
@@ -7464,7 +7269,7 @@
       <c r="K85" s="8"/>
       <c r="O85" s="4"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="G86" s="4"/>
@@ -7473,7 +7278,7 @@
       <c r="K86" s="8"/>
       <c r="O86" s="4"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="G87" s="4"/>
@@ -7482,7 +7287,7 @@
       <c r="K87" s="8"/>
       <c r="O87" s="4"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -7503,18 +7308,18 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="3" max="3" width="15.6640625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>175</v>
       </c>
@@ -7522,13 +7327,13 @@
         <v>17</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -7542,7 +7347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -7550,13 +7355,13 @@
         <v>142</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -7570,7 +7375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -7584,7 +7389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -7598,7 +7403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>7</v>
       </c>
@@ -7606,13 +7411,13 @@
         <v>79</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>8</v>
       </c>
@@ -7626,7 +7431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>14</v>
       </c>
@@ -7640,7 +7445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>15</v>
       </c>
@@ -7654,7 +7459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>16</v>
       </c>
@@ -7668,7 +7473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>17</v>
       </c>
@@ -7682,7 +7487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>18</v>
       </c>
@@ -7696,7 +7501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>19</v>
       </c>
@@ -7710,7 +7515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>22</v>
       </c>
@@ -7724,7 +7529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>25</v>
       </c>
@@ -7738,7 +7543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>27</v>
       </c>
@@ -7752,7 +7557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>29</v>
       </c>
@@ -7766,7 +7571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>30</v>
       </c>
@@ -7780,7 +7585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>31</v>
       </c>
@@ -7794,7 +7599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>32</v>
       </c>
@@ -7808,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>33</v>
       </c>
@@ -7822,7 +7627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>36</v>
       </c>
@@ -7836,12 +7641,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>102</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C24" s="8">
         <v>3737</v>
@@ -7850,26 +7655,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>104</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>105</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C26" s="8">
         <v>3994</v>
@@ -7878,12 +7683,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>106</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C27" s="8">
         <v>10431</v>
@@ -7892,12 +7697,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>107</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C28" s="8">
         <v>4394</v>
@@ -7906,40 +7711,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>108</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>109</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>110</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C31" s="8">
         <v>5321</v>
@@ -7948,12 +7753,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>111</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C32" s="8">
         <v>8735</v>
@@ -7962,12 +7767,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>112</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C33" s="8">
         <v>10420</v>
@@ -7976,12 +7781,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>113</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C34" s="8">
         <v>10421</v>
@@ -7990,12 +7795,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>115</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C35" s="8">
         <v>4071</v>
@@ -8004,12 +7809,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>116</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C36" s="8">
         <v>10456</v>
@@ -8018,12 +7823,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>117</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C37" s="8">
         <v>10490</v>
@@ -8032,12 +7837,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>120</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C38" s="8">
         <v>9870</v>

</xml_diff>

<commit_message>
Update representative links for cmp analysis
Also removed project 40
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A9B8A-B71B-43FF-A594-E14C7B8FE9C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD832FB-5B32-4323-A9FC-FD3C4F06A321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proj Attributes and Scenarios" sheetId="1" r:id="rId1"/>
@@ -13,16 +13,16 @@
     <sheet name="CMP_Rep_Link" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$60:$O$80</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$R$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$R$70</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="267">
   <si>
     <t>Cost</t>
   </si>
@@ -820,6 +820,9 @@
   </si>
   <si>
     <t>Completed 2015</t>
+  </si>
+  <si>
+    <t>Kyle: this project doesn't make sense and is currently coded along the entire LRT route</t>
   </si>
 </sst>
 </file>
@@ -2072,13 +2075,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC90"/>
+  <dimension ref="A1:AC89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="D64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3919,22 +3922,23 @@
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E44" t="s">
         <v>141</v>
       </c>
       <c r="F44" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G44" t="s">
         <v>147</v>
       </c>
+      <c r="H44" s="4"/>
       <c r="J44" s="26">
-        <v>19.809999999999999</v>
+        <v>3.88</v>
       </c>
       <c r="K44" s="8">
         <v>0</v>
@@ -3943,10 +3947,10 @@
         <v>2</v>
       </c>
       <c r="M44" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N44" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q44" s="8">
         <v>0</v>
@@ -3959,23 +3963,17 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>182</v>
-      </c>
-      <c r="E45" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="G45" t="s">
         <v>147</v>
       </c>
       <c r="H45" s="4"/>
       <c r="J45" s="26">
-        <v>3.88</v>
+        <v>2.68</v>
       </c>
       <c r="K45" s="8">
         <v>0</v>
@@ -3984,10 +3982,10 @@
         <v>2</v>
       </c>
       <c r="M45" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N45" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q45" s="8">
         <v>0</v>
@@ -4000,17 +3998,19 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G46" t="s">
         <v>147</v>
       </c>
-      <c r="H46" s="4"/>
+      <c r="H46" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="J46" s="26">
-        <v>2.68</v>
+        <v>5.36</v>
       </c>
       <c r="K46" s="8">
         <v>0</v>
@@ -4028,38 +4028,47 @@
         <v>0</v>
       </c>
       <c r="R46" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S46" s="8"/>
       <c r="AC46" s="24"/>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="E47" t="s">
+        <v>116</v>
+      </c>
+      <c r="F47" t="s">
+        <v>186</v>
       </c>
       <c r="G47" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J47" s="26">
-        <v>5.36</v>
-      </c>
-      <c r="K47" s="8">
-        <v>0</v>
-      </c>
-      <c r="L47" s="8">
+        <v>2.95</v>
+      </c>
+      <c r="K47" s="4">
+        <v>1</v>
+      </c>
+      <c r="L47" s="4">
         <v>2</v>
       </c>
       <c r="M47" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N47" s="8">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="O47" t="s">
+        <v>188</v>
       </c>
       <c r="Q47" s="8">
         <v>0</v>
@@ -4072,40 +4081,37 @@
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E48" t="s">
+        <v>190</v>
+      </c>
+      <c r="F48" t="s">
         <v>116</v>
       </c>
-      <c r="F48" t="s">
-        <v>186</v>
-      </c>
       <c r="G48" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H48" s="4" t="s">
         <v>252</v>
       </c>
       <c r="J48" s="26">
-        <v>2.95</v>
+        <v>5.03</v>
       </c>
       <c r="K48" s="4">
         <v>1</v>
       </c>
       <c r="L48" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M48" s="8">
         <v>1</v>
       </c>
       <c r="N48" s="8">
         <v>1</v>
-      </c>
-      <c r="O48" t="s">
-        <v>188</v>
       </c>
       <c r="Q48" s="8">
         <v>0</v>
@@ -4118,16 +4124,16 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E49" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="F49" t="s">
-        <v>116</v>
+        <v>193</v>
       </c>
       <c r="G49" t="s">
         <v>191</v>
@@ -4136,7 +4142,7 @@
         <v>252</v>
       </c>
       <c r="J49" s="26">
-        <v>5.03</v>
+        <v>7.61</v>
       </c>
       <c r="K49" s="4">
         <v>1</v>
@@ -4161,16 +4167,16 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="E50" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="F50" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G50" t="s">
         <v>191</v>
@@ -4179,7 +4185,7 @@
         <v>252</v>
       </c>
       <c r="J50" s="26">
-        <v>7.61</v>
+        <v>2.93</v>
       </c>
       <c r="K50" s="4">
         <v>1</v>
@@ -4204,31 +4210,31 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A51" s="4">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E51" t="s">
-        <v>60</v>
+        <v>197</v>
       </c>
       <c r="F51" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G51" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>252</v>
       </c>
       <c r="J51" s="26">
-        <v>2.93</v>
+        <v>0.78</v>
       </c>
       <c r="K51" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L51" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" s="8">
         <v>1</v>
@@ -4246,67 +4252,59 @@
       <c r="AC51" s="24"/>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A52" s="4">
-        <v>48</v>
+      <c r="A52" s="24">
+        <v>102</v>
       </c>
       <c r="D52" t="s">
-        <v>196</v>
-      </c>
-      <c r="E52" t="s">
-        <v>197</v>
-      </c>
-      <c r="F52" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G52" t="s">
         <v>187</v>
       </c>
-      <c r="H52" s="4" t="s">
-        <v>252</v>
-      </c>
+      <c r="H52" s="4"/>
       <c r="J52" s="26">
-        <v>0.78</v>
+        <v>0.23</v>
       </c>
       <c r="K52" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52" s="4">
-        <v>1</v>
-      </c>
-      <c r="M52" s="8">
-        <v>1</v>
-      </c>
-      <c r="N52" s="8">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="M52">
+        <v>8</v>
+      </c>
+      <c r="N52">
+        <v>8</v>
       </c>
       <c r="Q52" s="8">
         <v>0</v>
       </c>
       <c r="R52" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S52" s="8"/>
       <c r="AC52" s="24"/>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A53" s="24">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D53" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G53" t="s">
-        <v>187</v>
+        <v>101</v>
       </c>
       <c r="H53" s="4"/>
       <c r="J53" s="26">
-        <v>0.23</v>
-      </c>
-      <c r="K53" s="4">
-        <v>1</v>
-      </c>
-      <c r="L53" s="4">
-        <v>2</v>
+        <v>0.41</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
       </c>
       <c r="M53">
         <v>8</v>
@@ -4325,29 +4323,35 @@
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A54" s="24">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D54" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="E54" t="s">
+        <v>148</v>
+      </c>
+      <c r="F54" t="s">
+        <v>204</v>
       </c>
       <c r="G54" t="s">
-        <v>101</v>
+        <v>187</v>
       </c>
       <c r="H54" s="4"/>
       <c r="J54" s="26">
-        <v>0.41</v>
+        <v>4.97</v>
       </c>
       <c r="K54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M54">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N54">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="Q54" s="8">
         <v>0</v>
@@ -4360,35 +4364,35 @@
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A55" s="24">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E55" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="F55" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G55" t="s">
         <v>187</v>
       </c>
       <c r="H55" s="4"/>
       <c r="J55" s="26">
-        <v>4.97</v>
+        <v>6.28</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L55">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q55" s="8">
         <v>0</v>
@@ -4401,35 +4405,29 @@
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A56" s="24">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
-      </c>
-      <c r="E56" t="s">
-        <v>206</v>
-      </c>
-      <c r="F56" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G56" t="s">
         <v>187</v>
       </c>
       <c r="H56" s="4"/>
       <c r="J56" s="26">
-        <v>6.28</v>
+        <v>0.05</v>
       </c>
       <c r="K56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L56">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M56">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N56">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q56" s="8">
         <v>0</v>
@@ -4442,29 +4440,35 @@
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A57" s="24">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="E57" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" t="s">
+        <v>210</v>
       </c>
       <c r="G57" t="s">
         <v>187</v>
       </c>
       <c r="H57" s="4"/>
       <c r="J57" s="26">
-        <v>0.05</v>
+        <v>0.49</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L57">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M57">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N57">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q57" s="8">
         <v>0</v>
@@ -4477,34 +4481,33 @@
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A58" s="24">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="E58" t="s">
-        <v>30</v>
+        <v>216</v>
       </c>
       <c r="F58" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="G58" t="s">
         <v>187</v>
       </c>
-      <c r="H58" s="4"/>
       <c r="J58" s="26">
-        <v>0.49</v>
-      </c>
-      <c r="K58">
-        <v>4</v>
-      </c>
-      <c r="L58">
-        <v>6</v>
-      </c>
-      <c r="M58">
+        <v>0.69</v>
+      </c>
+      <c r="K58" s="5">
         <v>3</v>
       </c>
-      <c r="N58">
+      <c r="L58" s="5">
+        <v>5</v>
+      </c>
+      <c r="M58" s="8">
+        <v>3</v>
+      </c>
+      <c r="N58" s="8">
         <v>3</v>
       </c>
       <c r="Q58" s="8">
@@ -4518,34 +4521,34 @@
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A59" s="24">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D59" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E59" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F59" t="s">
-        <v>217</v>
+        <v>119</v>
       </c>
       <c r="G59" t="s">
         <v>187</v>
       </c>
       <c r="J59" s="26">
-        <v>0.69</v>
-      </c>
-      <c r="K59" s="5">
-        <v>3</v>
-      </c>
-      <c r="L59" s="5">
-        <v>5</v>
-      </c>
-      <c r="M59" s="8">
-        <v>3</v>
-      </c>
-      <c r="N59" s="8">
-        <v>3</v>
+        <v>16.190000000000001</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>4</v>
+      </c>
+      <c r="M59">
+        <v>4</v>
+      </c>
+      <c r="N59">
+        <v>4</v>
       </c>
       <c r="Q59" s="8">
         <v>0</v>
@@ -4558,35 +4561,36 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A60" s="24">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D60" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E60" t="s">
+        <v>221</v>
+      </c>
+      <c r="F60" t="s">
         <v>219</v>
-      </c>
-      <c r="F60" t="s">
-        <v>119</v>
       </c>
       <c r="G60" t="s">
         <v>187</v>
       </c>
       <c r="J60" s="26">
-        <v>16.190000000000001</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
+        <v>3.25</v>
+      </c>
+      <c r="K60" s="5">
+        <v>0</v>
+      </c>
+      <c r="L60" s="5">
+        <v>2</v>
+      </c>
+      <c r="M60" s="8">
         <v>4</v>
       </c>
-      <c r="M60">
+      <c r="N60" s="8">
         <v>4</v>
       </c>
-      <c r="N60">
-        <v>4</v>
-      </c>
+      <c r="P60" s="19"/>
       <c r="Q60" s="8">
         <v>0</v>
       </c>
@@ -4598,34 +4602,37 @@
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A61" s="24">
-        <v>112</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
       <c r="D61" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E61" t="s">
-        <v>221</v>
+        <v>141</v>
       </c>
       <c r="F61" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="G61" t="s">
         <v>187</v>
       </c>
+      <c r="H61" s="4"/>
       <c r="J61" s="26">
-        <v>3.25</v>
-      </c>
-      <c r="K61" s="5">
-        <v>0</v>
-      </c>
-      <c r="L61" s="5">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="K61" s="8">
+        <v>0</v>
+      </c>
+      <c r="L61" s="8">
         <v>2</v>
       </c>
       <c r="M61" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N61" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P61" s="19"/>
       <c r="Q61" s="8">
@@ -4639,25 +4646,26 @@
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A62" s="24">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
-      <c r="D62" t="s">
-        <v>222</v>
-      </c>
-      <c r="E62" t="s">
-        <v>141</v>
-      </c>
-      <c r="F62" t="s">
-        <v>223</v>
-      </c>
-      <c r="G62" t="s">
+      <c r="D62" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>187</v>
       </c>
       <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
       <c r="J62" s="26">
-        <v>4.8499999999999996</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K62" s="8">
         <v>0</v>
@@ -4666,10 +4674,10 @@
         <v>2</v>
       </c>
       <c r="M62" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N62" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P62" s="19"/>
       <c r="Q62" s="8">
@@ -4683,26 +4691,21 @@
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A63" s="24">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>140</v>
+        <v>228</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
+      <c r="H63" s="21" t="s">
+        <v>252</v>
+      </c>
       <c r="J63" s="26">
-        <v>0.28999999999999998</v>
+        <v>0.23</v>
       </c>
       <c r="K63" s="8">
         <v>0</v>
@@ -4711,29 +4714,29 @@
         <v>2</v>
       </c>
       <c r="M63" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N63" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P63" s="19"/>
       <c r="Q63" s="8">
         <v>0</v>
       </c>
       <c r="R63" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S63" s="8"/>
       <c r="AC63" s="24"/>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A64" s="24">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>187</v>
@@ -4742,7 +4745,7 @@
         <v>252</v>
       </c>
       <c r="J64" s="26">
-        <v>0.23</v>
+        <v>0.42</v>
       </c>
       <c r="K64" s="8">
         <v>0</v>
@@ -4768,21 +4771,20 @@
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A65" s="24">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H65" s="21" t="s">
-        <v>252</v>
-      </c>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
       <c r="J65" s="26">
-        <v>0.42</v>
+        <v>4.41</v>
       </c>
       <c r="K65" s="8">
         <v>0</v>
@@ -4794,7 +4796,7 @@
         <v>7</v>
       </c>
       <c r="N65" s="8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P65" s="19"/>
       <c r="Q65" s="8">
@@ -4807,37 +4809,45 @@
       <c r="AC65" s="24"/>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A66" s="24">
-        <v>118</v>
+      <c r="A66" s="4">
+        <v>119</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="E66" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" t="s">
+        <v>167</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H66" s="4"/>
+      <c r="H66" s="21" t="s">
+        <v>252</v>
+      </c>
       <c r="I66" s="4"/>
       <c r="J66" s="26">
-        <v>4.41</v>
+        <v>2.57</v>
       </c>
       <c r="K66" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L66" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M66" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N66" s="8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P66" s="19"/>
       <c r="Q66" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R66" s="8">
         <v>1</v>
@@ -4847,31 +4857,29 @@
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A67" s="4">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="E67" t="s">
-        <v>28</v>
+        <v>232</v>
       </c>
       <c r="F67" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H67" s="21" t="s">
-        <v>252</v>
-      </c>
+      <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="26">
-        <v>2.57</v>
+        <v>0.37</v>
       </c>
       <c r="K67" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L67" s="8">
         <v>6</v>
@@ -4884,47 +4892,43 @@
       </c>
       <c r="P67" s="19"/>
       <c r="Q67" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R67" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S67" s="8"/>
       <c r="AC67" s="24"/>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A68" s="4">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="E68" t="s">
-        <v>232</v>
-      </c>
-      <c r="F68" t="s">
-        <v>79</v>
+        <v>259</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="H68" s="4"/>
+        <v>260</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>252</v>
+      </c>
       <c r="I68" s="4"/>
       <c r="J68" s="26">
-        <v>0.37</v>
+        <v>3.32</v>
       </c>
       <c r="K68" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L68" s="8">
-        <v>6</v>
-      </c>
-      <c r="M68" s="8">
-        <v>3</v>
-      </c>
-      <c r="N68" s="8">
         <v>3</v>
       </c>
       <c r="P68" s="19"/>
@@ -4932,32 +4936,28 @@
         <v>0</v>
       </c>
       <c r="R68" s="8">
-        <v>0</v>
-      </c>
-      <c r="S68" s="8"/>
-      <c r="AC68" s="24"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A69" s="4">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="30" t="s">
         <v>259</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H69" s="21" t="s">
-        <v>252</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H69" s="4"/>
       <c r="I69" s="4"/>
       <c r="J69" s="26">
         <v>3.32</v>
@@ -4966,38 +4966,40 @@
         <v>2</v>
       </c>
       <c r="L69" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P69" s="19"/>
       <c r="Q69" s="8">
         <v>0</v>
       </c>
       <c r="R69" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A70" s="4">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E70" s="30" t="s">
-        <v>259</v>
+        <v>162</v>
+      </c>
+      <c r="E70" t="s">
+        <v>264</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>30</v>
+        <v>136</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H70" s="4"/>
+      <c r="H70" s="21" t="s">
+        <v>265</v>
+      </c>
       <c r="I70" s="4"/>
       <c r="J70" s="26">
-        <v>3.32</v>
+        <v>0.47</v>
       </c>
       <c r="K70" s="8">
         <v>2</v>
@@ -5005,58 +5007,28 @@
       <c r="L70" s="8">
         <v>4</v>
       </c>
+      <c r="M70" s="8">
+        <v>4</v>
+      </c>
+      <c r="N70" s="8">
+        <v>4</v>
+      </c>
       <c r="P70" s="19"/>
       <c r="Q70" s="8">
         <v>0</v>
       </c>
       <c r="R70" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A71" s="4">
-        <v>123</v>
-      </c>
+      <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E71" t="s">
-        <v>264</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H71" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="I71" s="4"/>
-      <c r="J71" s="26">
-        <v>0.47</v>
-      </c>
-      <c r="K71" s="8">
-        <v>2</v>
-      </c>
-      <c r="L71" s="8">
-        <v>4</v>
-      </c>
-      <c r="M71" s="8">
-        <v>4</v>
-      </c>
-      <c r="N71" s="8">
-        <v>4</v>
-      </c>
+      <c r="H71" s="4"/>
       <c r="P71" s="19"/>
-      <c r="Q71" s="8">
-        <v>0</v>
-      </c>
-      <c r="R71" s="8">
-        <v>1</v>
-      </c>
+      <c r="Q71" s="8"/>
+      <c r="R71" s="8"/>
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A72" s="4"/>
@@ -5117,6 +5089,7 @@
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
       <c r="P78" s="19"/>
       <c r="Q78" s="8"/>
       <c r="R78" s="8"/>
@@ -5125,8 +5098,8 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
       <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
       <c r="P79" s="19"/>
       <c r="Q79" s="8"/>
       <c r="R79" s="8"/>
@@ -5137,6 +5110,8 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="H80" s="4"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="8"/>
       <c r="P80" s="19"/>
       <c r="Q80" s="8"/>
       <c r="R80" s="8"/>
@@ -5145,9 +5120,8 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
       <c r="H81" s="4"/>
-      <c r="K81" s="9"/>
+      <c r="K81" s="8"/>
       <c r="L81" s="8"/>
       <c r="P81" s="19"/>
       <c r="Q81" s="8"/>
@@ -5169,17 +5143,9 @@
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="H83" s="4"/>
-      <c r="K83" s="8"/>
-      <c r="L83" s="8"/>
-      <c r="P83" s="19"/>
-      <c r="Q83" s="8"/>
-      <c r="R83" s="8"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="H84" s="4"/>
+      <c r="J84" s="5"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.45">
       <c r="J85" s="5"/>
@@ -5187,19 +5153,16 @@
     <row r="86" spans="1:18" x14ac:dyDescent="0.45">
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="J87" s="5"/>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:R68" xr:uid="{7020DE52-0B61-9644-93F1-364D58F6F3FB}"/>
+  <autoFilter ref="A9:R70" xr:uid="{7020DE52-0B61-9644-93F1-364D58F6F3FB}"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I82:I84" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I81:I83" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="40" orientation="landscape" r:id="rId1"/>
@@ -5212,13 +5175,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W89"/>
+  <dimension ref="A1:AC89"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A32" sqref="A32:XFD33"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6083,7 +6046,7 @@
       </c>
       <c r="S32" s="8"/>
     </row>
-    <row r="33" spans="1:19" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="30">
         <v>109</v>
       </c>
@@ -6117,17 +6080,51 @@
       </c>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="J34"/>
-      <c r="K34"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="A34" s="4">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" t="s">
+        <v>141</v>
+      </c>
+      <c r="G34" t="s">
+        <v>147</v>
+      </c>
+      <c r="J34" s="26">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="K34" s="8">
+        <v>0</v>
+      </c>
+      <c r="L34" s="8">
+        <v>2</v>
+      </c>
+      <c r="M34" s="8">
+        <v>0</v>
+      </c>
+      <c r="N34" s="8">
+        <v>4</v>
+      </c>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="8">
+        <v>0</v>
+      </c>
+      <c r="R34" s="8">
+        <v>0</v>
+      </c>
+      <c r="S34" s="8"/>
+      <c r="W34" t="s">
+        <v>266</v>
+      </c>
+      <c r="AC34" s="24"/>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -6137,7 +6134,7 @@
       <c r="J35"/>
       <c r="K35"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -6147,7 +6144,7 @@
       <c r="J36"/>
       <c r="K36"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -6157,57 +6154,57 @@
       <c r="J37"/>
       <c r="K37"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G38" s="4"/>
       <c r="J38"/>
       <c r="K38"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G39" s="4"/>
       <c r="J39"/>
       <c r="K39"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G40" s="4"/>
       <c r="J40"/>
       <c r="K40"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G41" s="4"/>
       <c r="J41"/>
       <c r="K41"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G42" s="4"/>
       <c r="J42"/>
       <c r="K42"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G43" s="4"/>
       <c r="J43"/>
       <c r="K43"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G44" s="4"/>
       <c r="J44"/>
       <c r="K44"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G45" s="4"/>
       <c r="J45"/>
       <c r="K45"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G46" s="4"/>
       <c r="J46"/>
       <c r="K46"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G47" s="4"/>
       <c r="J47"/>
       <c r="K47"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.45">
       <c r="G48" s="4"/>
       <c r="J48"/>
       <c r="K48"/>
@@ -6443,11 +6440,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -6681,7 +6676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>27</v>
       </c>
@@ -6695,7 +6690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>29</v>
       </c>
@@ -6709,7 +6704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>30</v>
       </c>
@@ -6723,7 +6718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>31</v>
       </c>
@@ -6737,7 +6732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>32</v>
       </c>
@@ -6751,7 +6746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>33</v>
       </c>
@@ -6765,229 +6760,358 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
+        <v>34</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="8">
+        <v>8229</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="4">
         <v>36</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C24" s="8">
         <v>3508</v>
       </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" s="4">
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="30"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="4">
+        <v>41</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="8">
+        <v>10606</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="4">
+        <v>42</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="8">
+        <v>10505</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="4">
         <v>102</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C27" s="8">
         <v>3737</v>
       </c>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="4">
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="30"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="4">
+        <v>103</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C28" s="8">
+        <v>10441</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="30"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="4">
         <v>104</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" s="4">
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="30"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="4">
         <v>105</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C30" s="8">
         <v>3994</v>
       </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="4">
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="4">
         <v>106</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C31" s="8">
         <v>10431</v>
       </c>
-      <c r="D27" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="4">
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="30"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="4">
         <v>107</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C32" s="8">
         <v>4394</v>
       </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="4">
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="4">
         <v>108</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B33" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="4">
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="30"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="4">
         <v>109</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D30" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A31" s="4">
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="30"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="4">
         <v>110</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C35" s="8">
         <v>5321</v>
       </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" s="4">
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35" s="30"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="4">
         <v>111</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C36" s="8">
         <v>8735</v>
       </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" s="4">
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36" s="30"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="4">
         <v>112</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C37" s="8">
         <v>10420</v>
       </c>
-      <c r="D33" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" s="4">
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="30"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="4">
         <v>113</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C38" s="8">
         <v>10421</v>
       </c>
-      <c r="D34" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="4">
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="G38" s="30"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="4">
         <v>115</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C39" s="8">
         <v>4071</v>
       </c>
-      <c r="D35" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="4">
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="4">
         <v>116</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C40" s="8">
         <v>10456</v>
       </c>
-      <c r="D36" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" s="4">
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="4">
         <v>117</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C41" s="8">
         <v>10490</v>
       </c>
-      <c r="D37" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" s="4">
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="4">
         <v>120</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C42" s="8">
         <v>9870</v>
       </c>
-      <c r="D38" s="4">
-        <v>0</v>
-      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="4">
+        <v>122</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="8">
+        <v>4379</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G54" s="30"/>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G55" s="30"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G56" s="30"/>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G57" s="30"/>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G58" s="30"/>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G59" s="30"/>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G60" s="30"/>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G61" s="30"/>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G62" s="30"/>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G63" s="30"/>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G64" s="30"/>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G65" s="30"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G66" s="30"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G67" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continue making highway edits based on ORTP call for projects
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F38B75-DBB7-4FEA-8156-4128F3072C4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA84160B-BA79-41BD-9B7A-B428DBC83942}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,16 +13,16 @@
     <sheet name="CMP_Rep_Link" sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$60:$O$80</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$R$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$R$66</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="273">
   <si>
     <t>Cost</t>
   </si>
@@ -1720,14 +1720,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>148166</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>301125</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>37795</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>37794</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2093,7 +2093,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC84"/>
+  <dimension ref="A1:AC85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10">
-        <v>100000000</v>
+        <v>110400000</v>
       </c>
       <c r="J10" s="26">
         <v>2.5</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="12" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2388,32 +2388,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
-        <v>353</v>
+        <v>251</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>160</v>
+        <v>54</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>249</v>
+        <v>8</v>
       </c>
       <c r="H13" s="4"/>
-      <c r="I13">
-        <v>12000000</v>
+      <c r="I13" s="24">
+        <v>50000000</v>
       </c>
       <c r="J13" s="26">
-        <v>0.28000000000000003</v>
+        <v>1.25</v>
       </c>
       <c r="K13" s="4">
         <v>2</v>
@@ -2422,75 +2422,74 @@
         <v>4</v>
       </c>
       <c r="M13" s="24">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N13" s="24">
         <v>4</v>
       </c>
+      <c r="O13" s="24"/>
+      <c r="P13" s="18"/>
       <c r="Q13" s="5">
         <v>0</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13" s="30"/>
+      <c r="R13" s="24">
+        <v>0</v>
+      </c>
+      <c r="S13" s="24"/>
       <c r="T13" s="24"/>
-      <c r="U13" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
-      <c r="AC13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="8"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>853</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>250</v>
+      <c r="A14" s="4">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4">
+        <v>353</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14">
+        <v>13200000</v>
       </c>
       <c r="J14" s="26">
-        <v>1.05</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K14" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L14" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M14" s="24">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N14" s="24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q14" s="5">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="30"/>
       <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
+      <c r="U14" s="24" t="s">
+        <v>243</v>
+      </c>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
@@ -2499,47 +2498,41 @@
       <c r="AC14" s="24"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A15" s="4">
-        <v>8</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="C15" s="4">
-        <v>208</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="I15">
-        <v>90000000</v>
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>853</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>250</v>
       </c>
       <c r="J15" s="26">
-        <v>2.0299999999999998</v>
-      </c>
-      <c r="K15" s="12">
+        <v>1.05</v>
+      </c>
+      <c r="K15" s="4">
         <v>5</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="4">
         <v>6</v>
       </c>
       <c r="M15" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="5">
         <v>0</v>
@@ -2558,40 +2551,46 @@
       <c r="AC15" s="24"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>855</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="A16" s="4">
         <v>8</v>
       </c>
-      <c r="H16" s="21" t="s">
-        <v>250</v>
+      <c r="B16" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="4">
+        <v>208</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="I16">
+        <v>251000000</v>
       </c>
       <c r="J16" s="26">
-        <v>4.18</v>
-      </c>
-      <c r="K16" s="4">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="K16" s="12">
+        <v>5</v>
+      </c>
+      <c r="L16" s="12">
         <v>6</v>
       </c>
-      <c r="L16" s="4">
-        <v>8</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
+      <c r="M16" s="24">
+        <v>1</v>
+      </c>
+      <c r="N16" s="24">
         <v>1</v>
       </c>
       <c r="Q16" s="5">
@@ -2612,34 +2611,34 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>256</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>255</v>
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>250</v>
       </c>
       <c r="J17" s="26">
-        <v>1.08</v>
-      </c>
-      <c r="K17" s="12">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7">
-        <v>1</v>
+        <v>4.18</v>
+      </c>
+      <c r="K17" s="4">
+        <v>6</v>
+      </c>
+      <c r="L17" s="4">
+        <v>8</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -2665,28 +2664,28 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>802</v>
+        <v>856</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>256</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>118</v>
+        <v>255</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>114</v>
+        <v>250</v>
       </c>
       <c r="J18" s="26">
-        <v>1.36</v>
+        <v>1.08</v>
       </c>
       <c r="K18" s="12">
         <v>0</v>
@@ -2700,8 +2699,8 @@
       <c r="N18">
         <v>1</v>
       </c>
-      <c r="Q18" s="8">
-        <v>1</v>
+      <c r="Q18" s="5">
+        <v>0</v>
       </c>
       <c r="R18">
         <v>1</v>
@@ -2717,91 +2716,92 @@
       <c r="AC18" s="24"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A19" s="4">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4">
-        <v>211</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="I19">
-        <v>103000000</v>
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>802</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>114</v>
       </c>
       <c r="J19" s="26">
-        <v>3.32</v>
-      </c>
-      <c r="K19" s="4">
-        <v>2</v>
-      </c>
-      <c r="L19" s="4">
-        <v>6</v>
+        <v>1.36</v>
+      </c>
+      <c r="K19" s="12">
+        <v>0</v>
+      </c>
+      <c r="L19" s="7">
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>1</v>
       </c>
       <c r="R19">
         <v>1</v>
       </c>
       <c r="S19" s="30"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
       <c r="AC19" s="24"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20">
-        <v>302</v>
-      </c>
-      <c r="D20" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4">
+        <v>211</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H20" s="22" t="s">
         <v>250</v>
       </c>
       <c r="I20">
-        <v>32000000</v>
+        <v>112000000</v>
       </c>
       <c r="J20" s="26">
-        <v>1.26</v>
+        <v>3.32</v>
       </c>
       <c r="K20" s="4">
         <v>2</v>
       </c>
       <c r="L20" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M20">
         <v>3</v>
@@ -2809,10 +2809,7 @@
       <c r="N20">
         <v>3</v>
       </c>
-      <c r="O20" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q20" s="8">
+      <c r="Q20" s="5">
         <v>0</v>
       </c>
       <c r="R20">
@@ -2823,140 +2820,146 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4">
-        <v>207</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21">
+        <v>302</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="4"/>
+      <c r="H21" s="22" t="s">
+        <v>250</v>
+      </c>
       <c r="I21">
-        <v>300000000</v>
+        <v>35300000</v>
       </c>
       <c r="J21" s="26">
-        <v>1.9</v>
+        <v>1.26</v>
       </c>
       <c r="K21" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L21" s="4">
         <v>4</v>
       </c>
       <c r="M21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N21">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="5">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q21" s="8">
         <v>0</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="30"/>
       <c r="AC21" s="24"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="C22">
-        <v>857</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>250</v>
+      <c r="A22" s="4">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4">
+        <v>207</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22">
+        <v>160300000</v>
       </c>
       <c r="J22" s="26">
-        <v>0.43</v>
+        <v>1.9</v>
       </c>
       <c r="K22" s="4">
+        <v>3</v>
+      </c>
+      <c r="L22" s="4">
         <v>4</v>
       </c>
-      <c r="L22" s="8">
-        <v>5</v>
-      </c>
-      <c r="M22" s="8">
-        <v>3</v>
-      </c>
-      <c r="N22" s="8">
-        <v>3</v>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
       </c>
       <c r="Q22" s="5">
         <v>0</v>
       </c>
       <c r="R22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" s="30"/>
       <c r="AC22" s="24"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A23" s="4">
-        <v>21</v>
+      <c r="A23">
+        <v>20</v>
       </c>
       <c r="C23">
-        <v>803</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>130</v>
+        <v>857</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>147</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23">
-        <v>1350000</v>
+        <v>33</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>250</v>
       </c>
       <c r="J23" s="26">
-        <v>0.19</v>
+        <v>0.43</v>
       </c>
       <c r="K23" s="4">
-        <v>0</v>
-      </c>
-      <c r="L23" s="4">
         <v>4</v>
       </c>
+      <c r="L23" s="8">
+        <v>5</v>
+      </c>
       <c r="M23" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N23" s="8">
-        <v>4</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>0</v>
       </c>
       <c r="R23">
         <v>1</v>
@@ -2966,30 +2969,31 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
-        <v>22</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4">
-        <v>352</v>
-      </c>
-      <c r="D24" t="s">
-        <v>158</v>
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>803</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="G24" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" t="s">
         <v>147</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="21" t="s">
+        <v>114</v>
+      </c>
       <c r="I24">
-        <v>26000000</v>
+        <v>1350000</v>
       </c>
       <c r="J24" s="26">
-        <v>0.65</v>
+        <v>0.19</v>
       </c>
       <c r="K24" s="4">
         <v>0</v>
@@ -3003,106 +3007,108 @@
       <c r="N24" s="8">
         <v>4</v>
       </c>
-      <c r="Q24" s="5">
-        <v>0</v>
+      <c r="Q24" s="8">
+        <v>1</v>
       </c>
       <c r="R24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" s="30"/>
       <c r="AC24" s="24"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
-        <v>23</v>
-      </c>
-      <c r="C25">
-        <v>804</v>
+        <v>22</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4">
+        <v>352</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" t="s">
-        <v>89</v>
-      </c>
-      <c r="G25" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>114</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="4"/>
       <c r="I25">
-        <v>77000</v>
+        <v>28700000</v>
       </c>
       <c r="J25" s="26">
-        <v>2.2999999999999998</v>
+        <v>0.65</v>
       </c>
       <c r="K25" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L25" s="4">
-        <v>6</v>
-      </c>
-      <c r="M25" s="24">
-        <v>3</v>
-      </c>
-      <c r="N25" s="24">
-        <v>3</v>
-      </c>
-      <c r="O25" t="s">
-        <v>112</v>
+        <v>4</v>
+      </c>
+      <c r="M25" s="8">
+        <v>4</v>
+      </c>
+      <c r="N25" s="8">
+        <v>4</v>
       </c>
       <c r="Q25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S25" s="30"/>
       <c r="AC25" s="24"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>204</v>
+        <v>804</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H26" s="22" t="s">
-        <v>250</v>
+        <v>88</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>114</v>
       </c>
       <c r="I26">
-        <v>116000000</v>
+        <v>77000</v>
       </c>
       <c r="J26" s="26">
-        <v>0.43</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K26" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L26" s="4">
-        <v>1</v>
-      </c>
-      <c r="M26">
-        <v>8</v>
-      </c>
-      <c r="N26">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="M26" s="24">
+        <v>3</v>
+      </c>
+      <c r="N26" s="24">
+        <v>3</v>
+      </c>
+      <c r="O26" t="s">
+        <v>112</v>
       </c>
       <c r="Q26" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26">
         <v>1</v>
@@ -3112,88 +3118,82 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4">
-        <v>303</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27" t="s">
-        <v>142</v>
-      </c>
-      <c r="H27" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27">
+        <v>204</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>250</v>
+      </c>
       <c r="I27">
-        <v>48000000</v>
+        <v>139000000</v>
       </c>
       <c r="J27" s="26">
-        <v>1.28</v>
+        <v>0.43</v>
       </c>
       <c r="K27" s="4">
         <v>0</v>
       </c>
-      <c r="L27" s="25">
-        <v>4</v>
+      <c r="L27" s="4">
+        <v>1</v>
       </c>
       <c r="M27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q27" s="5">
         <v>0</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S27" s="30"/>
       <c r="AC27" s="24"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>240</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B28" s="4"/>
       <c r="C28" s="4">
-        <v>801</v>
-      </c>
-      <c r="D28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" t="s">
-        <v>83</v>
+        <v>303</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="G28" t="s">
-        <v>147</v>
-      </c>
-      <c r="H28" s="22" t="s">
-        <v>250</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="H28" s="4"/>
       <c r="I28">
-        <v>13300000</v>
+        <v>53000000</v>
       </c>
       <c r="J28" s="26">
-        <v>1.43</v>
+        <v>1.28</v>
       </c>
       <c r="K28" s="4">
         <v>0</v>
       </c>
-      <c r="L28" s="4">
-        <v>6</v>
+      <c r="L28" s="25">
+        <v>4</v>
       </c>
       <c r="M28">
         <v>4</v>
@@ -3205,52 +3205,55 @@
         <v>0</v>
       </c>
       <c r="R28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S28" s="30"/>
       <c r="AC28" s="24"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
-        <v>28</v>
-      </c>
-      <c r="C29">
-        <v>858</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>134</v>
+        <v>26</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C29" s="4">
+        <v>801</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" t="s">
+        <v>147</v>
       </c>
       <c r="H29" s="22" t="s">
         <v>250</v>
       </c>
       <c r="I29">
-        <v>500000</v>
+        <v>13300000</v>
       </c>
       <c r="J29" s="26">
-        <v>1</v>
+        <v>1.43</v>
       </c>
       <c r="K29" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L29" s="4">
+        <v>6</v>
+      </c>
+      <c r="M29">
         <v>4</v>
       </c>
-      <c r="M29">
-        <v>3</v>
-      </c>
       <c r="N29">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="5">
         <v>0</v>
       </c>
       <c r="R29">
@@ -3261,36 +3264,37 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4">
-        <v>304</v>
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>858</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="4"/>
+        <v>134</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>250</v>
+      </c>
       <c r="I30">
-        <v>180000000</v>
+        <v>500000</v>
       </c>
       <c r="J30" s="26">
-        <v>2.36</v>
+        <v>1</v>
       </c>
       <c r="K30" s="4">
+        <v>5</v>
+      </c>
+      <c r="L30" s="4">
         <v>4</v>
-      </c>
-      <c r="L30" s="4">
-        <v>6</v>
       </c>
       <c r="M30">
         <v>3</v>
@@ -3298,51 +3302,47 @@
       <c r="N30">
         <v>3</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="Q30" s="8">
         <v>0</v>
       </c>
       <c r="R30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S30" s="30"/>
       <c r="AC30" s="24"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31">
-        <v>206</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E31" t="s">
-        <v>77</v>
-      </c>
-      <c r="F31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>72</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4">
+        <v>304</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="4"/>
       <c r="I31">
-        <v>20000000</v>
+        <v>180000000</v>
       </c>
       <c r="J31" s="26">
-        <v>0.35</v>
+        <v>2.36</v>
       </c>
       <c r="K31" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L31" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M31">
         <v>3</v>
@@ -3361,10 +3361,13 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
       </c>
       <c r="C32">
-        <v>304</v>
+        <v>206</v>
       </c>
       <c r="D32" t="s">
         <v>52</v>
@@ -3376,11 +3379,13 @@
         <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="4"/>
+        <v>147</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="I32">
-        <v>180000000</v>
+        <v>20000000</v>
       </c>
       <c r="J32" s="26">
         <v>0.35</v>
@@ -3389,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M32">
         <v>3</v>
@@ -3408,51 +3413,43 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="C33">
-        <v>210</v>
+        <v>304</v>
       </c>
       <c r="D33" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G33" t="s">
-        <v>147</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>72</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H33" s="4"/>
       <c r="I33">
-        <v>76000000</v>
+        <v>180000000</v>
       </c>
       <c r="J33" s="26">
-        <v>2.48</v>
+        <v>0.35</v>
       </c>
       <c r="K33" s="4">
         <v>0</v>
       </c>
       <c r="L33" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N33">
-        <v>4</v>
-      </c>
-      <c r="O33" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q33" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="5">
         <v>0</v>
       </c>
       <c r="R33">
@@ -3463,43 +3460,49 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
       </c>
       <c r="C34">
-        <v>709</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>127</v>
+        <v>210</v>
+      </c>
+      <c r="D34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" t="s">
+        <v>147</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="I34">
-        <v>18200000</v>
+        <v>83900000</v>
       </c>
       <c r="J34" s="26">
-        <v>0.54</v>
+        <v>2.48</v>
       </c>
       <c r="K34" s="4">
         <v>0</v>
       </c>
       <c r="L34" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N34">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="O34" t="s">
+        <v>112</v>
       </c>
       <c r="Q34" s="8">
         <v>0</v>
@@ -3511,41 +3514,46 @@
       <c r="AC34" s="24"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>34</v>
+      <c r="A35" s="4">
+        <v>33</v>
       </c>
       <c r="C35">
-        <v>859</v>
-      </c>
-      <c r="D35" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="21"/>
+        <v>709</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35">
+        <v>18200000</v>
+      </c>
       <c r="J35" s="26">
-        <v>0.47</v>
+        <v>0.54</v>
       </c>
       <c r="K35" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L35" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N35">
-        <v>1</v>
-      </c>
-      <c r="Q35" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q35" s="8">
         <v>0</v>
       </c>
       <c r="R35">
@@ -3556,83 +3564,75 @@
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>859</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>25</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="G36" t="s">
-        <v>180</v>
-      </c>
-      <c r="H36" s="22" t="s">
-        <v>250</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H36" s="21"/>
       <c r="J36" s="26">
-        <v>0.51</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>232</v>
+        <v>0.47</v>
+      </c>
+      <c r="K36" s="4">
+        <v>2</v>
+      </c>
+      <c r="L36" s="4">
+        <v>3</v>
       </c>
       <c r="M36">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N36">
-        <v>8</v>
-      </c>
-      <c r="Q36" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="5">
         <v>0</v>
       </c>
       <c r="R36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" s="30"/>
       <c r="AC36" s="24"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A37" s="4">
-        <v>36</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="C37" s="4">
-        <v>209</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G37" s="4" t="s">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" t="s">
+        <v>180</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="J37" s="26">
+        <v>0.51</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="M37">
         <v>8</v>
       </c>
-      <c r="H37" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="I37">
-        <v>87280000</v>
-      </c>
-      <c r="J37" s="26">
-        <v>0.99</v>
-      </c>
-      <c r="K37" s="4">
-        <v>2</v>
-      </c>
-      <c r="L37" s="4">
-        <v>6</v>
-      </c>
-      <c r="M37">
-        <v>4</v>
-      </c>
       <c r="N37">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q37" s="8">
         <v>0</v>
@@ -3645,37 +3645,40 @@
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
-        <v>39</v>
-      </c>
-      <c r="C38">
-        <v>806</v>
-      </c>
-      <c r="D38" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38" t="s">
-        <v>85</v>
-      </c>
-      <c r="G38" t="s">
-        <v>87</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>114</v>
+        <v>36</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" s="4">
+        <v>209</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="22" t="s">
+        <v>251</v>
       </c>
       <c r="I38">
-        <v>77000</v>
+        <v>92000000</v>
       </c>
       <c r="J38" s="26">
-        <v>0.28999999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="K38" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L38" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M38">
         <v>4</v>
@@ -3683,11 +3686,8 @@
       <c r="N38">
         <v>4</v>
       </c>
-      <c r="O38" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q38" s="5">
-        <v>1</v>
+      <c r="Q38" s="8">
+        <v>0</v>
       </c>
       <c r="R38">
         <v>1</v>
@@ -3697,58 +3697,75 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="C39">
+        <v>806</v>
       </c>
       <c r="D39" t="s">
-        <v>182</v>
+        <v>86</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="F39" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="G39" t="s">
-        <v>147</v>
-      </c>
-      <c r="H39" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="I39">
+        <v>77000</v>
+      </c>
       <c r="J39" s="26">
-        <v>3.88</v>
-      </c>
-      <c r="K39" s="8">
-        <v>0</v>
-      </c>
-      <c r="L39" s="8">
-        <v>2</v>
-      </c>
-      <c r="M39" s="8">
-        <v>5</v>
-      </c>
-      <c r="N39" s="8">
-        <v>5</v>
-      </c>
-      <c r="Q39" s="8">
-        <v>0</v>
-      </c>
-      <c r="R39" s="8">
-        <v>0</v>
-      </c>
-      <c r="S39" s="8"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K39" s="4">
+        <v>4</v>
+      </c>
+      <c r="L39" s="4">
+        <v>4</v>
+      </c>
+      <c r="M39">
+        <v>4</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+      <c r="O39" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39" s="30"/>
       <c r="AC39" s="24"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="E40" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>144</v>
       </c>
       <c r="G40" t="s">
         <v>147</v>
       </c>
       <c r="H40" s="4"/>
       <c r="J40" s="26">
-        <v>2.68</v>
+        <v>3.88</v>
       </c>
       <c r="K40" s="8">
         <v>0</v>
@@ -3757,10 +3774,10 @@
         <v>2</v>
       </c>
       <c r="M40" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N40" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q40" s="8">
         <v>0</v>
@@ -3773,19 +3790,17 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G41" t="s">
         <v>147</v>
       </c>
-      <c r="H41" s="4" t="s">
-        <v>251</v>
-      </c>
+      <c r="H41" s="4"/>
       <c r="J41" s="26">
-        <v>5.36</v>
+        <v>2.68</v>
       </c>
       <c r="K41" s="8">
         <v>0</v>
@@ -3803,47 +3818,38 @@
         <v>0</v>
       </c>
       <c r="R41" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41" s="8"/>
       <c r="AC41" s="24"/>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>185</v>
-      </c>
-      <c r="E42" t="s">
-        <v>116</v>
-      </c>
-      <c r="F42" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G42" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J42" s="26">
-        <v>2.95</v>
-      </c>
-      <c r="K42" s="4">
-        <v>1</v>
-      </c>
-      <c r="L42" s="4">
+        <v>5.36</v>
+      </c>
+      <c r="K42" s="8">
+        <v>0</v>
+      </c>
+      <c r="L42" s="8">
         <v>2</v>
       </c>
       <c r="M42" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N42" s="8">
-        <v>1</v>
-      </c>
-      <c r="O42" t="s">
-        <v>188</v>
+        <v>6</v>
       </c>
       <c r="Q42" s="8">
         <v>0</v>
@@ -3856,37 +3862,40 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D43" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E43" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="F43" t="s">
-        <v>116</v>
+        <v>186</v>
       </c>
       <c r="G43" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>250</v>
       </c>
       <c r="J43" s="26">
-        <v>5.03</v>
+        <v>2.95</v>
       </c>
       <c r="K43" s="4">
         <v>1</v>
       </c>
       <c r="L43" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M43" s="8">
         <v>1</v>
       </c>
       <c r="N43" s="8">
         <v>1</v>
+      </c>
+      <c r="O43" t="s">
+        <v>188</v>
       </c>
       <c r="Q43" s="8">
         <v>0</v>
@@ -3899,16 +3908,16 @@
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D44" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E44" t="s">
+        <v>190</v>
+      </c>
+      <c r="F44" t="s">
         <v>116</v>
-      </c>
-      <c r="F44" t="s">
-        <v>193</v>
       </c>
       <c r="G44" t="s">
         <v>191</v>
@@ -3917,7 +3926,7 @@
         <v>250</v>
       </c>
       <c r="J44" s="26">
-        <v>7.61</v>
+        <v>5.03</v>
       </c>
       <c r="K44" s="4">
         <v>1</v>
@@ -3942,16 +3951,16 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E45" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="F45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G45" t="s">
         <v>191</v>
@@ -3960,7 +3969,7 @@
         <v>250</v>
       </c>
       <c r="J45" s="26">
-        <v>2.93</v>
+        <v>7.61</v>
       </c>
       <c r="K45" s="4">
         <v>1</v>
@@ -3985,31 +3994,31 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E46" t="s">
-        <v>197</v>
+        <v>60</v>
       </c>
       <c r="F46" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G46" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>250</v>
       </c>
       <c r="J46" s="26">
-        <v>0.78</v>
+        <v>2.93</v>
       </c>
       <c r="K46" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46" s="8">
         <v>1</v>
@@ -4027,59 +4036,67 @@
       <c r="AC46" s="24"/>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A47" s="24">
-        <v>102</v>
+      <c r="A47" s="4">
+        <v>48</v>
       </c>
       <c r="D47" t="s">
-        <v>201</v>
+        <v>196</v>
+      </c>
+      <c r="E47" t="s">
+        <v>197</v>
+      </c>
+      <c r="F47" t="s">
+        <v>198</v>
       </c>
       <c r="G47" t="s">
         <v>187</v>
       </c>
-      <c r="H47" s="4"/>
+      <c r="H47" s="4" t="s">
+        <v>250</v>
+      </c>
       <c r="J47" s="26">
-        <v>0.23</v>
+        <v>0.78</v>
       </c>
       <c r="K47" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="4">
-        <v>2</v>
-      </c>
-      <c r="M47">
-        <v>8</v>
-      </c>
-      <c r="N47">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="M47" s="8">
+        <v>1</v>
+      </c>
+      <c r="N47" s="8">
+        <v>1</v>
       </c>
       <c r="Q47" s="8">
         <v>0</v>
       </c>
       <c r="R47" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S47" s="8"/>
       <c r="AC47" s="24"/>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A48" s="24">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>187</v>
       </c>
       <c r="H48" s="4"/>
       <c r="J48" s="26">
-        <v>0.41</v>
-      </c>
-      <c r="K48">
-        <v>1</v>
-      </c>
-      <c r="L48">
-        <v>1</v>
+        <v>0.23</v>
+      </c>
+      <c r="K48" s="4">
+        <v>1</v>
+      </c>
+      <c r="L48" s="4">
+        <v>2</v>
       </c>
       <c r="M48">
         <v>8</v>
@@ -4098,35 +4115,29 @@
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A49" s="24">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D49" t="s">
-        <v>203</v>
-      </c>
-      <c r="E49" t="s">
-        <v>148</v>
-      </c>
-      <c r="F49" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G49" t="s">
-        <v>187</v>
+        <v>101</v>
       </c>
       <c r="H49" s="4"/>
       <c r="J49" s="26">
-        <v>4.97</v>
+        <v>0.41</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M49">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="N49">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Q49" s="8">
         <v>0</v>
@@ -4139,35 +4150,35 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A50" s="24">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E50" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
       <c r="F50" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G50" t="s">
         <v>187</v>
       </c>
       <c r="H50" s="4"/>
       <c r="J50" s="26">
-        <v>6.28</v>
+        <v>4.97</v>
       </c>
       <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
         <v>2</v>
       </c>
-      <c r="L50">
-        <v>4</v>
-      </c>
       <c r="M50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q50" s="8">
         <v>0</v>
@@ -4180,38 +4191,41 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A51" s="24">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="C51">
+        <v>702</v>
       </c>
       <c r="D51" t="s">
-        <v>265</v>
+        <v>205</v>
       </c>
       <c r="E51" t="s">
-        <v>269</v>
+        <v>206</v>
+      </c>
+      <c r="F51" t="s">
+        <v>207</v>
       </c>
       <c r="G51" t="s">
         <v>187</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51">
-        <v>160000000</v>
+        <v>348900000</v>
       </c>
       <c r="J51" s="26">
-        <v>0.05</v>
-      </c>
-      <c r="K51" t="s">
-        <v>232</v>
-      </c>
-      <c r="L51" t="s">
-        <v>232</v>
-      </c>
-      <c r="M51" s="30" t="s">
-        <v>232</v>
-      </c>
-      <c r="N51" s="30" t="s">
-        <v>232</v>
-      </c>
-      <c r="O51" t="s">
-        <v>188</v>
+        <v>6.28</v>
+      </c>
+      <c r="K51">
+        <v>2</v>
+      </c>
+      <c r="L51">
+        <v>4</v>
+      </c>
+      <c r="M51">
+        <v>4</v>
+      </c>
+      <c r="N51">
+        <v>4</v>
       </c>
       <c r="Q51" s="8">
         <v>0</v>
@@ -4224,35 +4238,38 @@
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A52" s="24">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D52" t="s">
-        <v>208</v>
+        <v>265</v>
       </c>
       <c r="E52" t="s">
-        <v>30</v>
-      </c>
-      <c r="F52" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="G52" t="s">
         <v>187</v>
       </c>
       <c r="H52" s="4"/>
+      <c r="I52">
+        <v>160000000</v>
+      </c>
       <c r="J52" s="26">
-        <v>0.49</v>
-      </c>
-      <c r="K52">
-        <v>4</v>
-      </c>
-      <c r="L52">
-        <v>6</v>
-      </c>
-      <c r="M52">
-        <v>3</v>
-      </c>
-      <c r="N52">
-        <v>3</v>
+        <v>0.05</v>
+      </c>
+      <c r="K52" t="s">
+        <v>232</v>
+      </c>
+      <c r="L52" t="s">
+        <v>232</v>
+      </c>
+      <c r="M52" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="N52" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="O52" t="s">
+        <v>188</v>
       </c>
       <c r="Q52" s="8">
         <v>0</v>
@@ -4265,33 +4282,34 @@
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A53" s="24">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D53" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E53" t="s">
-        <v>215</v>
+        <v>30</v>
       </c>
       <c r="F53" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G53" t="s">
         <v>187</v>
       </c>
+      <c r="H53" s="4"/>
       <c r="J53" s="26">
-        <v>0.69</v>
-      </c>
-      <c r="K53" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="K53">
+        <v>4</v>
+      </c>
+      <c r="L53">
+        <v>6</v>
+      </c>
+      <c r="M53">
         <v>3</v>
       </c>
-      <c r="L53" s="5">
-        <v>5</v>
-      </c>
-      <c r="M53" s="8">
-        <v>3</v>
-      </c>
-      <c r="N53" s="8">
+      <c r="N53">
         <v>3</v>
       </c>
       <c r="Q53" s="8">
@@ -4305,34 +4323,34 @@
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A54" s="24">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D54" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E54" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F54" t="s">
-        <v>119</v>
+        <v>216</v>
       </c>
       <c r="G54" t="s">
         <v>187</v>
       </c>
       <c r="J54" s="26">
-        <v>16.190000000000001</v>
-      </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <v>4</v>
-      </c>
-      <c r="M54">
-        <v>4</v>
-      </c>
-      <c r="N54">
-        <v>4</v>
+        <v>0.69</v>
+      </c>
+      <c r="K54" s="5">
+        <v>3</v>
+      </c>
+      <c r="L54" s="5">
+        <v>5</v>
+      </c>
+      <c r="M54" s="8">
+        <v>3</v>
+      </c>
+      <c r="N54" s="8">
+        <v>3</v>
       </c>
       <c r="Q54" s="8">
         <v>0</v>
@@ -4345,36 +4363,35 @@
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A55" s="24">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D55" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E55" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F55" t="s">
-        <v>218</v>
+        <v>119</v>
       </c>
       <c r="G55" t="s">
         <v>187</v>
       </c>
       <c r="J55" s="26">
-        <v>3.25</v>
-      </c>
-      <c r="K55" s="5">
-        <v>0</v>
-      </c>
-      <c r="L55" s="5">
-        <v>2</v>
-      </c>
-      <c r="M55" s="8">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
         <v>4</v>
       </c>
-      <c r="N55" s="8">
+      <c r="M55">
         <v>4</v>
       </c>
-      <c r="P55" s="19"/>
+      <c r="N55">
+        <v>4</v>
+      </c>
       <c r="Q55" s="8">
         <v>0</v>
       </c>
@@ -4386,37 +4403,34 @@
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A56" s="24">
-        <v>113</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
+        <v>112</v>
+      </c>
       <c r="D56" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E56" t="s">
-        <v>141</v>
+        <v>220</v>
       </c>
       <c r="F56" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G56" t="s">
         <v>187</v>
       </c>
-      <c r="H56" s="4"/>
       <c r="J56" s="26">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="K56" s="8">
-        <v>0</v>
-      </c>
-      <c r="L56" s="8">
+        <v>3.25</v>
+      </c>
+      <c r="K56" s="5">
+        <v>0</v>
+      </c>
+      <c r="L56" s="5">
         <v>2</v>
       </c>
       <c r="M56" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N56" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P56" s="19"/>
       <c r="Q56" s="8">
@@ -4430,26 +4444,30 @@
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A57" s="24">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G57" s="4" t="s">
+      <c r="C57" s="4">
+        <v>708</v>
+      </c>
+      <c r="D57" t="s">
+        <v>221</v>
+      </c>
+      <c r="E57" t="s">
+        <v>141</v>
+      </c>
+      <c r="F57" t="s">
+        <v>222</v>
+      </c>
+      <c r="G57" t="s">
         <v>187</v>
       </c>
       <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
+      <c r="I57">
+        <v>1269000000</v>
+      </c>
       <c r="J57" s="26">
-        <v>0.28999999999999998</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="K57" s="8">
         <v>0</v>
@@ -4458,10 +4476,10 @@
         <v>2</v>
       </c>
       <c r="M57" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N57" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P57" s="19"/>
       <c r="Q57" s="8">
@@ -4475,21 +4493,26 @@
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A58" s="24">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H58" s="21" t="s">
-        <v>250</v>
-      </c>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
       <c r="J58" s="26">
-        <v>0.23</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K58" s="8">
         <v>0</v>
@@ -4498,29 +4521,29 @@
         <v>2</v>
       </c>
       <c r="M58" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N58" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P58" s="19"/>
       <c r="Q58" s="8">
         <v>0</v>
       </c>
       <c r="R58" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S58" s="8"/>
       <c r="AC58" s="24"/>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A59" s="24">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>187</v>
@@ -4529,7 +4552,7 @@
         <v>250</v>
       </c>
       <c r="J59" s="26">
-        <v>0.42</v>
+        <v>0.23</v>
       </c>
       <c r="K59" s="8">
         <v>0</v>
@@ -4555,20 +4578,21 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A60" s="24">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
+      <c r="H60" s="21" t="s">
+        <v>250</v>
+      </c>
       <c r="J60" s="26">
-        <v>4.41</v>
+        <v>0.42</v>
       </c>
       <c r="K60" s="8">
         <v>0</v>
@@ -4580,7 +4604,7 @@
         <v>7</v>
       </c>
       <c r="N60" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P60" s="19"/>
       <c r="Q60" s="8">
@@ -4593,45 +4617,37 @@
       <c r="AC60" s="24"/>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A61" s="4">
-        <v>119</v>
+      <c r="A61" s="24">
+        <v>118</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E61" t="s">
-        <v>28</v>
-      </c>
-      <c r="F61" t="s">
-        <v>167</v>
+        <v>229</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H61" s="21" t="s">
-        <v>250</v>
-      </c>
+      <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="26">
-        <v>2.57</v>
+        <v>4.41</v>
       </c>
       <c r="K61" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L61" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="M61" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N61" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="P61" s="19"/>
       <c r="Q61" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R61" s="8">
         <v>1</v>
@@ -4641,29 +4657,31 @@
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A62" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="E62" t="s">
-        <v>231</v>
+        <v>28</v>
       </c>
       <c r="F62" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H62" s="4"/>
+      <c r="H62" s="21" t="s">
+        <v>250</v>
+      </c>
       <c r="I62" s="4"/>
       <c r="J62" s="26">
-        <v>0.37</v>
+        <v>2.57</v>
       </c>
       <c r="K62" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L62" s="8">
         <v>6</v>
@@ -4676,43 +4694,47 @@
       </c>
       <c r="P62" s="19"/>
       <c r="Q62" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R62" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S62" s="8"/>
       <c r="AC62" s="24"/>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A63" s="4">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>164</v>
+        <v>205</v>
       </c>
       <c r="E63" t="s">
-        <v>257</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>30</v>
+        <v>231</v>
+      </c>
+      <c r="F63" t="s">
+        <v>79</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="H63" s="21" t="s">
-        <v>250</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="26">
-        <v>3.32</v>
+        <v>0.37</v>
       </c>
       <c r="K63" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L63" s="8">
+        <v>6</v>
+      </c>
+      <c r="M63" s="8">
+        <v>3</v>
+      </c>
+      <c r="N63" s="8">
         <v>3</v>
       </c>
       <c r="P63" s="19"/>
@@ -4720,28 +4742,32 @@
         <v>0</v>
       </c>
       <c r="R63" s="8">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="S63" s="8"/>
+      <c r="AC63" s="24"/>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A64" s="4">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E64" s="30" t="s">
+      <c r="E64" t="s">
         <v>257</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H64" s="4"/>
+        <v>258</v>
+      </c>
+      <c r="H64" s="21" t="s">
+        <v>250</v>
+      </c>
       <c r="I64" s="4"/>
       <c r="J64" s="26">
         <v>3.32</v>
@@ -4750,40 +4776,38 @@
         <v>2</v>
       </c>
       <c r="L64" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P64" s="19"/>
       <c r="Q64" s="8">
         <v>0</v>
       </c>
       <c r="R64" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A65" s="4">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E65" t="s">
-        <v>262</v>
+        <v>164</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>257</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>136</v>
+        <v>30</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="21" t="s">
-        <v>263</v>
-      </c>
+      <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="J65" s="26">
-        <v>0.47</v>
+        <v>3.32</v>
       </c>
       <c r="K65" s="8">
         <v>2</v>
@@ -4791,28 +4815,58 @@
       <c r="L65" s="8">
         <v>4</v>
       </c>
-      <c r="M65" s="8">
-        <v>4</v>
-      </c>
-      <c r="N65" s="8">
-        <v>4</v>
-      </c>
       <c r="P65" s="19"/>
       <c r="Q65" s="8">
         <v>0</v>
       </c>
       <c r="R65" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A66" s="4"/>
+      <c r="A66" s="4">
+        <v>123</v>
+      </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="H66" s="4"/>
+      <c r="D66" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E66" t="s">
+        <v>262</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="I66" s="4"/>
+      <c r="J66" s="26">
+        <v>0.47</v>
+      </c>
+      <c r="K66" s="8">
+        <v>2</v>
+      </c>
+      <c r="L66" s="8">
+        <v>4</v>
+      </c>
+      <c r="M66" s="8">
+        <v>4</v>
+      </c>
+      <c r="N66" s="8">
+        <v>4</v>
+      </c>
       <c r="P66" s="19"/>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="8"/>
+      <c r="Q66" s="8">
+        <v>0</v>
+      </c>
+      <c r="R66" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A67" s="4"/>
@@ -4873,7 +4927,6 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
       <c r="P73" s="19"/>
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
@@ -4882,8 +4935,8 @@
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
       <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
       <c r="P74" s="19"/>
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
@@ -4894,8 +4947,6 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="H75" s="4"/>
-      <c r="K75" s="9"/>
-      <c r="L75" s="8"/>
       <c r="P75" s="19"/>
       <c r="Q75" s="8"/>
       <c r="R75" s="8"/>
@@ -4904,8 +4955,9 @@
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
       <c r="H76" s="4"/>
-      <c r="K76" s="8"/>
+      <c r="K76" s="9"/>
       <c r="L76" s="8"/>
       <c r="P76" s="19"/>
       <c r="Q76" s="8"/>
@@ -4927,9 +4979,17 @@
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="H78" s="4"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="P78" s="19"/>
+      <c r="Q78" s="8"/>
+      <c r="R78" s="8"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="J79" s="5"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="H79" s="4"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.45">
       <c r="J80" s="5"/>
@@ -4937,16 +4997,19 @@
     <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="J81" s="5"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J82" s="5"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:R65" xr:uid="{7020DE52-0B61-9644-93F1-364D58F6F3FB}"/>
+  <autoFilter ref="A9:R66" xr:uid="{7020DE52-0B61-9644-93F1-364D58F6F3FB}"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I76:I78" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I77:I79" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" scale="40" orientation="landscape" r:id="rId1"/>
@@ -4965,7 +5028,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5555,63 +5618,6 @@
       </c>
     </row>
     <row r="27" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="4">
-        <v>4</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4">
-        <v>251</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="I27" s="24">
-        <v>50000000</v>
-      </c>
-      <c r="J27" s="26">
-        <v>1.25</v>
-      </c>
-      <c r="K27" s="4">
-        <v>2</v>
-      </c>
-      <c r="L27" s="4">
-        <v>4</v>
-      </c>
-      <c r="M27" s="24">
-        <v>4</v>
-      </c>
-      <c r="N27" s="24">
-        <v>4</v>
-      </c>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="5">
-        <v>0</v>
-      </c>
-      <c r="R27" s="24">
-        <v>0</v>
-      </c>
-      <c r="S27" s="24">
-        <v>1</v>
-      </c>
-      <c r="T27" s="24">
-        <v>1</v>
-      </c>
-      <c r="U27" s="24">
-        <v>0</v>
-      </c>
-      <c r="V27" s="8">
-        <v>0</v>
-      </c>
       <c r="W27" s="24" t="s">
         <v>247</v>
       </c>
@@ -6498,11 +6504,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -6556,7 +6560,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>141</v>
@@ -6570,13 +6574,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>161</v>
       </c>
       <c r="C5" s="8">
-        <v>10109</v>
+        <v>9787</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -6584,27 +6588,27 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
       <c r="C6" s="8">
-        <v>7456</v>
+        <v>10109</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="C7" s="8">
-        <v>4379</v>
+        <v>7456</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -6612,55 +6616,55 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>164</v>
       </c>
       <c r="C8" s="8">
-        <v>4089</v>
+        <v>4379</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="C9" s="8">
-        <v>4213</v>
+        <v>4089</v>
       </c>
       <c r="D9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C10" s="8">
-        <v>10951</v>
+        <v>4213</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="C11" s="8">
-        <v>10416</v>
+        <v>10951</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
@@ -6668,13 +6672,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C12" s="8">
-        <v>10507</v>
+        <v>10416</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -6682,13 +6686,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="C13" s="8">
-        <v>10428</v>
+        <v>10507</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -6696,13 +6700,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="8">
-        <v>11003</v>
+        <v>10428</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -6710,13 +6714,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="C15" s="8">
-        <v>10447</v>
+        <v>11003</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
@@ -6724,42 +6728,41 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C16" s="8">
-        <v>8768</v>
+        <v>10447</v>
       </c>
       <c r="D16" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
-        <v>34</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="C17" s="8">
-        <v>8229</v>
+        <v>8768</v>
       </c>
       <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="30"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
-        <v>36</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>162</v>
+        <v>34</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>25</v>
       </c>
       <c r="C18" s="8">
-        <v>3508</v>
+        <v>8229</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
@@ -6768,27 +6771,28 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
-        <v>41</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>182</v>
+        <v>36</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="C19" s="8">
-        <v>10606</v>
+        <v>3508</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
       </c>
+      <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" s="8">
-        <v>10505</v>
+        <v>10606</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -6796,133 +6800,132 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
-        <v>102</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>201</v>
+        <v>42</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>183</v>
       </c>
       <c r="C21" s="8">
-        <v>3737</v>
+        <v>10505</v>
       </c>
       <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="G21" s="30"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
-        <v>103</v>
-      </c>
-      <c r="B22" s="30" t="s">
-        <v>202</v>
+        <v>102</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="C22" s="8">
-        <v>10441</v>
+        <v>3737</v>
       </c>
       <c r="D22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
-        <v>104</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>235</v>
+        <v>103</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="8">
+        <v>10441</v>
       </c>
       <c r="D23" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="30"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C24" s="8">
-        <v>3994</v>
+        <v>203</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="D24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
-        <v>106</v>
-      </c>
-      <c r="B25" s="30" t="s">
-        <v>265</v>
+        <v>105</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="C25" s="8">
-        <v>9153</v>
+        <v>3994</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
-        <v>107</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>208</v>
+        <v>106</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>265</v>
       </c>
       <c r="C26" s="8">
-        <v>4394</v>
+        <v>9153</v>
       </c>
       <c r="D26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="30"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>236</v>
+        <v>208</v>
+      </c>
+      <c r="C27" s="8">
+        <v>4394</v>
       </c>
       <c r="D27" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>237</v>
+        <v>210</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>236</v>
       </c>
       <c r="D28" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="30"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C29" s="8">
-        <v>5321</v>
+        <v>212</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>237</v>
       </c>
       <c r="D29" s="4">
         <v>0</v>
@@ -6931,13 +6934,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C30" s="8">
-        <v>8735</v>
+        <v>5321</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -6946,13 +6949,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C31" s="8">
-        <v>10420</v>
+        <v>8735</v>
       </c>
       <c r="D31" s="4">
         <v>0</v>
@@ -6961,13 +6964,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C32" s="8">
-        <v>10421</v>
+        <v>10420</v>
       </c>
       <c r="D32" s="4">
         <v>0</v>
@@ -6976,13 +6979,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C33" s="8">
-        <v>4071</v>
+        <v>10421</v>
       </c>
       <c r="D33" s="4">
         <v>0</v>
@@ -6991,13 +6994,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C34" s="8">
-        <v>10456</v>
+        <v>4071</v>
       </c>
       <c r="D34" s="4">
         <v>0</v>
@@ -7006,13 +7009,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C35" s="8">
-        <v>10490</v>
+        <v>10456</v>
       </c>
       <c r="D35" s="4">
         <v>0</v>
@@ -7021,34 +7024,46 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="C36" s="8">
-        <v>9870</v>
+        <v>10490</v>
       </c>
       <c r="D36" s="4">
         <v>0</v>
       </c>
+      <c r="G36" s="30"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
+        <v>120</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" s="8">
+        <v>9870</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="4">
         <v>122</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C38" s="8">
         <v>4379</v>
       </c>
-      <c r="D37" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G48" s="30"/>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G49" s="30"/>
@@ -7088,6 +7103,9 @@
     </row>
     <row r="61" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G61" s="30"/>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G62" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update single-project analysis and project sheets
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97FBAEB-7015-47A1-AF83-D102DCD1CEF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EE60B9-FDC1-423A-8470-A8A781A0D42B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,23 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$60:$O$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$R$66</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="277">
   <si>
     <t>Cost</t>
   </si>
@@ -850,6 +861,9 @@
   </si>
   <si>
     <t>Illustrative</t>
+  </si>
+  <si>
+    <t>This is a new interchange, and can't accurately be captured by the regional model</t>
   </si>
 </sst>
 </file>
@@ -6524,9 +6538,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -6536,7 +6552,7 @@
     <col min="4" max="16384" width="9.1328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="28" t="s">
         <v>173</v>
       </c>
@@ -6550,7 +6566,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6564,7 +6580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6578,7 +6594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>124</v>
       </c>
@@ -6592,7 +6608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -6606,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -6619,8 +6635,15 @@
       <c r="D6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H6" s="4">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4">
+        <f>VLOOKUP(H6,$A$2:$A$38,1,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>8</v>
       </c>
@@ -6633,8 +6656,15 @@
       <c r="D7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H7" s="4">
+        <v>124</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" ref="I7:I34" si="0">VLOOKUP(H7,$A$2:$A$38,1,FALSE)</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>16</v>
       </c>
@@ -6647,8 +6677,15 @@
       <c r="D8" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H8" s="4">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>17</v>
       </c>
@@ -6661,8 +6698,15 @@
       <c r="D9" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>19</v>
       </c>
@@ -6675,8 +6719,15 @@
       <c r="D10" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H10" s="4">
+        <v>19</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>22</v>
       </c>
@@ -6689,8 +6740,15 @@
       <c r="D11" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H11" s="4">
+        <v>22</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>25</v>
       </c>
@@ -6703,8 +6761,15 @@
       <c r="D12" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H12" s="4">
+        <v>24</v>
+      </c>
+      <c r="I12" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>29</v>
       </c>
@@ -6717,8 +6782,15 @@
       <c r="D13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H13" s="4">
+        <v>25</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>30</v>
       </c>
@@ -6731,8 +6803,15 @@
       <c r="D14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H14" s="4">
+        <v>29</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>31</v>
       </c>
@@ -6745,8 +6824,15 @@
       <c r="D15" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="H15" s="4">
+        <v>30</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>32</v>
       </c>
@@ -6759,8 +6845,15 @@
       <c r="D16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H16" s="4">
+        <v>31</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>33</v>
       </c>
@@ -6773,8 +6866,15 @@
       <c r="D17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H17" s="4">
+        <v>32</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>34</v>
       </c>
@@ -6788,8 +6888,15 @@
         <v>0</v>
       </c>
       <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H18" s="4">
+        <v>33</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>36</v>
       </c>
@@ -6803,8 +6910,15 @@
         <v>0</v>
       </c>
       <c r="G19" s="30"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H19" s="4">
+        <v>34</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>41</v>
       </c>
@@ -6817,8 +6931,15 @@
       <c r="D20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H20" s="4">
+        <v>41</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>42</v>
       </c>
@@ -6831,8 +6952,15 @@
       <c r="D21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H21" s="4">
+        <v>42</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>102</v>
       </c>
@@ -6846,8 +6974,15 @@
         <v>1</v>
       </c>
       <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H22" s="4">
+        <v>102</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>103</v>
       </c>
@@ -6861,8 +6996,15 @@
         <v>0</v>
       </c>
       <c r="G23" s="30"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H23" s="4">
+        <v>103</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>104</v>
       </c>
@@ -6876,8 +7018,15 @@
         <v>1</v>
       </c>
       <c r="G24" s="30"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H24" s="4">
+        <v>104</v>
+      </c>
+      <c r="I24" s="4">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>105</v>
       </c>
@@ -6891,8 +7040,15 @@
         <v>0</v>
       </c>
       <c r="G25" s="30"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H25" s="4">
+        <v>105</v>
+      </c>
+      <c r="I25" s="4">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>106</v>
       </c>
@@ -6906,8 +7062,15 @@
         <v>1</v>
       </c>
       <c r="G26" s="30"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H26" s="4">
+        <v>106</v>
+      </c>
+      <c r="I26" s="4">
+        <f t="shared" si="0"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>107</v>
       </c>
@@ -6921,8 +7084,15 @@
         <v>0</v>
       </c>
       <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H27" s="4">
+        <v>107</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>108</v>
       </c>
@@ -6936,8 +7106,15 @@
         <v>1</v>
       </c>
       <c r="G28" s="30"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H28" s="4">
+        <v>110</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>109</v>
       </c>
@@ -6951,8 +7128,15 @@
         <v>0</v>
       </c>
       <c r="G29" s="30"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H29" s="4">
+        <v>111</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>110</v>
       </c>
@@ -6966,8 +7150,15 @@
         <v>0</v>
       </c>
       <c r="G30" s="30"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H30" s="4">
+        <v>112</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>111</v>
       </c>
@@ -6981,8 +7172,15 @@
         <v>0</v>
       </c>
       <c r="G31" s="30"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H31" s="4">
+        <v>113</v>
+      </c>
+      <c r="I31" s="4">
+        <f t="shared" si="0"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>112</v>
       </c>
@@ -6996,8 +7194,15 @@
         <v>0</v>
       </c>
       <c r="G32" s="30"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H32" s="4">
+        <v>115</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>113</v>
       </c>
@@ -7011,8 +7216,15 @@
         <v>0</v>
       </c>
       <c r="G33" s="30"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H33" s="4">
+        <v>120</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>115</v>
       </c>
@@ -7026,8 +7238,15 @@
         <v>0</v>
       </c>
       <c r="G34" s="30"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H34" s="4">
+        <v>122</v>
+      </c>
+      <c r="I34" s="4">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>116</v>
       </c>
@@ -7042,7 +7261,7 @@
       </c>
       <c r="G35" s="30"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>117</v>
       </c>
@@ -7057,7 +7276,7 @@
       </c>
       <c r="G36" s="30"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>120</v>
       </c>
@@ -7071,7 +7290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>122</v>
       </c>
@@ -7083,6 +7302,23 @@
       </c>
       <c r="D38" s="4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" s="4">
+        <v>24</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="8">
+        <v>10987</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add a 2045 ORTP scenario column
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EE60B9-FDC1-423A-8470-A8A781A0D42B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3709997B-A680-4005-918E-C2AC183AA955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CMP_Rep_Link!$A$1:$C$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Modeled Projects'!$C$60:$O$80</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$R$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Proj Attributes and Scenarios'!$A$9:$S$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="278">
   <si>
     <t>Cost</t>
   </si>
@@ -864,6 +864,9 @@
   </si>
   <si>
     <t>This is a new interchange, and can't accurately be captured by the regional model</t>
+  </si>
+  <si>
+    <t>ORTP2045</t>
   </si>
 </sst>
 </file>
@@ -2139,6 +2142,7 @@
     <col min="16" max="16" width="13.6640625" style="18" customWidth="1"/>
     <col min="17" max="17" width="18" style="5" customWidth="1"/>
     <col min="18" max="18" width="18" customWidth="1"/>
+    <col min="19" max="19" width="11.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
@@ -2258,7 +2262,9 @@
       <c r="R9" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="S9" s="3"/>
+      <c r="S9" s="3" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
@@ -2313,7 +2319,9 @@
       <c r="R10">
         <v>1</v>
       </c>
-      <c r="S10" s="30"/>
+      <c r="S10" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
@@ -2360,7 +2368,9 @@
       <c r="R11">
         <v>0</v>
       </c>
-      <c r="S11" s="30"/>
+      <c r="S11" s="30">
+        <v>1</v>
+      </c>
       <c r="AC11" s="24"/>
     </row>
     <row r="12" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
@@ -2410,6 +2420,9 @@
       <c r="R12" s="8">
         <v>0</v>
       </c>
+      <c r="S12" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
@@ -2458,7 +2471,9 @@
       <c r="R13" s="24">
         <v>0</v>
       </c>
-      <c r="S13" s="24"/>
+      <c r="S13" s="30">
+        <v>1</v>
+      </c>
       <c r="T13" s="24"/>
       <c r="U13" s="24"/>
       <c r="V13" s="8"/>
@@ -2508,7 +2523,9 @@
       <c r="R14">
         <v>0</v>
       </c>
-      <c r="S14" s="30"/>
+      <c r="S14" s="30">
+        <v>1</v>
+      </c>
       <c r="T14" s="24"/>
       <c r="U14" s="24" t="s">
         <v>242</v>
@@ -2563,7 +2580,9 @@
       <c r="R15">
         <v>1</v>
       </c>
-      <c r="S15" s="30"/>
+      <c r="S15" s="30">
+        <v>1</v>
+      </c>
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
       <c r="V15" s="24"/>
@@ -2622,7 +2641,9 @@
       <c r="R16">
         <v>1</v>
       </c>
-      <c r="S16" s="30"/>
+      <c r="S16" s="30">
+        <v>1</v>
+      </c>
       <c r="T16" s="24"/>
       <c r="U16" s="24"/>
       <c r="V16" s="24"/>
@@ -2675,7 +2696,9 @@
       <c r="R17">
         <v>1</v>
       </c>
-      <c r="S17" s="30"/>
+      <c r="S17" s="30">
+        <v>1</v>
+      </c>
       <c r="T17" s="24"/>
       <c r="U17" s="24"/>
       <c r="V17" s="24"/>
@@ -2728,7 +2751,9 @@
       <c r="R18">
         <v>1</v>
       </c>
-      <c r="S18" s="30"/>
+      <c r="S18" s="30">
+        <v>1</v>
+      </c>
       <c r="T18" s="24"/>
       <c r="U18" s="24"/>
       <c r="V18" s="24"/>
@@ -2781,7 +2806,9 @@
       <c r="R19">
         <v>1</v>
       </c>
-      <c r="S19" s="30"/>
+      <c r="S19" s="30">
+        <v>1</v>
+      </c>
       <c r="T19" s="24"/>
       <c r="U19" s="24"/>
       <c r="V19" s="24"/>
@@ -2838,7 +2865,9 @@
       <c r="R20">
         <v>1</v>
       </c>
-      <c r="S20" s="30"/>
+      <c r="S20" s="30">
+        <v>1</v>
+      </c>
       <c r="AC20" s="24"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.45">
@@ -2893,7 +2922,9 @@
       <c r="R21">
         <v>1</v>
       </c>
-      <c r="S21" s="30"/>
+      <c r="S21" s="30">
+        <v>1</v>
+      </c>
       <c r="AC21" s="24"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.45">
@@ -2941,7 +2972,9 @@
       <c r="R22">
         <v>0</v>
       </c>
-      <c r="S22" s="30"/>
+      <c r="S22" s="30">
+        <v>1</v>
+      </c>
       <c r="AC22" s="24"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.45">
@@ -2987,7 +3020,9 @@
       <c r="R23">
         <v>1</v>
       </c>
-      <c r="S23" s="30"/>
+      <c r="S23" s="30">
+        <v>1</v>
+      </c>
       <c r="AC23" s="24"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.45">
@@ -3036,7 +3071,9 @@
       <c r="R24">
         <v>1</v>
       </c>
-      <c r="S24" s="30"/>
+      <c r="S24" s="30">
+        <v>1</v>
+      </c>
       <c r="AC24" s="24"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
@@ -3084,7 +3121,9 @@
       <c r="R25">
         <v>0</v>
       </c>
-      <c r="S25" s="30"/>
+      <c r="S25" s="30">
+        <v>1</v>
+      </c>
       <c r="AC25" s="24"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
@@ -3136,7 +3175,9 @@
       <c r="R26">
         <v>1</v>
       </c>
-      <c r="S26" s="30"/>
+      <c r="S26" s="30">
+        <v>1</v>
+      </c>
       <c r="AC26" s="24"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
@@ -3177,7 +3218,9 @@
       <c r="R27">
         <v>0</v>
       </c>
-      <c r="S27" s="30"/>
+      <c r="S27" s="30">
+        <v>1</v>
+      </c>
       <c r="AC27" s="24"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
@@ -3225,7 +3268,9 @@
       <c r="R28">
         <v>0</v>
       </c>
-      <c r="S28" s="30"/>
+      <c r="S28" s="30">
+        <v>1</v>
+      </c>
       <c r="AC28" s="24"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
@@ -3277,7 +3322,9 @@
       <c r="R29">
         <v>1</v>
       </c>
-      <c r="S29" s="30"/>
+      <c r="S29" s="30">
+        <v>1</v>
+      </c>
       <c r="AC29" s="24"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
@@ -3326,7 +3373,9 @@
       <c r="R30">
         <v>1</v>
       </c>
-      <c r="S30" s="30"/>
+      <c r="S30" s="30">
+        <v>1</v>
+      </c>
       <c r="AC30" s="24"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
@@ -3374,7 +3423,9 @@
       <c r="R31">
         <v>0</v>
       </c>
-      <c r="S31" s="30"/>
+      <c r="S31" s="30">
+        <v>1</v>
+      </c>
       <c r="AC31" s="24"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
@@ -3426,7 +3477,9 @@
       <c r="R32">
         <v>0</v>
       </c>
-      <c r="S32" s="30"/>
+      <c r="S32" s="30">
+        <v>1</v>
+      </c>
       <c r="AC32" s="24"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.45">
@@ -3473,7 +3526,9 @@
       <c r="R33">
         <v>0</v>
       </c>
-      <c r="S33" s="30"/>
+      <c r="S33" s="30">
+        <v>1</v>
+      </c>
       <c r="AC33" s="24"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.45">
@@ -3528,7 +3583,9 @@
       <c r="R34">
         <v>0</v>
       </c>
-      <c r="S34" s="30"/>
+      <c r="S34" s="30">
+        <v>1</v>
+      </c>
       <c r="AC34" s="24"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.45">
@@ -3577,7 +3634,9 @@
       <c r="R35">
         <v>0</v>
       </c>
-      <c r="S35" s="30"/>
+      <c r="S35" s="30">
+        <v>1</v>
+      </c>
       <c r="AC35" s="24"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.45">
@@ -3621,7 +3680,9 @@
       <c r="R36">
         <v>0</v>
       </c>
-      <c r="S36" s="30"/>
+      <c r="S36" s="30">
+        <v>1</v>
+      </c>
       <c r="AC36" s="24"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.45">
@@ -3658,7 +3719,9 @@
       <c r="R37">
         <v>1</v>
       </c>
-      <c r="S37" s="30"/>
+      <c r="S37" s="30">
+        <v>1</v>
+      </c>
       <c r="AC37" s="24"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.45">
@@ -3710,7 +3773,9 @@
       <c r="R38">
         <v>1</v>
       </c>
-      <c r="S38" s="30"/>
+      <c r="S38" s="30">
+        <v>1</v>
+      </c>
       <c r="AC38" s="24"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.45">
@@ -3762,7 +3827,9 @@
       <c r="R39">
         <v>1</v>
       </c>
-      <c r="S39" s="30"/>
+      <c r="S39" s="30">
+        <v>1</v>
+      </c>
       <c r="AC39" s="24"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.45">
@@ -3803,7 +3870,9 @@
       <c r="R40" s="8">
         <v>0</v>
       </c>
-      <c r="S40" s="8"/>
+      <c r="S40" s="30">
+        <v>1</v>
+      </c>
       <c r="AC40" s="24"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.45">
@@ -3838,7 +3907,9 @@
       <c r="R41" s="8">
         <v>0</v>
       </c>
-      <c r="S41" s="8"/>
+      <c r="S41" s="30">
+        <v>1</v>
+      </c>
       <c r="AC41" s="24"/>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.45">
@@ -3875,7 +3946,9 @@
       <c r="R42" s="8">
         <v>1</v>
       </c>
-      <c r="S42" s="8"/>
+      <c r="S42" s="30">
+        <v>1</v>
+      </c>
       <c r="AC42" s="24"/>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.45">
@@ -3921,7 +3994,9 @@
       <c r="R43" s="8">
         <v>1</v>
       </c>
-      <c r="S43" s="8"/>
+      <c r="S43" s="30">
+        <v>1</v>
+      </c>
       <c r="AC43" s="24"/>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.45">
@@ -3964,7 +4039,9 @@
       <c r="R44" s="8">
         <v>1</v>
       </c>
-      <c r="S44" s="8"/>
+      <c r="S44" s="30">
+        <v>1</v>
+      </c>
       <c r="AC44" s="24"/>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.45">
@@ -4007,7 +4084,9 @@
       <c r="R45" s="8">
         <v>1</v>
       </c>
-      <c r="S45" s="8"/>
+      <c r="S45" s="30">
+        <v>1</v>
+      </c>
       <c r="AC45" s="24"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.45">
@@ -4050,7 +4129,9 @@
       <c r="R46" s="8">
         <v>1</v>
       </c>
-      <c r="S46" s="8"/>
+      <c r="S46" s="30">
+        <v>1</v>
+      </c>
       <c r="AC46" s="24"/>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.45">
@@ -4093,7 +4174,9 @@
       <c r="R47" s="8">
         <v>1</v>
       </c>
-      <c r="S47" s="8"/>
+      <c r="S47" s="30">
+        <v>1</v>
+      </c>
       <c r="AC47" s="24"/>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.45">
@@ -4128,7 +4211,9 @@
       <c r="R48" s="8">
         <v>0</v>
       </c>
-      <c r="S48" s="8"/>
+      <c r="S48" s="30">
+        <v>1</v>
+      </c>
       <c r="AC48" s="24"/>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.45">
@@ -4163,7 +4248,9 @@
       <c r="R49" s="8">
         <v>0</v>
       </c>
-      <c r="S49" s="8"/>
+      <c r="S49" s="30">
+        <v>1</v>
+      </c>
       <c r="AC49" s="24"/>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.45">
@@ -4204,7 +4291,9 @@
       <c r="R50" s="8">
         <v>0</v>
       </c>
-      <c r="S50" s="8"/>
+      <c r="S50" s="30">
+        <v>1</v>
+      </c>
       <c r="AC50" s="24"/>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.45">
@@ -4253,7 +4342,9 @@
       <c r="R51" s="8">
         <v>0</v>
       </c>
-      <c r="S51" s="8"/>
+      <c r="S51" s="30">
+        <v>1</v>
+      </c>
       <c r="AC51" s="24"/>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.45">
@@ -4297,7 +4388,9 @@
       <c r="R52" s="8">
         <v>0</v>
       </c>
-      <c r="S52" s="8"/>
+      <c r="S52" s="30">
+        <v>1</v>
+      </c>
       <c r="AC52" s="24"/>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.45">
@@ -4338,7 +4431,9 @@
       <c r="R53" s="8">
         <v>0</v>
       </c>
-      <c r="S53" s="8"/>
+      <c r="S53" s="30">
+        <v>1</v>
+      </c>
       <c r="AC53" s="24"/>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.45">
@@ -4378,7 +4473,9 @@
       <c r="R54" s="8">
         <v>0</v>
       </c>
-      <c r="S54" s="8"/>
+      <c r="S54" s="30">
+        <v>1</v>
+      </c>
       <c r="AC54" s="24"/>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.45">
@@ -4418,7 +4515,9 @@
       <c r="R55" s="8">
         <v>0</v>
       </c>
-      <c r="S55" s="8"/>
+      <c r="S55" s="30">
+        <v>1</v>
+      </c>
       <c r="AC55" s="24"/>
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.45">
@@ -4459,7 +4558,9 @@
       <c r="R56" s="8">
         <v>0</v>
       </c>
-      <c r="S56" s="8"/>
+      <c r="S56" s="30">
+        <v>1</v>
+      </c>
       <c r="AC56" s="24"/>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.45">
@@ -4510,7 +4611,9 @@
       <c r="R57" s="8">
         <v>0</v>
       </c>
-      <c r="S57" s="8"/>
+      <c r="S57" s="30">
+        <v>1</v>
+      </c>
       <c r="AC57" s="24"/>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.45">
@@ -4555,7 +4658,9 @@
       <c r="R58" s="8">
         <v>0</v>
       </c>
-      <c r="S58" s="8"/>
+      <c r="S58" s="30">
+        <v>1</v>
+      </c>
       <c r="AC58" s="24"/>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.45">
@@ -4595,7 +4700,9 @@
       <c r="R59" s="8">
         <v>1</v>
       </c>
-      <c r="S59" s="8"/>
+      <c r="S59" s="30">
+        <v>1</v>
+      </c>
       <c r="AC59" s="24"/>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.45">
@@ -4635,7 +4742,9 @@
       <c r="R60" s="8">
         <v>1</v>
       </c>
-      <c r="S60" s="8"/>
+      <c r="S60" s="30">
+        <v>1</v>
+      </c>
       <c r="AC60" s="24"/>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.45">
@@ -4674,7 +4783,9 @@
       <c r="R61" s="8">
         <v>1</v>
       </c>
-      <c r="S61" s="8"/>
+      <c r="S61" s="30">
+        <v>1</v>
+      </c>
       <c r="AC61" s="24"/>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.45">
@@ -4721,7 +4832,9 @@
       <c r="R62" s="8">
         <v>1</v>
       </c>
-      <c r="S62" s="8"/>
+      <c r="S62" s="30">
+        <v>1</v>
+      </c>
       <c r="AC62" s="24"/>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.45">
@@ -4766,7 +4879,9 @@
       <c r="R63" s="8">
         <v>0</v>
       </c>
-      <c r="S63" s="8"/>
+      <c r="S63" s="30">
+        <v>1</v>
+      </c>
       <c r="AC63" s="24"/>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.45">
@@ -4807,8 +4922,11 @@
       <c r="R64" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="S64" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A65" s="4">
         <v>122</v>
       </c>
@@ -4844,8 +4962,11 @@
       <c r="R65" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="S65" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A66" s="4">
         <v>123</v>
       </c>
@@ -4889,8 +5010,11 @@
       <c r="R66" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="S66" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -4899,7 +5023,7 @@
       <c r="Q67" s="8"/>
       <c r="R67" s="8"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -4908,7 +5032,7 @@
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
@@ -4917,7 +5041,7 @@
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -4926,7 +5050,7 @@
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -4935,7 +5059,7 @@
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -4944,7 +5068,7 @@
       <c r="Q72" s="8"/>
       <c r="R72" s="8"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -4953,7 +5077,7 @@
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -4963,7 +5087,7 @@
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -4973,7 +5097,7 @@
       <c r="Q75" s="8"/>
       <c r="R75" s="8"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -4985,7 +5109,7 @@
       <c r="Q76" s="8"/>
       <c r="R76" s="8"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -4996,7 +5120,7 @@
       <c r="Q77" s="8"/>
       <c r="R77" s="8"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -5007,13 +5131,13 @@
       <c r="Q78" s="8"/>
       <c r="R78" s="8"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="H79" s="4"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.45">
       <c r="J80" s="5"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.45">
@@ -5029,7 +5153,7 @@
       <c r="D85" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:R66" xr:uid="{7020DE52-0B61-9644-93F1-364D58F6F3FB}"/>
+  <autoFilter ref="A9:S66" xr:uid="{D60FA062-1816-4788-B662-1133BEED731D}"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I77:I79" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>

</xml_diff>

<commit_message>
Add TIP number for OS17
</commit_message>
<xml_diff>
--- a/Project Management Tool.xlsx
+++ b/Project Management Tool.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3709997B-A680-4005-918E-C2AC183AA955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660B8A9A-F389-4FDB-9627-EE4FDD5BAA90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="278">
   <si>
     <t>Cost</t>
   </si>
@@ -776,9 +776,6 @@
     <t>delete, off of HDOT's list</t>
   </si>
   <si>
-    <t>EC 2025</t>
-  </si>
-  <si>
     <t>Widening &amp; New Location</t>
   </si>
   <si>
@@ -867,6 +864,9 @@
   </si>
   <si>
     <t>ORTP2045</t>
+  </si>
+  <si>
+    <t>EC 2020</t>
   </si>
 </sst>
 </file>
@@ -1744,16 +1744,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>148166</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>126206</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>92603</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>301125</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>424156</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>37794</xdr:rowOff>
+      <xdr:rowOff>164794</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1782,8 +1782,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29633333" y="2815166"/>
-          <a:ext cx="4407458" cy="842128"/>
+          <a:off x="26966863" y="2831041"/>
+          <a:ext cx="4060325" cy="802441"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2119,10 +2119,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC85"/>
+  <dimension ref="A1:AA85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
@@ -2145,43 +2145,43 @@
     <col min="19" max="19" width="11.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="P1" s="16"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="P2" s="16"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="P3" s="16"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="P4" s="16"/>
       <c r="Q4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="P5" s="16"/>
       <c r="Q5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="P6" s="16"/>
       <c r="Q6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="P7" s="16"/>
       <c r="Q7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2204,10 +2204,8 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>173</v>
       </c>
@@ -2257,16 +2255,16 @@
         <v>64</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -2308,11 +2306,11 @@
         <v>5</v>
       </c>
       <c r="O10" t="s">
+        <v>269</v>
+      </c>
+      <c r="P10" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="P10" s="18" t="s">
-        <v>271</v>
-      </c>
       <c r="Q10" s="5">
         <v>0</v>
       </c>
@@ -2323,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -2371,22 +2369,22 @@
       <c r="S11" s="30">
         <v>1</v>
       </c>
-      <c r="AC11" s="24"/>
-    </row>
-    <row r="12" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="AA11" s="24"/>
+    </row>
+    <row r="12" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>124</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>265</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>266</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>8</v>
@@ -2424,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" s="30" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2474,11 +2472,9 @@
       <c r="S13" s="30">
         <v>1</v>
       </c>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="8"/>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="T13" s="8"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>5</v>
       </c>
@@ -2496,7 +2492,7 @@
         <v>159</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14">
@@ -2527,17 +2523,13 @@
         <v>1</v>
       </c>
       <c r="T14" s="24"/>
-      <c r="U14" s="24" t="s">
-        <v>242</v>
-      </c>
+      <c r="U14" s="24"/>
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AC14" s="24"/>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA14" s="24"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2557,7 +2549,7 @@
         <v>28</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J15" s="26">
         <v>1.05</v>
@@ -2585,14 +2577,14 @@
       </c>
       <c r="T15" s="24"/>
       <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
+      <c r="V15" s="24" t="s">
+        <v>242</v>
+      </c>
       <c r="W15" s="24"/>
       <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AC15" s="24"/>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA15" s="24"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -2606,7 +2598,7 @@
         <v>55</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>59</v>
@@ -2615,7 +2607,7 @@
         <v>154</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I16">
         <v>251000000</v>
@@ -2649,11 +2641,9 @@
       <c r="V16" s="24"/>
       <c r="W16" s="24"/>
       <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AC16" s="24"/>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA16" s="24"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>10</v>
       </c>
@@ -2673,7 +2663,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J17" s="26">
         <v>4.18</v>
@@ -2704,11 +2694,9 @@
       <c r="V17" s="24"/>
       <c r="W17" s="24"/>
       <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AC17" s="24"/>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA17" s="24"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>11</v>
       </c>
@@ -2722,13 +2710,13 @@
         <v>114</v>
       </c>
       <c r="F18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J18" s="26">
         <v>1.08</v>
@@ -2759,11 +2747,9 @@
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
       <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AC18" s="24"/>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA18" s="24"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>12</v>
       </c>
@@ -2814,11 +2800,9 @@
       <c r="V19" s="24"/>
       <c r="W19" s="24"/>
       <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AC19" s="24"/>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA19" s="24"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>16</v>
       </c>
@@ -2833,13 +2817,13 @@
         <v>155</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I20">
         <v>112000000</v>
@@ -2868,9 +2852,9 @@
       <c r="S20" s="30">
         <v>1</v>
       </c>
-      <c r="AC20" s="24"/>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA20" s="24"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>17</v>
       </c>
@@ -2893,7 +2877,7 @@
         <v>8</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I21">
         <v>35300000</v>
@@ -2925,9 +2909,9 @@
       <c r="S21" s="30">
         <v>1</v>
       </c>
-      <c r="AC21" s="24"/>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA21" s="24"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -2975,9 +2959,9 @@
       <c r="S22" s="30">
         <v>1</v>
       </c>
-      <c r="AC22" s="24"/>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA22" s="24"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2997,7 +2981,7 @@
         <v>32</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J23" s="26">
         <v>0.43</v>
@@ -3023,9 +3007,9 @@
       <c r="S23" s="30">
         <v>1</v>
       </c>
-      <c r="AC23" s="24"/>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA23" s="24"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -3074,9 +3058,9 @@
       <c r="S24" s="30">
         <v>1</v>
       </c>
-      <c r="AC24" s="24"/>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA24" s="24"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>22</v>
       </c>
@@ -3124,9 +3108,9 @@
       <c r="S25" s="30">
         <v>1</v>
       </c>
-      <c r="AC25" s="24"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA25" s="24"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>23</v>
       </c>
@@ -3178,11 +3162,14 @@
       <c r="S26" s="30">
         <v>1</v>
       </c>
-      <c r="AC26" s="24"/>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA26" s="24"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
       </c>
       <c r="C27">
         <v>204</v>
@@ -3221,9 +3208,9 @@
       <c r="S27" s="30">
         <v>1</v>
       </c>
-      <c r="AC27" s="24"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA27" s="24"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -3271,9 +3258,9 @@
       <c r="S28" s="30">
         <v>1</v>
       </c>
-      <c r="AC28" s="24"/>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA28" s="24"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>26</v>
       </c>
@@ -3296,7 +3283,7 @@
         <v>146</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I29">
         <v>13300000</v>
@@ -3325,9 +3312,9 @@
       <c r="S29" s="30">
         <v>1</v>
       </c>
-      <c r="AC29" s="24"/>
-    </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA29" s="24"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -3347,7 +3334,7 @@
         <v>133</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I30">
         <v>500000</v>
@@ -3376,9 +3363,9 @@
       <c r="S30" s="30">
         <v>1</v>
       </c>
-      <c r="AC30" s="24"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA30" s="24"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -3426,9 +3413,9 @@
       <c r="S31" s="30">
         <v>1</v>
       </c>
-      <c r="AC31" s="24"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA31" s="24"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -3480,9 +3467,9 @@
       <c r="S32" s="30">
         <v>1</v>
       </c>
-      <c r="AC32" s="24"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA32" s="24"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -3529,9 +3516,9 @@
       <c r="S33" s="30">
         <v>1</v>
       </c>
-      <c r="AC33" s="24"/>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA33" s="24"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -3586,9 +3573,9 @@
       <c r="S34" s="30">
         <v>1</v>
       </c>
-      <c r="AC34" s="24"/>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA34" s="24"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -3608,7 +3595,7 @@
         <v>126</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I35">
         <v>18200000</v>
@@ -3637,9 +3624,9 @@
       <c r="S35" s="30">
         <v>1</v>
       </c>
-      <c r="AC35" s="24"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA35" s="24"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3683,9 +3670,9 @@
       <c r="S36" s="30">
         <v>1</v>
       </c>
-      <c r="AC36" s="24"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA36" s="24"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3696,7 +3683,7 @@
         <v>179</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J37" s="26">
         <v>0.51</v>
@@ -3722,9 +3709,9 @@
       <c r="S37" s="30">
         <v>1</v>
       </c>
-      <c r="AC37" s="24"/>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA37" s="24"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3747,7 +3734,7 @@
         <v>8</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I38">
         <v>92000000</v>
@@ -3776,9 +3763,9 @@
       <c r="S38" s="30">
         <v>1</v>
       </c>
-      <c r="AC38" s="24"/>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA38" s="24"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>39</v>
       </c>
@@ -3830,9 +3817,9 @@
       <c r="S39" s="30">
         <v>1</v>
       </c>
-      <c r="AC39" s="24"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA39" s="24"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>41</v>
       </c>
@@ -3873,9 +3860,9 @@
       <c r="S40" s="30">
         <v>1</v>
       </c>
-      <c r="AC40" s="24"/>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA40" s="24"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>42</v>
       </c>
@@ -3910,9 +3897,9 @@
       <c r="S41" s="30">
         <v>1</v>
       </c>
-      <c r="AC41" s="24"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA41" s="24"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>43</v>
       </c>
@@ -3923,7 +3910,7 @@
         <v>146</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J42" s="26">
         <v>5.36</v>
@@ -3949,9 +3936,9 @@
       <c r="S42" s="30">
         <v>1</v>
       </c>
-      <c r="AC42" s="24"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA42" s="24"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>44</v>
       </c>
@@ -3968,7 +3955,7 @@
         <v>186</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J43" s="26">
         <v>2.95</v>
@@ -3997,9 +3984,9 @@
       <c r="S43" s="30">
         <v>1</v>
       </c>
-      <c r="AC43" s="24"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA43" s="24"/>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>45</v>
       </c>
@@ -4016,7 +4003,7 @@
         <v>190</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J44" s="26">
         <v>5.03</v>
@@ -4042,9 +4029,9 @@
       <c r="S44" s="30">
         <v>1</v>
       </c>
-      <c r="AC44" s="24"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA44" s="24"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>46</v>
       </c>
@@ -4061,7 +4048,7 @@
         <v>190</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J45" s="26">
         <v>7.61</v>
@@ -4087,9 +4074,9 @@
       <c r="S45" s="30">
         <v>1</v>
       </c>
-      <c r="AC45" s="24"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA45" s="24"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>47</v>
       </c>
@@ -4106,7 +4093,7 @@
         <v>190</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J46" s="26">
         <v>2.93</v>
@@ -4132,9 +4119,9 @@
       <c r="S46" s="30">
         <v>1</v>
       </c>
-      <c r="AC46" s="24"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA46" s="24"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>48</v>
       </c>
@@ -4151,7 +4138,7 @@
         <v>186</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J47" s="26">
         <v>0.78</v>
@@ -4177,9 +4164,9 @@
       <c r="S47" s="30">
         <v>1</v>
       </c>
-      <c r="AC47" s="24"/>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA47" s="24"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A48" s="24">
         <v>102</v>
       </c>
@@ -4214,9 +4201,9 @@
       <c r="S48" s="30">
         <v>1</v>
       </c>
-      <c r="AC48" s="24"/>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA48" s="24"/>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A49" s="24">
         <v>103</v>
       </c>
@@ -4251,9 +4238,9 @@
       <c r="S49" s="30">
         <v>1</v>
       </c>
-      <c r="AC49" s="24"/>
-    </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA49" s="24"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A50" s="24">
         <v>104</v>
       </c>
@@ -4294,9 +4281,9 @@
       <c r="S50" s="30">
         <v>1</v>
       </c>
-      <c r="AC50" s="24"/>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA50" s="24"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A51" s="24">
         <v>105</v>
       </c>
@@ -4316,7 +4303,7 @@
         <v>186</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I51">
         <v>348900000</v>
@@ -4345,17 +4332,17 @@
       <c r="S51" s="30">
         <v>1</v>
       </c>
-      <c r="AC51" s="24"/>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA51" s="24"/>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A52" s="24">
         <v>106</v>
       </c>
       <c r="D52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G52" t="s">
         <v>186</v>
@@ -4391,9 +4378,9 @@
       <c r="S52" s="30">
         <v>1</v>
       </c>
-      <c r="AC52" s="24"/>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA52" s="24"/>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A53" s="24">
         <v>107</v>
       </c>
@@ -4434,9 +4421,9 @@
       <c r="S53" s="30">
         <v>1</v>
       </c>
-      <c r="AC53" s="24"/>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA53" s="24"/>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A54" s="24">
         <v>110</v>
       </c>
@@ -4476,9 +4463,9 @@
       <c r="S54" s="30">
         <v>1</v>
       </c>
-      <c r="AC54" s="24"/>
-    </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA54" s="24"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A55" s="24">
         <v>111</v>
       </c>
@@ -4518,9 +4505,9 @@
       <c r="S55" s="30">
         <v>1</v>
       </c>
-      <c r="AC55" s="24"/>
-    </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA55" s="24"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A56" s="24">
         <v>112</v>
       </c>
@@ -4561,9 +4548,9 @@
       <c r="S56" s="30">
         <v>1</v>
       </c>
-      <c r="AC56" s="24"/>
-    </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA56" s="24"/>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A57" s="24">
         <v>113</v>
       </c>
@@ -4584,7 +4571,7 @@
         <v>186</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I57">
         <v>1269000000</v>
@@ -4614,9 +4601,9 @@
       <c r="S57" s="30">
         <v>1</v>
       </c>
-      <c r="AC57" s="24"/>
-    </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA57" s="24"/>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A58" s="24">
         <v>115</v>
       </c>
@@ -4661,9 +4648,9 @@
       <c r="S58" s="30">
         <v>1</v>
       </c>
-      <c r="AC58" s="24"/>
-    </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA58" s="24"/>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A59" s="24">
         <v>116</v>
       </c>
@@ -4676,7 +4663,7 @@
         <v>186</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J59" s="26">
         <v>0.23</v>
@@ -4703,9 +4690,9 @@
       <c r="S59" s="30">
         <v>1</v>
       </c>
-      <c r="AC59" s="24"/>
-    </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA59" s="24"/>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A60" s="24">
         <v>117</v>
       </c>
@@ -4718,7 +4705,7 @@
         <v>186</v>
       </c>
       <c r="H60" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J60" s="26">
         <v>0.42</v>
@@ -4745,9 +4732,9 @@
       <c r="S60" s="30">
         <v>1</v>
       </c>
-      <c r="AC60" s="24"/>
-    </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA60" s="24"/>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A61" s="24">
         <v>118</v>
       </c>
@@ -4786,9 +4773,9 @@
       <c r="S61" s="30">
         <v>1</v>
       </c>
-      <c r="AC61" s="24"/>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA61" s="24"/>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A62" s="4">
         <v>119</v>
       </c>
@@ -4807,7 +4794,7 @@
         <v>186</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I62" s="4"/>
       <c r="J62" s="26">
@@ -4835,9 +4822,9 @@
       <c r="S62" s="30">
         <v>1</v>
       </c>
-      <c r="AC62" s="24"/>
-    </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA62" s="24"/>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A63" s="4">
         <v>120</v>
       </c>
@@ -4882,9 +4869,9 @@
       <c r="S63" s="30">
         <v>1</v>
       </c>
-      <c r="AC63" s="24"/>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.45">
+      <c r="AA63" s="24"/>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A64" s="4">
         <v>121</v>
       </c>
@@ -4894,16 +4881,16 @@
         <v>163</v>
       </c>
       <c r="E64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H64" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="26">
@@ -4936,7 +4923,7 @@
         <v>163</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>29</v>
@@ -4976,7 +4963,7 @@
         <v>161</v>
       </c>
       <c r="E66" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>135</v>
@@ -4985,7 +4972,7 @@
         <v>8</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I66" s="4"/>
       <c r="J66" s="26">
@@ -5153,7 +5140,7 @@
       <c r="D85" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:S66" xr:uid="{D60FA062-1816-4788-B662-1133BEED731D}"/>
+  <autoFilter ref="A9:S66" xr:uid="{CE59956F-0441-4350-8092-3776C95CB252}"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Functional Class" sqref="I77:I79" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
@@ -5816,7 +5803,7 @@
         <v>1</v>
       </c>
       <c r="W28" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.45">
@@ -5854,7 +5841,7 @@
         <v>0</v>
       </c>
       <c r="W29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.45">
@@ -5901,7 +5888,7 @@
       </c>
       <c r="P30" s="18"/>
       <c r="W30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.45">
@@ -5942,7 +5929,7 @@
       <c r="O31" s="30"/>
       <c r="P31" s="18"/>
       <c r="W31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:23" s="30" customFormat="1" x14ac:dyDescent="0.45">
@@ -6059,7 +6046,7 @@
       </c>
       <c r="S34" s="8"/>
       <c r="W34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AC34" s="24"/>
     </row>
@@ -6110,7 +6097,7 @@
       </c>
       <c r="S35" s="30"/>
       <c r="W35" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AC35" s="24"/>
     </row>
@@ -6162,7 +6149,7 @@
       </c>
       <c r="S36" s="30"/>
       <c r="W36" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AC36" s="24"/>
     </row>
@@ -6181,7 +6168,7 @@
         <v>147</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G37" t="s">
         <v>149</v>
@@ -6217,7 +6204,7 @@
       <c r="U37" s="24"/>
       <c r="V37" s="24"/>
       <c r="W37" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X37" s="24"/>
       <c r="Y37" s="24"/>
@@ -6268,7 +6255,7 @@
       </c>
       <c r="S38" s="30"/>
       <c r="W38" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AC38" s="24"/>
     </row>
@@ -6320,7 +6307,7 @@
       </c>
       <c r="S39" s="30"/>
       <c r="W39" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AC39" s="24"/>
     </row>
@@ -6375,7 +6362,7 @@
       <c r="U40" s="24"/>
       <c r="V40" s="24"/>
       <c r="W40" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X40" s="24"/>
       <c r="Y40" s="24"/>
@@ -6384,16 +6371,16 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
+        <v>271</v>
+      </c>
+      <c r="D41" t="s">
         <v>272</v>
-      </c>
-      <c r="D41" t="s">
-        <v>273</v>
       </c>
       <c r="G41" s="4"/>
       <c r="J41"/>
       <c r="K41"/>
       <c r="W41" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.45">
@@ -7177,7 +7164,7 @@
         <v>106</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C26" s="8">
         <v>9153</v>
@@ -7442,7 +7429,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.45">

</xml_diff>